<commit_message>
WT Course Course form working Started candidate form Module heading update
</commit_message>
<xml_diff>
--- a/Phase 1 Candidate Database v2.xlsx
+++ b/Phase 1 Candidate Database v2.xlsx
@@ -148,7 +148,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="310">
   <si>
     <t>DAY</t>
   </si>
@@ -994,6 +994,90 @@
   </si>
   <si>
     <t>58 ,194, 146</t>
+  </si>
+  <si>
+    <t>PPV</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>Health and Safety</t>
+  </si>
+  <si>
+    <t>Trauma</t>
+  </si>
+  <si>
+    <t>Hose - Day 1</t>
+  </si>
+  <si>
+    <t>Hose - Day 2</t>
+  </si>
+  <si>
+    <t>Hose - Day 3</t>
+  </si>
+  <si>
+    <t>HR Input</t>
+  </si>
+  <si>
+    <t>Ladders</t>
+  </si>
+  <si>
+    <t>Pumps - Day 1</t>
+  </si>
+  <si>
+    <t>Pumps - Day 2</t>
+  </si>
+  <si>
+    <t>Pumps - Day 3</t>
+  </si>
+  <si>
+    <t>BA - Day 1</t>
+  </si>
+  <si>
+    <t>BA - Day 2</t>
+  </si>
+  <si>
+    <t>BA - Day 3</t>
+  </si>
+  <si>
+    <t>BA - Day 4</t>
+  </si>
+  <si>
+    <t>Fire Science</t>
+  </si>
+  <si>
+    <t>BA Search and Rescue</t>
+  </si>
+  <si>
+    <t>BA Exercise</t>
+  </si>
+  <si>
+    <t>BA Board Assessment</t>
+  </si>
+  <si>
+    <t>BA Written Exam</t>
+  </si>
+  <si>
+    <t>RTC - Day 1</t>
+  </si>
+  <si>
+    <t>RTC - Day 2</t>
+  </si>
+  <si>
+    <t>RTC - Day 3</t>
+  </si>
+  <si>
+    <t>Consolidation Training</t>
+  </si>
+  <si>
+    <t>Tech Rope Rescue - Day 1</t>
+  </si>
+  <si>
+    <t>Tech Rope Rescue - Day 2</t>
+  </si>
+  <si>
+    <t>Tech Rope Rescue - Day 3</t>
   </si>
 </sst>
 </file>
@@ -3910,6 +3994,114 @@
     <xf numFmtId="0" fontId="34" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="19" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="22" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="22" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="22" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="18" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="24" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="23" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
@@ -3919,6 +4111,18 @@
     <xf numFmtId="0" fontId="32" fillId="23" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="22" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="22" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="22" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="23" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
@@ -3964,125 +4168,32 @@
     <xf numFmtId="0" fontId="32" fillId="23" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="25" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="24" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="63" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="18" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="41" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4093,33 +4204,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="41" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="41" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4156,68 +4240,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="22" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="23" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="22" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="21" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="18" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="23" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="22" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="21" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -7787,7 +7871,7 @@
         <xdr:cNvPr id="21" name="Rectangle 20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000015000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000015000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7847,7 +7931,7 @@
         <xdr:cNvPr id="22" name="Rectangle 21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000016000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7907,7 +7991,7 @@
         <xdr:cNvPr id="23" name="Rectangle 22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000017000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7967,7 +8051,7 @@
         <xdr:cNvPr id="24" name="Rectangle 23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000018000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8027,7 +8111,7 @@
         <xdr:cNvPr id="25" name="Rectangle 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000019000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8087,7 +8171,7 @@
         <xdr:cNvPr id="26" name="Rectangle 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8147,7 +8231,7 @@
         <xdr:cNvPr id="27" name="Rectangle 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8207,7 +8291,7 @@
         <xdr:cNvPr id="28" name="Rectangle 27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8267,7 +8351,7 @@
         <xdr:cNvPr id="29" name="Rectangle 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8327,7 +8411,7 @@
         <xdr:cNvPr id="30" name="Rectangle 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8387,7 +8471,7 @@
         <xdr:cNvPr id="31" name="Rectangle 30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00001F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8447,7 +8531,7 @@
         <xdr:cNvPr id="32" name="Rectangle 31" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000020000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000020000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8507,7 +8591,7 @@
         <xdr:cNvPr id="33" name="Rectangle 32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000021000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000021000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -14778,7 +14862,7 @@
       <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="K10" sqref="K10"/>
+      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15056,7 +15140,7 @@
       <c r="AZ4" s="235"/>
       <c r="BA4" s="235"/>
     </row>
-    <row r="5" spans="1:55" s="238" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" s="238" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="236"/>
       <c r="B5" s="236"/>
       <c r="C5" s="230">
@@ -15205,42 +15289,108 @@
       </c>
       <c r="AY5" s="237"/>
     </row>
-    <row r="6" spans="1:55" s="238" customFormat="1" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" s="238" customFormat="1" ht="128.25" x14ac:dyDescent="0.25">
       <c r="A6" s="236"/>
       <c r="B6" s="236"/>
-      <c r="C6" s="232"/>
-      <c r="D6" s="232"/>
-      <c r="E6" s="232"/>
-      <c r="F6" s="232"/>
-      <c r="G6" s="232"/>
-      <c r="H6" s="233"/>
-      <c r="I6" s="233"/>
-      <c r="J6" s="233"/>
-      <c r="K6" s="233"/>
-      <c r="L6" s="233"/>
-      <c r="M6" s="232"/>
-      <c r="N6" s="232"/>
-      <c r="O6" s="232"/>
-      <c r="P6" s="232"/>
-      <c r="Q6" s="232"/>
-      <c r="R6" s="233"/>
-      <c r="S6" s="233"/>
-      <c r="T6" s="233"/>
-      <c r="U6" s="233"/>
-      <c r="V6" s="233"/>
-      <c r="W6" s="232"/>
-      <c r="X6" s="232"/>
-      <c r="Y6" s="232"/>
-      <c r="Z6" s="232"/>
-      <c r="AA6" s="232"/>
-      <c r="AB6" s="233"/>
-      <c r="AC6" s="233"/>
-      <c r="AD6" s="233"/>
-      <c r="AE6" s="233"/>
-      <c r="AF6" s="233"/>
-      <c r="AG6" s="232"/>
-      <c r="AH6" s="232"/>
-      <c r="AI6" s="232"/>
+      <c r="C6" s="232" t="s">
+        <v>283</v>
+      </c>
+      <c r="D6" s="232" t="s">
+        <v>284</v>
+      </c>
+      <c r="E6" s="232" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="232" t="s">
+        <v>285</v>
+      </c>
+      <c r="G6" s="232" t="s">
+        <v>286</v>
+      </c>
+      <c r="H6" s="233" t="s">
+        <v>287</v>
+      </c>
+      <c r="I6" s="233" t="s">
+        <v>288</v>
+      </c>
+      <c r="J6" s="233" t="s">
+        <v>289</v>
+      </c>
+      <c r="K6" s="233" t="s">
+        <v>290</v>
+      </c>
+      <c r="L6" s="233" t="s">
+        <v>240</v>
+      </c>
+      <c r="M6" s="232" t="s">
+        <v>291</v>
+      </c>
+      <c r="N6" s="232" t="s">
+        <v>292</v>
+      </c>
+      <c r="O6" s="232" t="s">
+        <v>293</v>
+      </c>
+      <c r="P6" s="232" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q6" s="232" t="s">
+        <v>295</v>
+      </c>
+      <c r="R6" s="233" t="s">
+        <v>296</v>
+      </c>
+      <c r="S6" s="233" t="s">
+        <v>297</v>
+      </c>
+      <c r="T6" s="233" t="s">
+        <v>298</v>
+      </c>
+      <c r="U6" s="233" t="s">
+        <v>299</v>
+      </c>
+      <c r="V6" s="233" t="s">
+        <v>50</v>
+      </c>
+      <c r="W6" s="232" t="s">
+        <v>300</v>
+      </c>
+      <c r="X6" s="232" t="s">
+        <v>49</v>
+      </c>
+      <c r="Y6" s="232" t="s">
+        <v>301</v>
+      </c>
+      <c r="Z6" s="232" t="s">
+        <v>302</v>
+      </c>
+      <c r="AA6" s="232" t="s">
+        <v>282</v>
+      </c>
+      <c r="AB6" s="233" t="s">
+        <v>303</v>
+      </c>
+      <c r="AC6" s="233" t="s">
+        <v>304</v>
+      </c>
+      <c r="AD6" s="233" t="s">
+        <v>305</v>
+      </c>
+      <c r="AE6" s="233" t="s">
+        <v>306</v>
+      </c>
+      <c r="AF6" s="233" t="s">
+        <v>240</v>
+      </c>
+      <c r="AG6" s="232" t="s">
+        <v>307</v>
+      </c>
+      <c r="AH6" s="232" t="s">
+        <v>308</v>
+      </c>
+      <c r="AI6" s="232" t="s">
+        <v>309</v>
+      </c>
       <c r="AJ6" s="232" t="s">
         <v>240</v>
       </c>
@@ -16935,7 +17085,7 @@
   </conditionalFormatting>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="55" fitToWidth="4" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="56" fitToWidth="4" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId2"/>
 </worksheet>
@@ -17179,8 +17329,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="15361" r:id="rId4" name="BtnDBConnect">
+        <control shapeId="15364" r:id="rId4" name="CommandButton1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>904875</xdr:colOff>
+                <xdr:row>18</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>19</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="15364" r:id="rId4" name="CommandButton1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="15361" r:id="rId6" name="BtnDBConnect">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>6</xdr:col>
@@ -17199,32 +17374,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="15361" r:id="rId4" name="BtnDBConnect"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="15364" r:id="rId6" name="CommandButton1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>904875</xdr:colOff>
-                <xdr:row>18</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>19</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="15364" r:id="rId6" name="CommandButton1"/>
+        <control shapeId="15361" r:id="rId6" name="BtnDBConnect"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -17730,44 +17880,44 @@
       <c r="U2" s="135"/>
       <c r="V2" s="135"/>
       <c r="W2" s="135"/>
-      <c r="X2" s="314" t="s">
+      <c r="X2" s="262" t="s">
         <v>75</v>
       </c>
-      <c r="Y2" s="314"/>
-      <c r="Z2" s="314"/>
-      <c r="AA2" s="314"/>
-      <c r="AB2" s="314"/>
-      <c r="AC2" s="314"/>
-      <c r="AD2" s="314"/>
-      <c r="AE2" s="314"/>
-      <c r="AF2" s="314"/>
-      <c r="AG2" s="314"/>
-      <c r="AH2" s="314"/>
-      <c r="AI2" s="314"/>
-      <c r="AJ2" s="314"/>
-      <c r="AK2" s="314"/>
-      <c r="AL2" s="314"/>
-      <c r="AM2" s="314"/>
-      <c r="AN2" s="314"/>
-      <c r="AO2" s="314"/>
-      <c r="AP2" s="314"/>
-      <c r="AQ2" s="314"/>
-      <c r="AR2" s="314"/>
-      <c r="AS2" s="313" t="str">
+      <c r="Y2" s="262"/>
+      <c r="Z2" s="262"/>
+      <c r="AA2" s="262"/>
+      <c r="AB2" s="262"/>
+      <c r="AC2" s="262"/>
+      <c r="AD2" s="262"/>
+      <c r="AE2" s="262"/>
+      <c r="AF2" s="262"/>
+      <c r="AG2" s="262"/>
+      <c r="AH2" s="262"/>
+      <c r="AI2" s="262"/>
+      <c r="AJ2" s="262"/>
+      <c r="AK2" s="262"/>
+      <c r="AL2" s="262"/>
+      <c r="AM2" s="262"/>
+      <c r="AN2" s="262"/>
+      <c r="AO2" s="262"/>
+      <c r="AP2" s="262"/>
+      <c r="AQ2" s="262"/>
+      <c r="AR2" s="262"/>
+      <c r="AS2" s="261" t="str">
         <f>CONCATENATE("Course No - ", CourseNo)</f>
         <v xml:space="preserve">Course No - </v>
       </c>
-      <c r="AT2" s="313"/>
-      <c r="AU2" s="313"/>
-      <c r="AV2" s="313"/>
-      <c r="AW2" s="313"/>
-      <c r="AX2" s="313"/>
-      <c r="AY2" s="313"/>
-      <c r="AZ2" s="313"/>
-      <c r="BA2" s="313"/>
-      <c r="BB2" s="313"/>
-      <c r="BC2" s="313"/>
-      <c r="BD2" s="313"/>
+      <c r="AT2" s="261"/>
+      <c r="AU2" s="261"/>
+      <c r="AV2" s="261"/>
+      <c r="AW2" s="261"/>
+      <c r="AX2" s="261"/>
+      <c r="AY2" s="261"/>
+      <c r="AZ2" s="261"/>
+      <c r="BA2" s="261"/>
+      <c r="BB2" s="261"/>
+      <c r="BC2" s="261"/>
+      <c r="BD2" s="261"/>
       <c r="BE2" s="136"/>
       <c r="BF2" s="136"/>
       <c r="BG2" s="136"/>
@@ -17802,454 +17952,454 @@
       <c r="CJ2" s="136"/>
     </row>
     <row r="3" spans="2:98" s="124" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="315" t="s">
+      <c r="B3" s="263" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="316"/>
-      <c r="D3" s="317">
+      <c r="C3" s="264"/>
+      <c r="D3" s="265">
         <v>3</v>
       </c>
-      <c r="E3" s="317"/>
-      <c r="F3" s="317"/>
-      <c r="G3" s="317"/>
-      <c r="H3" s="318"/>
-      <c r="I3" s="295">
+      <c r="E3" s="265"/>
+      <c r="F3" s="265"/>
+      <c r="G3" s="265"/>
+      <c r="H3" s="266"/>
+      <c r="I3" s="267">
         <v>9</v>
       </c>
-      <c r="J3" s="317"/>
-      <c r="K3" s="317"/>
-      <c r="L3" s="317"/>
-      <c r="M3" s="318"/>
-      <c r="N3" s="295">
+      <c r="J3" s="265"/>
+      <c r="K3" s="265"/>
+      <c r="L3" s="265"/>
+      <c r="M3" s="266"/>
+      <c r="N3" s="267">
         <v>11</v>
       </c>
-      <c r="O3" s="317"/>
-      <c r="P3" s="317"/>
-      <c r="Q3" s="317"/>
-      <c r="R3" s="317"/>
-      <c r="S3" s="317"/>
-      <c r="T3" s="317"/>
-      <c r="U3" s="317"/>
-      <c r="V3" s="317"/>
-      <c r="W3" s="318"/>
-      <c r="X3" s="295">
+      <c r="O3" s="265"/>
+      <c r="P3" s="265"/>
+      <c r="Q3" s="265"/>
+      <c r="R3" s="265"/>
+      <c r="S3" s="265"/>
+      <c r="T3" s="265"/>
+      <c r="U3" s="265"/>
+      <c r="V3" s="265"/>
+      <c r="W3" s="266"/>
+      <c r="X3" s="267">
         <v>17</v>
       </c>
-      <c r="Y3" s="317"/>
-      <c r="Z3" s="317"/>
-      <c r="AA3" s="317"/>
-      <c r="AB3" s="317"/>
-      <c r="AC3" s="317"/>
-      <c r="AD3" s="317"/>
-      <c r="AE3" s="317"/>
-      <c r="AF3" s="317"/>
-      <c r="AG3" s="318"/>
-      <c r="AH3" s="295">
+      <c r="Y3" s="265"/>
+      <c r="Z3" s="265"/>
+      <c r="AA3" s="265"/>
+      <c r="AB3" s="265"/>
+      <c r="AC3" s="265"/>
+      <c r="AD3" s="265"/>
+      <c r="AE3" s="265"/>
+      <c r="AF3" s="265"/>
+      <c r="AG3" s="266"/>
+      <c r="AH3" s="267">
         <v>20</v>
       </c>
-      <c r="AI3" s="317"/>
-      <c r="AJ3" s="317"/>
-      <c r="AK3" s="317"/>
-      <c r="AL3" s="317"/>
-      <c r="AM3" s="317"/>
-      <c r="AN3" s="317"/>
-      <c r="AO3" s="317"/>
-      <c r="AP3" s="317"/>
-      <c r="AQ3" s="317"/>
-      <c r="AR3" s="317"/>
-      <c r="AS3" s="317"/>
-      <c r="AT3" s="317"/>
-      <c r="AU3" s="317"/>
-      <c r="AV3" s="317"/>
-      <c r="AW3" s="317"/>
-      <c r="AX3" s="317"/>
-      <c r="AY3" s="317"/>
-      <c r="AZ3" s="317"/>
-      <c r="BA3" s="318"/>
-      <c r="BB3" s="295">
+      <c r="AI3" s="265"/>
+      <c r="AJ3" s="265"/>
+      <c r="AK3" s="265"/>
+      <c r="AL3" s="265"/>
+      <c r="AM3" s="265"/>
+      <c r="AN3" s="265"/>
+      <c r="AO3" s="265"/>
+      <c r="AP3" s="265"/>
+      <c r="AQ3" s="265"/>
+      <c r="AR3" s="265"/>
+      <c r="AS3" s="265"/>
+      <c r="AT3" s="265"/>
+      <c r="AU3" s="265"/>
+      <c r="AV3" s="265"/>
+      <c r="AW3" s="265"/>
+      <c r="AX3" s="265"/>
+      <c r="AY3" s="265"/>
+      <c r="AZ3" s="265"/>
+      <c r="BA3" s="266"/>
+      <c r="BB3" s="267">
         <v>27</v>
       </c>
-      <c r="BC3" s="317"/>
-      <c r="BD3" s="317"/>
-      <c r="BE3" s="317"/>
-      <c r="BF3" s="317"/>
-      <c r="BG3" s="317"/>
-      <c r="BH3" s="317"/>
-      <c r="BI3" s="317"/>
-      <c r="BJ3" s="317"/>
-      <c r="BK3" s="318"/>
-      <c r="BL3" s="294">
+      <c r="BC3" s="265"/>
+      <c r="BD3" s="265"/>
+      <c r="BE3" s="265"/>
+      <c r="BF3" s="265"/>
+      <c r="BG3" s="265"/>
+      <c r="BH3" s="265"/>
+      <c r="BI3" s="265"/>
+      <c r="BJ3" s="265"/>
+      <c r="BK3" s="266"/>
+      <c r="BL3" s="268">
         <v>28</v>
       </c>
-      <c r="BM3" s="294"/>
-      <c r="BN3" s="295"/>
-      <c r="BO3" s="295"/>
-      <c r="BP3" s="295"/>
-      <c r="BQ3" s="295"/>
-      <c r="BR3" s="295"/>
-      <c r="BS3" s="295"/>
-      <c r="BT3" s="295"/>
-      <c r="BU3" s="295"/>
-      <c r="BV3" s="295"/>
-      <c r="BW3" s="295"/>
-      <c r="BX3" s="295"/>
-      <c r="BY3" s="295"/>
-      <c r="BZ3" s="295"/>
-      <c r="CA3" s="295"/>
-      <c r="CB3" s="295"/>
-      <c r="CC3" s="295"/>
-      <c r="CD3" s="295"/>
-      <c r="CE3" s="295"/>
-      <c r="CF3" s="270">
+      <c r="BM3" s="268"/>
+      <c r="BN3" s="267"/>
+      <c r="BO3" s="267"/>
+      <c r="BP3" s="267"/>
+      <c r="BQ3" s="267"/>
+      <c r="BR3" s="267"/>
+      <c r="BS3" s="267"/>
+      <c r="BT3" s="267"/>
+      <c r="BU3" s="267"/>
+      <c r="BV3" s="267"/>
+      <c r="BW3" s="267"/>
+      <c r="BX3" s="267"/>
+      <c r="BY3" s="267"/>
+      <c r="BZ3" s="267"/>
+      <c r="CA3" s="267"/>
+      <c r="CB3" s="267"/>
+      <c r="CC3" s="267"/>
+      <c r="CD3" s="267"/>
+      <c r="CE3" s="267"/>
+      <c r="CF3" s="310">
         <v>29</v>
       </c>
-      <c r="CG3" s="271"/>
-      <c r="CH3" s="271"/>
-      <c r="CI3" s="271"/>
-      <c r="CJ3" s="272"/>
+      <c r="CG3" s="311"/>
+      <c r="CH3" s="311"/>
+      <c r="CI3" s="311"/>
+      <c r="CJ3" s="312"/>
       <c r="CK3" s="148"/>
       <c r="CL3" s="141"/>
     </row>
     <row r="4" spans="2:98" s="122" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="296" t="s">
+      <c r="B4" s="269" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="297"/>
-      <c r="D4" s="298" t="s">
+      <c r="C4" s="270"/>
+      <c r="D4" s="271" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="299"/>
-      <c r="F4" s="299"/>
-      <c r="G4" s="299"/>
-      <c r="H4" s="300"/>
-      <c r="I4" s="301" t="s">
+      <c r="E4" s="272"/>
+      <c r="F4" s="272"/>
+      <c r="G4" s="272"/>
+      <c r="H4" s="273"/>
+      <c r="I4" s="274" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="302"/>
-      <c r="K4" s="302"/>
-      <c r="L4" s="302"/>
-      <c r="M4" s="303"/>
-      <c r="N4" s="304" t="s">
+      <c r="J4" s="275"/>
+      <c r="K4" s="275"/>
+      <c r="L4" s="275"/>
+      <c r="M4" s="276"/>
+      <c r="N4" s="277" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="305"/>
-      <c r="P4" s="305"/>
-      <c r="Q4" s="305"/>
-      <c r="R4" s="305"/>
-      <c r="S4" s="305"/>
-      <c r="T4" s="305"/>
-      <c r="U4" s="305"/>
-      <c r="V4" s="305"/>
-      <c r="W4" s="306"/>
-      <c r="X4" s="307" t="s">
+      <c r="O4" s="278"/>
+      <c r="P4" s="278"/>
+      <c r="Q4" s="278"/>
+      <c r="R4" s="278"/>
+      <c r="S4" s="278"/>
+      <c r="T4" s="278"/>
+      <c r="U4" s="278"/>
+      <c r="V4" s="278"/>
+      <c r="W4" s="279"/>
+      <c r="X4" s="280" t="s">
         <v>14</v>
       </c>
-      <c r="Y4" s="308"/>
-      <c r="Z4" s="308"/>
-      <c r="AA4" s="308"/>
-      <c r="AB4" s="308"/>
-      <c r="AC4" s="308"/>
-      <c r="AD4" s="308"/>
-      <c r="AE4" s="308"/>
-      <c r="AF4" s="308"/>
-      <c r="AG4" s="309"/>
-      <c r="AH4" s="307" t="s">
+      <c r="Y4" s="281"/>
+      <c r="Z4" s="281"/>
+      <c r="AA4" s="281"/>
+      <c r="AB4" s="281"/>
+      <c r="AC4" s="281"/>
+      <c r="AD4" s="281"/>
+      <c r="AE4" s="281"/>
+      <c r="AF4" s="281"/>
+      <c r="AG4" s="282"/>
+      <c r="AH4" s="280" t="s">
         <v>18</v>
       </c>
-      <c r="AI4" s="308"/>
-      <c r="AJ4" s="308"/>
-      <c r="AK4" s="308"/>
-      <c r="AL4" s="308"/>
-      <c r="AM4" s="308"/>
-      <c r="AN4" s="308"/>
-      <c r="AO4" s="308"/>
-      <c r="AP4" s="308"/>
-      <c r="AQ4" s="308"/>
-      <c r="AR4" s="308"/>
-      <c r="AS4" s="308"/>
-      <c r="AT4" s="308"/>
-      <c r="AU4" s="308"/>
-      <c r="AV4" s="308"/>
-      <c r="AW4" s="308"/>
-      <c r="AX4" s="308"/>
-      <c r="AY4" s="308"/>
-      <c r="AZ4" s="308"/>
-      <c r="BA4" s="309"/>
-      <c r="BB4" s="310" t="s">
+      <c r="AI4" s="281"/>
+      <c r="AJ4" s="281"/>
+      <c r="AK4" s="281"/>
+      <c r="AL4" s="281"/>
+      <c r="AM4" s="281"/>
+      <c r="AN4" s="281"/>
+      <c r="AO4" s="281"/>
+      <c r="AP4" s="281"/>
+      <c r="AQ4" s="281"/>
+      <c r="AR4" s="281"/>
+      <c r="AS4" s="281"/>
+      <c r="AT4" s="281"/>
+      <c r="AU4" s="281"/>
+      <c r="AV4" s="281"/>
+      <c r="AW4" s="281"/>
+      <c r="AX4" s="281"/>
+      <c r="AY4" s="281"/>
+      <c r="AZ4" s="281"/>
+      <c r="BA4" s="282"/>
+      <c r="BB4" s="283" t="s">
         <v>27</v>
       </c>
-      <c r="BC4" s="311"/>
-      <c r="BD4" s="311"/>
-      <c r="BE4" s="311"/>
-      <c r="BF4" s="311"/>
-      <c r="BG4" s="311"/>
-      <c r="BH4" s="311"/>
-      <c r="BI4" s="311"/>
-      <c r="BJ4" s="311"/>
-      <c r="BK4" s="312"/>
-      <c r="BL4" s="310" t="s">
+      <c r="BC4" s="284"/>
+      <c r="BD4" s="284"/>
+      <c r="BE4" s="284"/>
+      <c r="BF4" s="284"/>
+      <c r="BG4" s="284"/>
+      <c r="BH4" s="284"/>
+      <c r="BI4" s="284"/>
+      <c r="BJ4" s="284"/>
+      <c r="BK4" s="285"/>
+      <c r="BL4" s="283" t="s">
         <v>23</v>
       </c>
-      <c r="BM4" s="311"/>
-      <c r="BN4" s="311"/>
-      <c r="BO4" s="311"/>
-      <c r="BP4" s="311"/>
-      <c r="BQ4" s="311"/>
-      <c r="BR4" s="311"/>
-      <c r="BS4" s="311"/>
-      <c r="BT4" s="311"/>
-      <c r="BU4" s="311"/>
-      <c r="BV4" s="311"/>
-      <c r="BW4" s="311"/>
-      <c r="BX4" s="311"/>
-      <c r="BY4" s="311"/>
-      <c r="BZ4" s="311"/>
-      <c r="CA4" s="311"/>
-      <c r="CB4" s="311"/>
-      <c r="CC4" s="311"/>
-      <c r="CD4" s="311"/>
-      <c r="CE4" s="312"/>
-      <c r="CF4" s="261" t="s">
+      <c r="BM4" s="284"/>
+      <c r="BN4" s="284"/>
+      <c r="BO4" s="284"/>
+      <c r="BP4" s="284"/>
+      <c r="BQ4" s="284"/>
+      <c r="BR4" s="284"/>
+      <c r="BS4" s="284"/>
+      <c r="BT4" s="284"/>
+      <c r="BU4" s="284"/>
+      <c r="BV4" s="284"/>
+      <c r="BW4" s="284"/>
+      <c r="BX4" s="284"/>
+      <c r="BY4" s="284"/>
+      <c r="BZ4" s="284"/>
+      <c r="CA4" s="284"/>
+      <c r="CB4" s="284"/>
+      <c r="CC4" s="284"/>
+      <c r="CD4" s="284"/>
+      <c r="CE4" s="285"/>
+      <c r="CF4" s="297" t="s">
         <v>17</v>
       </c>
-      <c r="CG4" s="262"/>
-      <c r="CH4" s="262"/>
-      <c r="CI4" s="262"/>
-      <c r="CJ4" s="263"/>
+      <c r="CG4" s="298"/>
+      <c r="CH4" s="298"/>
+      <c r="CI4" s="298"/>
+      <c r="CJ4" s="299"/>
       <c r="CK4" s="149"/>
       <c r="CL4" s="142"/>
     </row>
     <row r="5" spans="2:98" s="122" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="283" t="s">
+      <c r="B5" s="286" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="284"/>
-      <c r="D5" s="285" t="s">
+      <c r="C5" s="287"/>
+      <c r="D5" s="288" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="286"/>
-      <c r="F5" s="286"/>
-      <c r="G5" s="286"/>
-      <c r="H5" s="287"/>
-      <c r="I5" s="288" t="s">
+      <c r="E5" s="289"/>
+      <c r="F5" s="289"/>
+      <c r="G5" s="289"/>
+      <c r="H5" s="290"/>
+      <c r="I5" s="291" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="289"/>
-      <c r="K5" s="289"/>
-      <c r="L5" s="289"/>
-      <c r="M5" s="290"/>
-      <c r="N5" s="291" t="s">
+      <c r="J5" s="292"/>
+      <c r="K5" s="292"/>
+      <c r="L5" s="292"/>
+      <c r="M5" s="293"/>
+      <c r="N5" s="294" t="s">
         <v>37</v>
       </c>
-      <c r="O5" s="292"/>
-      <c r="P5" s="292"/>
-      <c r="Q5" s="292"/>
-      <c r="R5" s="292"/>
-      <c r="S5" s="292"/>
-      <c r="T5" s="292"/>
-      <c r="U5" s="292"/>
-      <c r="V5" s="292"/>
-      <c r="W5" s="293"/>
-      <c r="X5" s="261" t="s">
+      <c r="O5" s="295"/>
+      <c r="P5" s="295"/>
+      <c r="Q5" s="295"/>
+      <c r="R5" s="295"/>
+      <c r="S5" s="295"/>
+      <c r="T5" s="295"/>
+      <c r="U5" s="295"/>
+      <c r="V5" s="295"/>
+      <c r="W5" s="296"/>
+      <c r="X5" s="297" t="s">
         <v>48</v>
       </c>
-      <c r="Y5" s="262"/>
-      <c r="Z5" s="262"/>
-      <c r="AA5" s="262"/>
-      <c r="AB5" s="262"/>
-      <c r="AC5" s="262"/>
-      <c r="AD5" s="262"/>
-      <c r="AE5" s="262"/>
-      <c r="AF5" s="262"/>
-      <c r="AG5" s="263"/>
-      <c r="AH5" s="261" t="s">
+      <c r="Y5" s="298"/>
+      <c r="Z5" s="298"/>
+      <c r="AA5" s="298"/>
+      <c r="AB5" s="298"/>
+      <c r="AC5" s="298"/>
+      <c r="AD5" s="298"/>
+      <c r="AE5" s="298"/>
+      <c r="AF5" s="298"/>
+      <c r="AG5" s="299"/>
+      <c r="AH5" s="297" t="s">
         <v>50</v>
       </c>
-      <c r="AI5" s="262"/>
-      <c r="AJ5" s="262"/>
-      <c r="AK5" s="262"/>
-      <c r="AL5" s="262"/>
-      <c r="AM5" s="262"/>
-      <c r="AN5" s="262"/>
-      <c r="AO5" s="262"/>
-      <c r="AP5" s="262"/>
-      <c r="AQ5" s="262"/>
-      <c r="AR5" s="262"/>
-      <c r="AS5" s="262"/>
-      <c r="AT5" s="262"/>
-      <c r="AU5" s="262"/>
-      <c r="AV5" s="262"/>
-      <c r="AW5" s="262"/>
-      <c r="AX5" s="262"/>
-      <c r="AY5" s="262"/>
-      <c r="AZ5" s="262"/>
-      <c r="BA5" s="263"/>
-      <c r="BB5" s="280" t="s">
+      <c r="AI5" s="298"/>
+      <c r="AJ5" s="298"/>
+      <c r="AK5" s="298"/>
+      <c r="AL5" s="298"/>
+      <c r="AM5" s="298"/>
+      <c r="AN5" s="298"/>
+      <c r="AO5" s="298"/>
+      <c r="AP5" s="298"/>
+      <c r="AQ5" s="298"/>
+      <c r="AR5" s="298"/>
+      <c r="AS5" s="298"/>
+      <c r="AT5" s="298"/>
+      <c r="AU5" s="298"/>
+      <c r="AV5" s="298"/>
+      <c r="AW5" s="298"/>
+      <c r="AX5" s="298"/>
+      <c r="AY5" s="298"/>
+      <c r="AZ5" s="298"/>
+      <c r="BA5" s="299"/>
+      <c r="BB5" s="301" t="s">
         <v>54</v>
       </c>
-      <c r="BC5" s="281"/>
-      <c r="BD5" s="281"/>
-      <c r="BE5" s="281"/>
-      <c r="BF5" s="281"/>
-      <c r="BG5" s="281"/>
-      <c r="BH5" s="281"/>
-      <c r="BI5" s="281"/>
-      <c r="BJ5" s="281"/>
-      <c r="BK5" s="282"/>
-      <c r="BL5" s="280" t="s">
+      <c r="BC5" s="302"/>
+      <c r="BD5" s="302"/>
+      <c r="BE5" s="302"/>
+      <c r="BF5" s="302"/>
+      <c r="BG5" s="302"/>
+      <c r="BH5" s="302"/>
+      <c r="BI5" s="302"/>
+      <c r="BJ5" s="302"/>
+      <c r="BK5" s="303"/>
+      <c r="BL5" s="301" t="s">
         <v>72</v>
       </c>
-      <c r="BM5" s="281"/>
-      <c r="BN5" s="281"/>
-      <c r="BO5" s="281"/>
-      <c r="BP5" s="281"/>
-      <c r="BQ5" s="281"/>
-      <c r="BR5" s="281"/>
-      <c r="BS5" s="281"/>
-      <c r="BT5" s="281"/>
-      <c r="BU5" s="281"/>
-      <c r="BV5" s="281"/>
-      <c r="BW5" s="281"/>
-      <c r="BX5" s="281"/>
-      <c r="BY5" s="281"/>
-      <c r="BZ5" s="281"/>
-      <c r="CA5" s="281"/>
-      <c r="CB5" s="281"/>
-      <c r="CC5" s="281"/>
-      <c r="CD5" s="281"/>
-      <c r="CE5" s="282"/>
-      <c r="CF5" s="264" t="s">
+      <c r="BM5" s="302"/>
+      <c r="BN5" s="302"/>
+      <c r="BO5" s="302"/>
+      <c r="BP5" s="302"/>
+      <c r="BQ5" s="302"/>
+      <c r="BR5" s="302"/>
+      <c r="BS5" s="302"/>
+      <c r="BT5" s="302"/>
+      <c r="BU5" s="302"/>
+      <c r="BV5" s="302"/>
+      <c r="BW5" s="302"/>
+      <c r="BX5" s="302"/>
+      <c r="BY5" s="302"/>
+      <c r="BZ5" s="302"/>
+      <c r="CA5" s="302"/>
+      <c r="CB5" s="302"/>
+      <c r="CC5" s="302"/>
+      <c r="CD5" s="302"/>
+      <c r="CE5" s="303"/>
+      <c r="CF5" s="304" t="s">
         <v>149</v>
       </c>
-      <c r="CG5" s="265"/>
-      <c r="CH5" s="265"/>
-      <c r="CI5" s="265"/>
-      <c r="CJ5" s="266"/>
+      <c r="CG5" s="305"/>
+      <c r="CH5" s="305"/>
+      <c r="CI5" s="305"/>
+      <c r="CJ5" s="306"/>
       <c r="CK5" s="150"/>
       <c r="CL5" s="143"/>
     </row>
     <row r="6" spans="2:98" s="137" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="156"/>
       <c r="C6" s="157"/>
-      <c r="D6" s="273" t="s">
+      <c r="D6" s="313" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="273"/>
-      <c r="F6" s="273"/>
-      <c r="G6" s="273"/>
-      <c r="H6" s="273"/>
-      <c r="I6" s="274" t="s">
+      <c r="E6" s="313"/>
+      <c r="F6" s="313"/>
+      <c r="G6" s="313"/>
+      <c r="H6" s="313"/>
+      <c r="I6" s="314" t="s">
         <v>79</v>
       </c>
-      <c r="J6" s="275"/>
-      <c r="K6" s="275"/>
-      <c r="L6" s="275"/>
-      <c r="M6" s="276"/>
-      <c r="N6" s="277" t="s">
+      <c r="J6" s="315"/>
+      <c r="K6" s="315"/>
+      <c r="L6" s="315"/>
+      <c r="M6" s="316"/>
+      <c r="N6" s="317" t="s">
         <v>78</v>
       </c>
-      <c r="O6" s="277"/>
-      <c r="P6" s="277"/>
-      <c r="Q6" s="277"/>
-      <c r="R6" s="277"/>
-      <c r="S6" s="277" t="s">
+      <c r="O6" s="317"/>
+      <c r="P6" s="317"/>
+      <c r="Q6" s="317"/>
+      <c r="R6" s="317"/>
+      <c r="S6" s="317" t="s">
         <v>79</v>
       </c>
-      <c r="T6" s="277"/>
-      <c r="U6" s="277"/>
-      <c r="V6" s="277"/>
-      <c r="W6" s="277"/>
-      <c r="X6" s="278" t="s">
+      <c r="T6" s="317"/>
+      <c r="U6" s="317"/>
+      <c r="V6" s="317"/>
+      <c r="W6" s="317"/>
+      <c r="X6" s="318" t="s">
         <v>78</v>
       </c>
-      <c r="Y6" s="278"/>
-      <c r="Z6" s="278"/>
-      <c r="AA6" s="278"/>
-      <c r="AB6" s="278"/>
-      <c r="AC6" s="278" t="s">
+      <c r="Y6" s="318"/>
+      <c r="Z6" s="318"/>
+      <c r="AA6" s="318"/>
+      <c r="AB6" s="318"/>
+      <c r="AC6" s="318" t="s">
         <v>79</v>
       </c>
-      <c r="AD6" s="278"/>
-      <c r="AE6" s="278"/>
-      <c r="AF6" s="278"/>
-      <c r="AG6" s="278"/>
-      <c r="AH6" s="278" t="s">
+      <c r="AD6" s="318"/>
+      <c r="AE6" s="318"/>
+      <c r="AF6" s="318"/>
+      <c r="AG6" s="318"/>
+      <c r="AH6" s="318" t="s">
         <v>78</v>
       </c>
-      <c r="AI6" s="278"/>
-      <c r="AJ6" s="278"/>
-      <c r="AK6" s="278"/>
-      <c r="AL6" s="278"/>
-      <c r="AM6" s="278" t="s">
+      <c r="AI6" s="318"/>
+      <c r="AJ6" s="318"/>
+      <c r="AK6" s="318"/>
+      <c r="AL6" s="318"/>
+      <c r="AM6" s="318" t="s">
         <v>79</v>
       </c>
-      <c r="AN6" s="278"/>
-      <c r="AO6" s="278"/>
-      <c r="AP6" s="278"/>
-      <c r="AQ6" s="278"/>
-      <c r="AR6" s="278" t="s">
+      <c r="AN6" s="318"/>
+      <c r="AO6" s="318"/>
+      <c r="AP6" s="318"/>
+      <c r="AQ6" s="318"/>
+      <c r="AR6" s="318" t="s">
         <v>80</v>
       </c>
-      <c r="AS6" s="278"/>
-      <c r="AT6" s="278"/>
-      <c r="AU6" s="278"/>
-      <c r="AV6" s="278"/>
-      <c r="AW6" s="278" t="s">
+      <c r="AS6" s="318"/>
+      <c r="AT6" s="318"/>
+      <c r="AU6" s="318"/>
+      <c r="AV6" s="318"/>
+      <c r="AW6" s="318" t="s">
         <v>81</v>
       </c>
-      <c r="AX6" s="278"/>
-      <c r="AY6" s="278"/>
-      <c r="AZ6" s="278"/>
-      <c r="BA6" s="278"/>
-      <c r="BB6" s="279" t="s">
+      <c r="AX6" s="318"/>
+      <c r="AY6" s="318"/>
+      <c r="AZ6" s="318"/>
+      <c r="BA6" s="318"/>
+      <c r="BB6" s="300" t="s">
         <v>78</v>
       </c>
-      <c r="BC6" s="279"/>
-      <c r="BD6" s="279"/>
-      <c r="BE6" s="279"/>
-      <c r="BF6" s="279"/>
-      <c r="BG6" s="279" t="s">
+      <c r="BC6" s="300"/>
+      <c r="BD6" s="300"/>
+      <c r="BE6" s="300"/>
+      <c r="BF6" s="300"/>
+      <c r="BG6" s="300" t="s">
         <v>79</v>
       </c>
-      <c r="BH6" s="279"/>
-      <c r="BI6" s="279"/>
-      <c r="BJ6" s="279"/>
-      <c r="BK6" s="279"/>
-      <c r="BL6" s="279" t="s">
+      <c r="BH6" s="300"/>
+      <c r="BI6" s="300"/>
+      <c r="BJ6" s="300"/>
+      <c r="BK6" s="300"/>
+      <c r="BL6" s="300" t="s">
         <v>78</v>
       </c>
-      <c r="BM6" s="279"/>
-      <c r="BN6" s="279"/>
-      <c r="BO6" s="279"/>
-      <c r="BP6" s="279"/>
-      <c r="BQ6" s="279" t="s">
+      <c r="BM6" s="300"/>
+      <c r="BN6" s="300"/>
+      <c r="BO6" s="300"/>
+      <c r="BP6" s="300"/>
+      <c r="BQ6" s="300" t="s">
         <v>82</v>
       </c>
-      <c r="BR6" s="279"/>
-      <c r="BS6" s="279"/>
-      <c r="BT6" s="279"/>
-      <c r="BU6" s="279"/>
-      <c r="BV6" s="279" t="s">
+      <c r="BR6" s="300"/>
+      <c r="BS6" s="300"/>
+      <c r="BT6" s="300"/>
+      <c r="BU6" s="300"/>
+      <c r="BV6" s="300" t="s">
         <v>119</v>
       </c>
-      <c r="BW6" s="279"/>
-      <c r="BX6" s="279"/>
-      <c r="BY6" s="279"/>
-      <c r="BZ6" s="279"/>
-      <c r="CA6" s="279" t="s">
+      <c r="BW6" s="300"/>
+      <c r="BX6" s="300"/>
+      <c r="BY6" s="300"/>
+      <c r="BZ6" s="300"/>
+      <c r="CA6" s="300" t="s">
         <v>79</v>
       </c>
-      <c r="CB6" s="279"/>
-      <c r="CC6" s="279"/>
-      <c r="CD6" s="279"/>
-      <c r="CE6" s="279"/>
-      <c r="CF6" s="267" t="s">
+      <c r="CB6" s="300"/>
+      <c r="CC6" s="300"/>
+      <c r="CD6" s="300"/>
+      <c r="CE6" s="300"/>
+      <c r="CF6" s="307" t="s">
         <v>78</v>
       </c>
-      <c r="CG6" s="268"/>
-      <c r="CH6" s="268"/>
-      <c r="CI6" s="268"/>
-      <c r="CJ6" s="269"/>
+      <c r="CG6" s="308"/>
+      <c r="CH6" s="308"/>
+      <c r="CI6" s="308"/>
+      <c r="CJ6" s="309"/>
       <c r="CK6" s="158" t="s">
         <v>77</v>
       </c>
@@ -21484,36 +21634,6 @@
   </sortState>
   <dataConsolidate/>
   <mergeCells count="46">
-    <mergeCell ref="AS2:BD2"/>
-    <mergeCell ref="X2:AR2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:W3"/>
-    <mergeCell ref="X3:AG3"/>
-    <mergeCell ref="AH3:BA3"/>
-    <mergeCell ref="BB3:BK3"/>
-    <mergeCell ref="BL3:CE3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="I4:M4"/>
-    <mergeCell ref="N4:W4"/>
-    <mergeCell ref="X4:AG4"/>
-    <mergeCell ref="AH4:BA4"/>
-    <mergeCell ref="BB4:BK4"/>
-    <mergeCell ref="BL4:CE4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="N5:W5"/>
-    <mergeCell ref="X5:AG5"/>
-    <mergeCell ref="BB6:BF6"/>
-    <mergeCell ref="BG6:BK6"/>
-    <mergeCell ref="BL6:BP6"/>
-    <mergeCell ref="BQ6:BU6"/>
-    <mergeCell ref="BB5:BK5"/>
-    <mergeCell ref="BL5:CE5"/>
-    <mergeCell ref="CA6:CE6"/>
     <mergeCell ref="CF4:CJ4"/>
     <mergeCell ref="CF5:CJ5"/>
     <mergeCell ref="CF6:CJ6"/>
@@ -21530,6 +21650,36 @@
     <mergeCell ref="BV6:BZ6"/>
     <mergeCell ref="AR6:AV6"/>
     <mergeCell ref="AW6:BA6"/>
+    <mergeCell ref="BB6:BF6"/>
+    <mergeCell ref="BG6:BK6"/>
+    <mergeCell ref="BL6:BP6"/>
+    <mergeCell ref="BQ6:BU6"/>
+    <mergeCell ref="BB5:BK5"/>
+    <mergeCell ref="BL5:CE5"/>
+    <mergeCell ref="CA6:CE6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="N5:W5"/>
+    <mergeCell ref="X5:AG5"/>
+    <mergeCell ref="BL3:CE3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="I4:M4"/>
+    <mergeCell ref="N4:W4"/>
+    <mergeCell ref="X4:AG4"/>
+    <mergeCell ref="AH4:BA4"/>
+    <mergeCell ref="BB4:BK4"/>
+    <mergeCell ref="BL4:CE4"/>
+    <mergeCell ref="AS2:BD2"/>
+    <mergeCell ref="X2:AR2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:W3"/>
+    <mergeCell ref="X3:AG3"/>
+    <mergeCell ref="AH3:BA3"/>
+    <mergeCell ref="BB3:BK3"/>
   </mergeCells>
   <conditionalFormatting sqref="CK35">
     <cfRule type="top10" dxfId="40" priority="38" percent="1" bottom="1" rank="10"/>
@@ -21649,8 +21799,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="3073" r:id="rId4" name="BtnAddAssess">
+        <control shapeId="3075" r:id="rId4" name="BtnEditAssess">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3075" r:id="rId4" name="BtnEditAssess"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3073" r:id="rId6" name="BtnAddAssess">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
@@ -21669,32 +21844,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="3073" r:id="rId4" name="BtnAddAssess"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="3075" r:id="rId6" name="BtnEditAssess">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>457200</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="3075" r:id="rId6" name="BtnEditAssess"/>
+        <control shapeId="3073" r:id="rId6" name="BtnAddAssess"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -22318,14 +22468,14 @@
       </c>
     </row>
     <row r="3" spans="1:11" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="322" t="s">
+      <c r="A3" s="319" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="323"/>
-      <c r="C3" s="323"/>
-      <c r="D3" s="323"/>
-      <c r="E3" s="323"/>
-      <c r="F3" s="324"/>
+      <c r="B3" s="320"/>
+      <c r="C3" s="320"/>
+      <c r="D3" s="320"/>
+      <c r="E3" s="320"/>
+      <c r="F3" s="321"/>
       <c r="H3" s="74"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -22370,14 +22520,14 @@
     </row>
     <row r="6" spans="1:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:11" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="322" t="s">
+      <c r="A7" s="319" t="s">
         <v>111</v>
       </c>
-      <c r="B7" s="323"/>
-      <c r="C7" s="323"/>
-      <c r="D7" s="323"/>
-      <c r="E7" s="323"/>
-      <c r="F7" s="324"/>
+      <c r="B7" s="320"/>
+      <c r="C7" s="320"/>
+      <c r="D7" s="320"/>
+      <c r="E7" s="320"/>
+      <c r="F7" s="321"/>
       <c r="H7" s="74"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -22390,11 +22540,11 @@
       <c r="C8" s="57" t="s">
         <v>113</v>
       </c>
-      <c r="D8" s="325" t="s">
+      <c r="D8" s="322" t="s">
         <v>237</v>
       </c>
-      <c r="E8" s="326"/>
-      <c r="F8" s="327"/>
+      <c r="E8" s="323"/>
+      <c r="F8" s="324"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="55" t="s">
@@ -22418,27 +22568,27 @@
     </row>
     <row r="10" spans="1:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:11" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="322" t="s">
+      <c r="A11" s="319" t="s">
         <v>88</v>
       </c>
-      <c r="B11" s="323"/>
-      <c r="C11" s="323"/>
-      <c r="D11" s="323"/>
-      <c r="E11" s="323"/>
-      <c r="F11" s="324"/>
+      <c r="B11" s="320"/>
+      <c r="C11" s="320"/>
+      <c r="D11" s="320"/>
+      <c r="E11" s="320"/>
+      <c r="F11" s="321"/>
       <c r="H11" s="74"/>
     </row>
     <row r="12" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="328" t="s">
+      <c r="B12" s="325" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="329"/>
-      <c r="D12" s="329"/>
-      <c r="E12" s="329"/>
-      <c r="F12" s="330"/>
+      <c r="C12" s="326"/>
+      <c r="D12" s="326"/>
+      <c r="E12" s="326"/>
+      <c r="F12" s="327"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="64"/>
@@ -22454,25 +22604,25 @@
     </row>
     <row r="14" spans="1:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:11" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="322" t="s">
+      <c r="A15" s="319" t="s">
         <v>86</v>
       </c>
-      <c r="B15" s="323"/>
-      <c r="C15" s="323"/>
-      <c r="D15" s="323"/>
-      <c r="E15" s="323"/>
-      <c r="F15" s="324"/>
+      <c r="B15" s="320"/>
+      <c r="C15" s="320"/>
+      <c r="D15" s="320"/>
+      <c r="E15" s="320"/>
+      <c r="F15" s="321"/>
       <c r="H15" s="74"/>
     </row>
     <row r="16" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="B16" s="319"/>
-      <c r="C16" s="320"/>
-      <c r="D16" s="320"/>
-      <c r="E16" s="320"/>
-      <c r="F16" s="321"/>
+      <c r="B16" s="328"/>
+      <c r="C16" s="329"/>
+      <c r="D16" s="329"/>
+      <c r="E16" s="329"/>
+      <c r="F16" s="330"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="64"/>
@@ -22488,25 +22638,25 @@
     </row>
     <row r="18" spans="1:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:8" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="322" t="s">
+      <c r="A19" s="319" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="323"/>
-      <c r="C19" s="323"/>
-      <c r="D19" s="323"/>
-      <c r="E19" s="323"/>
-      <c r="F19" s="324"/>
+      <c r="B19" s="320"/>
+      <c r="C19" s="320"/>
+      <c r="D19" s="320"/>
+      <c r="E19" s="320"/>
+      <c r="F19" s="321"/>
       <c r="H19" s="74"/>
     </row>
     <row r="20" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="319"/>
-      <c r="C20" s="320"/>
-      <c r="D20" s="320"/>
-      <c r="E20" s="320"/>
-      <c r="F20" s="321"/>
+      <c r="B20" s="328"/>
+      <c r="C20" s="329"/>
+      <c r="D20" s="329"/>
+      <c r="E20" s="329"/>
+      <c r="F20" s="330"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="64"/>
@@ -22522,25 +22672,25 @@
     </row>
     <row r="22" spans="1:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:8" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="322" t="s">
+      <c r="A23" s="319" t="s">
         <v>117</v>
       </c>
-      <c r="B23" s="323"/>
-      <c r="C23" s="323"/>
-      <c r="D23" s="323"/>
-      <c r="E23" s="323"/>
-      <c r="F23" s="324"/>
+      <c r="B23" s="320"/>
+      <c r="C23" s="320"/>
+      <c r="D23" s="320"/>
+      <c r="E23" s="320"/>
+      <c r="F23" s="321"/>
       <c r="H23" s="74"/>
     </row>
     <row r="24" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="B24" s="319"/>
-      <c r="C24" s="320"/>
-      <c r="D24" s="320"/>
-      <c r="E24" s="320"/>
-      <c r="F24" s="321"/>
+      <c r="B24" s="328"/>
+      <c r="C24" s="329"/>
+      <c r="D24" s="329"/>
+      <c r="E24" s="329"/>
+      <c r="F24" s="330"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="64"/>
@@ -22556,27 +22706,27 @@
     </row>
     <row r="26" spans="1:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:8" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="322" t="s">
+      <c r="A27" s="319" t="s">
         <v>118</v>
       </c>
-      <c r="B27" s="323"/>
-      <c r="C27" s="323"/>
-      <c r="D27" s="323"/>
-      <c r="E27" s="323"/>
-      <c r="F27" s="324"/>
+      <c r="B27" s="320"/>
+      <c r="C27" s="320"/>
+      <c r="D27" s="320"/>
+      <c r="E27" s="320"/>
+      <c r="F27" s="321"/>
       <c r="H27" s="74"/>
     </row>
     <row r="28" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="B28" s="319" t="s">
+      <c r="B28" s="328" t="s">
         <v>238</v>
       </c>
-      <c r="C28" s="320"/>
-      <c r="D28" s="320"/>
-      <c r="E28" s="320"/>
-      <c r="F28" s="321"/>
+      <c r="C28" s="329"/>
+      <c r="D28" s="329"/>
+      <c r="E28" s="329"/>
+      <c r="F28" s="330"/>
       <c r="H28" s="74" t="s">
         <v>238</v>
       </c>
@@ -22592,12 +22742,6 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="13">
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="B12:F12"/>
     <mergeCell ref="B28:F28"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="A19:F19"/>
@@ -22605,6 +22749,12 @@
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="B12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -22807,30 +22957,30 @@
         <v>120</v>
       </c>
       <c r="C3" s="100"/>
-      <c r="E3" s="344">
+      <c r="E3" s="355">
         <v>5665</v>
       </c>
-      <c r="F3" s="344"/>
+      <c r="F3" s="355"/>
       <c r="G3" s="96" t="s">
         <v>93</v>
       </c>
-      <c r="I3" s="344" t="s">
+      <c r="I3" s="355" t="s">
         <v>236</v>
       </c>
-      <c r="J3" s="344"/>
-      <c r="K3" s="344"/>
-      <c r="L3" s="344"/>
-      <c r="M3" s="344"/>
+      <c r="J3" s="355"/>
+      <c r="K3" s="355"/>
+      <c r="L3" s="355"/>
+      <c r="M3" s="355"/>
       <c r="N3" s="96" t="s">
         <v>108</v>
       </c>
-      <c r="P3" s="344" t="s">
+      <c r="P3" s="355" t="s">
         <v>170</v>
       </c>
-      <c r="Q3" s="344"/>
-      <c r="R3" s="344"/>
-      <c r="S3" s="344"/>
-      <c r="T3" s="344"/>
+      <c r="Q3" s="355"/>
+      <c r="R3" s="355"/>
+      <c r="S3" s="355"/>
+      <c r="T3" s="355"/>
       <c r="V3" s="96" t="s">
         <v>109</v>
       </c>
@@ -22841,10 +22991,10 @@
         <v>63</v>
       </c>
       <c r="AD3" s="99"/>
-      <c r="AF3" s="343" t="s">
+      <c r="AF3" s="354" t="s">
         <v>234</v>
       </c>
-      <c r="AG3" s="343"/>
+      <c r="AG3" s="354"/>
     </row>
     <row r="5" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="76" t="s">
@@ -23437,148 +23587,153 @@
     </row>
     <row r="17" spans="2:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="348" t="s">
+      <c r="B18" s="346" t="s">
         <v>142</v>
       </c>
-      <c r="C18" s="349"/>
-      <c r="D18" s="345" t="s">
+      <c r="C18" s="347"/>
+      <c r="D18" s="343" t="s">
         <v>137</v>
       </c>
-      <c r="E18" s="346"/>
-      <c r="F18" s="346"/>
-      <c r="G18" s="346"/>
-      <c r="H18" s="346"/>
-      <c r="I18" s="346"/>
-      <c r="J18" s="346"/>
-      <c r="K18" s="346"/>
-      <c r="L18" s="346"/>
-      <c r="M18" s="346"/>
-      <c r="N18" s="346"/>
-      <c r="O18" s="346"/>
-      <c r="P18" s="346"/>
-      <c r="Q18" s="346"/>
-      <c r="R18" s="346"/>
-      <c r="S18" s="346"/>
-      <c r="T18" s="346"/>
-      <c r="U18" s="346"/>
-      <c r="V18" s="346"/>
-      <c r="W18" s="347"/>
+      <c r="E18" s="344"/>
+      <c r="F18" s="344"/>
+      <c r="G18" s="344"/>
+      <c r="H18" s="344"/>
+      <c r="I18" s="344"/>
+      <c r="J18" s="344"/>
+      <c r="K18" s="344"/>
+      <c r="L18" s="344"/>
+      <c r="M18" s="344"/>
+      <c r="N18" s="344"/>
+      <c r="O18" s="344"/>
+      <c r="P18" s="344"/>
+      <c r="Q18" s="344"/>
+      <c r="R18" s="344"/>
+      <c r="S18" s="344"/>
+      <c r="T18" s="344"/>
+      <c r="U18" s="344"/>
+      <c r="V18" s="344"/>
+      <c r="W18" s="345"/>
     </row>
     <row r="19" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="350">
+      <c r="B19" s="348">
         <v>2</v>
       </c>
-      <c r="C19" s="351"/>
-      <c r="D19" s="345" t="s">
+      <c r="C19" s="349"/>
+      <c r="D19" s="343" t="s">
         <v>138</v>
       </c>
-      <c r="E19" s="346"/>
-      <c r="F19" s="346"/>
-      <c r="G19" s="346"/>
-      <c r="H19" s="346"/>
-      <c r="I19" s="346"/>
-      <c r="J19" s="346"/>
-      <c r="K19" s="346"/>
-      <c r="L19" s="346"/>
-      <c r="M19" s="346"/>
-      <c r="N19" s="346"/>
-      <c r="O19" s="346"/>
-      <c r="P19" s="346"/>
-      <c r="Q19" s="346"/>
-      <c r="R19" s="346"/>
-      <c r="S19" s="346"/>
-      <c r="T19" s="346"/>
-      <c r="U19" s="346"/>
-      <c r="V19" s="346"/>
-      <c r="W19" s="347"/>
+      <c r="E19" s="344"/>
+      <c r="F19" s="344"/>
+      <c r="G19" s="344"/>
+      <c r="H19" s="344"/>
+      <c r="I19" s="344"/>
+      <c r="J19" s="344"/>
+      <c r="K19" s="344"/>
+      <c r="L19" s="344"/>
+      <c r="M19" s="344"/>
+      <c r="N19" s="344"/>
+      <c r="O19" s="344"/>
+      <c r="P19" s="344"/>
+      <c r="Q19" s="344"/>
+      <c r="R19" s="344"/>
+      <c r="S19" s="344"/>
+      <c r="T19" s="344"/>
+      <c r="U19" s="344"/>
+      <c r="V19" s="344"/>
+      <c r="W19" s="345"/>
     </row>
     <row r="20" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="352">
+      <c r="B20" s="350">
         <v>3</v>
       </c>
-      <c r="C20" s="353"/>
-      <c r="D20" s="345" t="s">
+      <c r="C20" s="351"/>
+      <c r="D20" s="343" t="s">
         <v>139</v>
       </c>
-      <c r="E20" s="346"/>
-      <c r="F20" s="346"/>
-      <c r="G20" s="346"/>
-      <c r="H20" s="346"/>
-      <c r="I20" s="346"/>
-      <c r="J20" s="346"/>
-      <c r="K20" s="346"/>
-      <c r="L20" s="346"/>
-      <c r="M20" s="346"/>
-      <c r="N20" s="346"/>
-      <c r="O20" s="346"/>
-      <c r="P20" s="346"/>
-      <c r="Q20" s="346"/>
-      <c r="R20" s="346"/>
-      <c r="S20" s="346"/>
-      <c r="T20" s="346"/>
-      <c r="U20" s="346"/>
-      <c r="V20" s="346"/>
-      <c r="W20" s="347"/>
+      <c r="E20" s="344"/>
+      <c r="F20" s="344"/>
+      <c r="G20" s="344"/>
+      <c r="H20" s="344"/>
+      <c r="I20" s="344"/>
+      <c r="J20" s="344"/>
+      <c r="K20" s="344"/>
+      <c r="L20" s="344"/>
+      <c r="M20" s="344"/>
+      <c r="N20" s="344"/>
+      <c r="O20" s="344"/>
+      <c r="P20" s="344"/>
+      <c r="Q20" s="344"/>
+      <c r="R20" s="344"/>
+      <c r="S20" s="344"/>
+      <c r="T20" s="344"/>
+      <c r="U20" s="344"/>
+      <c r="V20" s="344"/>
+      <c r="W20" s="345"/>
     </row>
     <row r="21" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="354">
+      <c r="B21" s="352">
         <v>4</v>
       </c>
-      <c r="C21" s="355"/>
-      <c r="D21" s="345" t="s">
+      <c r="C21" s="353"/>
+      <c r="D21" s="343" t="s">
         <v>140</v>
       </c>
-      <c r="E21" s="346"/>
-      <c r="F21" s="346"/>
-      <c r="G21" s="346"/>
-      <c r="H21" s="346"/>
-      <c r="I21" s="346"/>
-      <c r="J21" s="346"/>
-      <c r="K21" s="346"/>
-      <c r="L21" s="346"/>
-      <c r="M21" s="346"/>
-      <c r="N21" s="346"/>
-      <c r="O21" s="346"/>
-      <c r="P21" s="346"/>
-      <c r="Q21" s="346"/>
-      <c r="R21" s="346"/>
-      <c r="S21" s="346"/>
-      <c r="T21" s="346"/>
-      <c r="U21" s="346"/>
-      <c r="V21" s="346"/>
-      <c r="W21" s="347"/>
+      <c r="E21" s="344"/>
+      <c r="F21" s="344"/>
+      <c r="G21" s="344"/>
+      <c r="H21" s="344"/>
+      <c r="I21" s="344"/>
+      <c r="J21" s="344"/>
+      <c r="K21" s="344"/>
+      <c r="L21" s="344"/>
+      <c r="M21" s="344"/>
+      <c r="N21" s="344"/>
+      <c r="O21" s="344"/>
+      <c r="P21" s="344"/>
+      <c r="Q21" s="344"/>
+      <c r="R21" s="344"/>
+      <c r="S21" s="344"/>
+      <c r="T21" s="344"/>
+      <c r="U21" s="344"/>
+      <c r="V21" s="344"/>
+      <c r="W21" s="345"/>
     </row>
     <row r="22" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="354">
+      <c r="B22" s="352">
         <v>5</v>
       </c>
-      <c r="C22" s="355"/>
-      <c r="D22" s="345" t="s">
+      <c r="C22" s="353"/>
+      <c r="D22" s="343" t="s">
         <v>141</v>
       </c>
-      <c r="E22" s="346"/>
-      <c r="F22" s="346"/>
-      <c r="G22" s="346"/>
-      <c r="H22" s="346"/>
-      <c r="I22" s="346"/>
-      <c r="J22" s="346"/>
-      <c r="K22" s="346"/>
-      <c r="L22" s="346"/>
-      <c r="M22" s="346"/>
-      <c r="N22" s="346"/>
-      <c r="O22" s="346"/>
-      <c r="P22" s="346"/>
-      <c r="Q22" s="346"/>
-      <c r="R22" s="346"/>
-      <c r="S22" s="346"/>
-      <c r="T22" s="346"/>
-      <c r="U22" s="346"/>
-      <c r="V22" s="346"/>
-      <c r="W22" s="347"/>
+      <c r="E22" s="344"/>
+      <c r="F22" s="344"/>
+      <c r="G22" s="344"/>
+      <c r="H22" s="344"/>
+      <c r="I22" s="344"/>
+      <c r="J22" s="344"/>
+      <c r="K22" s="344"/>
+      <c r="L22" s="344"/>
+      <c r="M22" s="344"/>
+      <c r="N22" s="344"/>
+      <c r="O22" s="344"/>
+      <c r="P22" s="344"/>
+      <c r="Q22" s="344"/>
+      <c r="R22" s="344"/>
+      <c r="S22" s="344"/>
+      <c r="T22" s="344"/>
+      <c r="U22" s="344"/>
+      <c r="V22" s="344"/>
+      <c r="W22" s="345"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="14">
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="D18:W18"/>
     <mergeCell ref="D19:W19"/>
     <mergeCell ref="D20:W20"/>
     <mergeCell ref="D21:W21"/>
@@ -23588,11 +23743,6 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="D18:W18"/>
   </mergeCells>
   <conditionalFormatting sqref="B8:AG13">
     <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
@@ -23927,30 +24077,30 @@
       <c r="C4" s="190">
         <v>9</v>
       </c>
-      <c r="D4" s="357">
+      <c r="D4" s="363">
         <v>11</v>
       </c>
-      <c r="E4" s="357"/>
-      <c r="F4" s="357">
+      <c r="E4" s="363"/>
+      <c r="F4" s="363">
         <v>17</v>
       </c>
-      <c r="G4" s="357"/>
-      <c r="H4" s="357">
+      <c r="G4" s="363"/>
+      <c r="H4" s="363">
         <v>20</v>
       </c>
-      <c r="I4" s="357"/>
-      <c r="J4" s="357"/>
-      <c r="K4" s="357"/>
-      <c r="L4" s="357">
+      <c r="I4" s="363"/>
+      <c r="J4" s="363"/>
+      <c r="K4" s="363"/>
+      <c r="L4" s="363">
         <v>27</v>
       </c>
-      <c r="M4" s="357"/>
-      <c r="N4" s="357">
+      <c r="M4" s="363"/>
+      <c r="N4" s="363">
         <v>28</v>
       </c>
-      <c r="O4" s="357"/>
-      <c r="P4" s="357"/>
-      <c r="Q4" s="357"/>
+      <c r="O4" s="363"/>
+      <c r="P4" s="363"/>
+      <c r="Q4" s="363"/>
       <c r="R4" s="190">
         <v>29</v>
       </c>
@@ -23964,30 +24114,30 @@
       <c r="C5" s="185" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="363" t="s">
+      <c r="D5" s="362" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="363"/>
-      <c r="F5" s="358" t="s">
+      <c r="E5" s="362"/>
+      <c r="F5" s="357" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="358"/>
-      <c r="H5" s="358" t="s">
+      <c r="G5" s="357"/>
+      <c r="H5" s="357" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="358"/>
-      <c r="J5" s="358"/>
-      <c r="K5" s="358"/>
-      <c r="L5" s="359" t="s">
+      <c r="I5" s="357"/>
+      <c r="J5" s="357"/>
+      <c r="K5" s="357"/>
+      <c r="L5" s="358" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="359"/>
-      <c r="N5" s="359" t="s">
+      <c r="M5" s="358"/>
+      <c r="N5" s="358" t="s">
         <v>23</v>
       </c>
-      <c r="O5" s="359"/>
-      <c r="P5" s="359"/>
-      <c r="Q5" s="359"/>
+      <c r="O5" s="358"/>
+      <c r="P5" s="358"/>
+      <c r="Q5" s="358"/>
       <c r="R5" s="186" t="s">
         <v>17</v>
       </c>
@@ -24001,30 +24151,30 @@
       <c r="C6" s="188" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="360" t="s">
+      <c r="D6" s="359" t="s">
         <v>37</v>
       </c>
-      <c r="E6" s="360"/>
-      <c r="F6" s="361" t="s">
+      <c r="E6" s="359"/>
+      <c r="F6" s="360" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="361"/>
-      <c r="H6" s="361" t="s">
+      <c r="G6" s="360"/>
+      <c r="H6" s="360" t="s">
         <v>50</v>
       </c>
-      <c r="I6" s="361"/>
-      <c r="J6" s="361"/>
-      <c r="K6" s="361"/>
-      <c r="L6" s="362" t="s">
+      <c r="I6" s="360"/>
+      <c r="J6" s="360"/>
+      <c r="K6" s="360"/>
+      <c r="L6" s="361" t="s">
         <v>54</v>
       </c>
-      <c r="M6" s="362"/>
-      <c r="N6" s="362" t="s">
+      <c r="M6" s="361"/>
+      <c r="N6" s="361" t="s">
         <v>72</v>
       </c>
-      <c r="O6" s="362"/>
-      <c r="P6" s="362"/>
-      <c r="Q6" s="362"/>
+      <c r="O6" s="361"/>
+      <c r="P6" s="361"/>
+      <c r="Q6" s="361"/>
       <c r="R6" s="189" t="s">
         <v>149</v>
       </c>
@@ -24266,6 +24416,11 @@
     <row r="13" spans="1:85" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:Q4"/>
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="N5:Q5"/>
     <mergeCell ref="L5:M5"/>
@@ -24276,11 +24431,6 @@
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:Q4"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:J8 B8:D12 F8:J12 L8:R12">
     <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">

</xml_diff>

<commit_message>
DailyLog Form update Working version
</commit_message>
<xml_diff>
--- a/Phase 1 Candidate Database v2.xlsx
+++ b/Phase 1 Candidate Database v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="20520" windowHeight="8160" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="20520" windowHeight="8160"/>
   </bookViews>
   <sheets>
     <sheet name="Daily Logs" sheetId="8" r:id="rId1"/>
@@ -115,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="393">
   <si>
     <t>DAY</t>
   </si>
@@ -1288,6 +1288,12 @@
   </si>
   <si>
     <t>Jeff Bloom</t>
+  </si>
+  <si>
+    <t>5696</t>
+  </si>
+  <si>
+    <t>John Ashby</t>
   </si>
 </sst>
 </file>
@@ -3566,7 +3572,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="384">
+  <cellXfs count="402">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
@@ -4425,6 +4431,123 @@
     <xf numFmtId="0" fontId="29" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="31" fillId="24" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="24" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="105" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="23" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="23" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="143" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="141" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="30" fillId="6" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="30" fillId="6" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="26" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="26" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="22" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="22" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="25" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="25" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="20" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4434,161 +4557,17 @@
     <xf numFmtId="0" fontId="30" fillId="6" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="6" borderId="142" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="141" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="143" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="30" fillId="6" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="30" fillId="6" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="26" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="26" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="22" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="22" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="24" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="24" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="24" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="23" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="23" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="25" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="25" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="22" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="22" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="22" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="115" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="105" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4617,15 +4596,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4662,6 +4632,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -4695,15 +4671,12 @@
     <xf numFmtId="0" fontId="20" fillId="14" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="121" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="24" borderId="120" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
@@ -4722,8 +4695,95 @@
     <xf numFmtId="0" fontId="31" fillId="22" borderId="120" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="19" borderId="121" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="167" fontId="31" fillId="19" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="19" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="21" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="21" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="19" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="19" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="19" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="115" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5948,14 +6008,14 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCAE2BC"/>
       <color rgb="FFEFEAD1"/>
-      <color rgb="FFCAE2BC"/>
+      <color rgb="FFCB99B2"/>
+      <color rgb="FFD4C685"/>
       <color rgb="FF727571"/>
       <color rgb="FFAED9E0"/>
-      <color rgb="FFD4C685"/>
       <color rgb="FFB0B4B2"/>
       <color rgb="FFEAD7D1"/>
-      <color rgb="FFCB99B2"/>
       <color rgb="FF484A47"/>
       <color rgb="FFFBFEFB"/>
     </mruColors>
@@ -7788,8 +7848,8 @@
   </sheetPr>
   <dimension ref="A1:AY52"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AY8" sqref="AY8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9998,27 +10058,27 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1031" r:id="rId5" name="BtnConnectDB">
+        <control shapeId="1036" r:id="rId5" name="BtnReset">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" r:id="rId6">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>28</xdr:col>
-                <xdr:colOff>285750</xdr:colOff>
+                <xdr:col>24</xdr:col>
+                <xdr:colOff>152400</xdr:colOff>
                 <xdr:row>37</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:rowOff>57150</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>32</xdr:col>
-                <xdr:colOff>285750</xdr:colOff>
+                <xdr:col>28</xdr:col>
+                <xdr:colOff>152400</xdr:colOff>
                 <xdr:row>39</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
+                <xdr:rowOff>66675</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1031" r:id="rId5" name="BtnConnectDB"/>
+        <control shapeId="1036" r:id="rId5" name="BtnReset"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10048,27 +10108,27 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1036" r:id="rId9" name="BtnReset">
+        <control shapeId="1031" r:id="rId9" name="BtnConnectDB">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>24</xdr:col>
-                <xdr:colOff>152400</xdr:colOff>
+                <xdr:col>28</xdr:col>
+                <xdr:colOff>285750</xdr:colOff>
                 <xdr:row>37</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
+                <xdr:rowOff>47625</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>28</xdr:col>
-                <xdr:colOff>152400</xdr:colOff>
+                <xdr:col>32</xdr:col>
+                <xdr:colOff>285750</xdr:colOff>
                 <xdr:row>39</xdr:row>
-                <xdr:rowOff>66675</xdr:rowOff>
+                <xdr:rowOff>57150</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1036" r:id="rId9" name="BtnReset"/>
+        <control shapeId="1031" r:id="rId9" name="BtnConnectDB"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -10193,30 +10253,30 @@
       <c r="C4" s="213">
         <v>9</v>
       </c>
-      <c r="D4" s="383">
+      <c r="D4" s="365">
         <v>11</v>
       </c>
-      <c r="E4" s="383"/>
-      <c r="F4" s="383">
+      <c r="E4" s="365"/>
+      <c r="F4" s="365">
         <v>17</v>
       </c>
-      <c r="G4" s="383"/>
-      <c r="H4" s="383">
+      <c r="G4" s="365"/>
+      <c r="H4" s="365">
         <v>20</v>
       </c>
-      <c r="I4" s="383"/>
-      <c r="J4" s="383"/>
-      <c r="K4" s="383"/>
-      <c r="L4" s="383">
+      <c r="I4" s="365"/>
+      <c r="J4" s="365"/>
+      <c r="K4" s="365"/>
+      <c r="L4" s="365">
         <v>27</v>
       </c>
-      <c r="M4" s="383"/>
-      <c r="N4" s="383">
+      <c r="M4" s="365"/>
+      <c r="N4" s="365">
         <v>28</v>
       </c>
-      <c r="O4" s="383"/>
-      <c r="P4" s="383"/>
-      <c r="Q4" s="383"/>
+      <c r="O4" s="365"/>
+      <c r="P4" s="365"/>
+      <c r="Q4" s="365"/>
       <c r="R4" s="213">
         <v>29</v>
       </c>
@@ -10230,30 +10290,30 @@
       <c r="C5" s="208" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="382" t="s">
+      <c r="D5" s="371" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="382"/>
-      <c r="F5" s="377" t="s">
+      <c r="E5" s="371"/>
+      <c r="F5" s="366" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="377"/>
-      <c r="H5" s="377" t="s">
+      <c r="G5" s="366"/>
+      <c r="H5" s="366" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="377"/>
-      <c r="J5" s="377"/>
-      <c r="K5" s="377"/>
-      <c r="L5" s="378" t="s">
+      <c r="I5" s="366"/>
+      <c r="J5" s="366"/>
+      <c r="K5" s="366"/>
+      <c r="L5" s="367" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="378"/>
-      <c r="N5" s="378" t="s">
+      <c r="M5" s="367"/>
+      <c r="N5" s="367" t="s">
         <v>23</v>
       </c>
-      <c r="O5" s="378"/>
-      <c r="P5" s="378"/>
-      <c r="Q5" s="378"/>
+      <c r="O5" s="367"/>
+      <c r="P5" s="367"/>
+      <c r="Q5" s="367"/>
       <c r="R5" s="209" t="s">
         <v>17</v>
       </c>
@@ -10267,30 +10327,30 @@
       <c r="C6" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="379" t="s">
+      <c r="D6" s="368" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="379"/>
-      <c r="F6" s="380" t="s">
+      <c r="E6" s="368"/>
+      <c r="F6" s="369" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="380"/>
-      <c r="H6" s="380" t="s">
+      <c r="G6" s="369"/>
+      <c r="H6" s="369" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="380"/>
-      <c r="J6" s="380"/>
-      <c r="K6" s="380"/>
-      <c r="L6" s="381" t="s">
+      <c r="I6" s="369"/>
+      <c r="J6" s="369"/>
+      <c r="K6" s="369"/>
+      <c r="L6" s="370" t="s">
         <v>53</v>
       </c>
-      <c r="M6" s="381"/>
-      <c r="N6" s="381" t="s">
+      <c r="M6" s="370"/>
+      <c r="N6" s="370" t="s">
         <v>72</v>
       </c>
-      <c r="O6" s="381"/>
-      <c r="P6" s="381"/>
-      <c r="Q6" s="381"/>
+      <c r="O6" s="370"/>
+      <c r="P6" s="370"/>
+      <c r="Q6" s="370"/>
       <c r="R6" s="212" t="s">
         <v>227</v>
       </c>
@@ -10532,11 +10592,6 @@
     <row r="13" spans="1:85" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:Q4"/>
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="N5:Q5"/>
     <mergeCell ref="L5:M5"/>
@@ -10547,6 +10602,11 @@
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:Q4"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:J8 B8:D12 F8:J12 L8:R12">
     <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
@@ -10651,11 +10711,11 @@
   </sheetPr>
   <dimension ref="A1:EJ53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7:DA35"/>
+      <selection pane="bottomRight" activeCell="BM11" sqref="BM11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10818,41 +10878,41 @@
       <c r="AU2" s="281"/>
       <c r="AV2" s="281"/>
       <c r="AW2" s="281"/>
-      <c r="AX2" s="284" t="str">
+      <c r="AX2" s="323" t="str">
         <f>CONCATENATE("Course No - ", CourseNo)</f>
         <v>Course No - WT2018</v>
       </c>
-      <c r="AY2" s="284"/>
-      <c r="AZ2" s="284"/>
-      <c r="BA2" s="284"/>
-      <c r="BB2" s="284"/>
-      <c r="BC2" s="284"/>
-      <c r="BD2" s="284"/>
-      <c r="BE2" s="284"/>
-      <c r="BF2" s="284"/>
-      <c r="BG2" s="284"/>
-      <c r="BH2" s="284"/>
-      <c r="BI2" s="284"/>
-      <c r="BJ2" s="284"/>
-      <c r="BK2" s="284"/>
-      <c r="BL2" s="284"/>
-      <c r="BM2" s="284"/>
-      <c r="BN2" s="284"/>
-      <c r="BO2" s="284"/>
-      <c r="BP2" s="284"/>
-      <c r="BQ2" s="284"/>
-      <c r="BR2" s="284"/>
-      <c r="BS2" s="284"/>
-      <c r="BT2" s="284"/>
-      <c r="BU2" s="284"/>
-      <c r="BV2" s="284"/>
-      <c r="BW2" s="284"/>
-      <c r="BX2" s="284"/>
-      <c r="BY2" s="284"/>
-      <c r="BZ2" s="284"/>
-      <c r="CA2" s="284"/>
-      <c r="CB2" s="284"/>
-      <c r="CC2" s="284"/>
+      <c r="AY2" s="323"/>
+      <c r="AZ2" s="323"/>
+      <c r="BA2" s="323"/>
+      <c r="BB2" s="323"/>
+      <c r="BC2" s="323"/>
+      <c r="BD2" s="323"/>
+      <c r="BE2" s="323"/>
+      <c r="BF2" s="323"/>
+      <c r="BG2" s="323"/>
+      <c r="BH2" s="323"/>
+      <c r="BI2" s="323"/>
+      <c r="BJ2" s="323"/>
+      <c r="BK2" s="323"/>
+      <c r="BL2" s="323"/>
+      <c r="BM2" s="323"/>
+      <c r="BN2" s="323"/>
+      <c r="BO2" s="323"/>
+      <c r="BP2" s="323"/>
+      <c r="BQ2" s="323"/>
+      <c r="BR2" s="323"/>
+      <c r="BS2" s="323"/>
+      <c r="BT2" s="323"/>
+      <c r="BU2" s="323"/>
+      <c r="BV2" s="323"/>
+      <c r="BW2" s="323"/>
+      <c r="BX2" s="323"/>
+      <c r="BY2" s="323"/>
+      <c r="BZ2" s="323"/>
+      <c r="CA2" s="323"/>
+      <c r="CB2" s="323"/>
+      <c r="CC2" s="323"/>
       <c r="CD2" s="170"/>
       <c r="CE2" s="170"/>
       <c r="CF2" s="170"/>
@@ -10886,18 +10946,18 @@
       <c r="DH2" s="170"/>
     </row>
     <row r="3" spans="2:113" s="129" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="285" t="s">
+      <c r="B3" s="324" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="286"/>
+      <c r="C3" s="325"/>
       <c r="D3" s="287">
         <v>3</v>
       </c>
       <c r="E3" s="287"/>
       <c r="F3" s="287"/>
       <c r="G3" s="287"/>
-      <c r="H3" s="288"/>
-      <c r="I3" s="289">
+      <c r="H3" s="326"/>
+      <c r="I3" s="311">
         <v>10</v>
       </c>
       <c r="J3" s="287"/>
@@ -10908,8 +10968,8 @@
       <c r="O3" s="287"/>
       <c r="P3" s="287"/>
       <c r="Q3" s="287"/>
-      <c r="R3" s="288"/>
-      <c r="S3" s="289">
+      <c r="R3" s="326"/>
+      <c r="S3" s="311">
         <v>13</v>
       </c>
       <c r="T3" s="287"/>
@@ -10920,8 +10980,8 @@
       <c r="Y3" s="287"/>
       <c r="Z3" s="287"/>
       <c r="AA3" s="287"/>
-      <c r="AB3" s="288"/>
-      <c r="AC3" s="289">
+      <c r="AB3" s="326"/>
+      <c r="AC3" s="311">
         <v>24</v>
       </c>
       <c r="AD3" s="287"/>
@@ -10942,8 +11002,8 @@
       <c r="AS3" s="287"/>
       <c r="AT3" s="287"/>
       <c r="AU3" s="287"/>
-      <c r="AV3" s="288"/>
-      <c r="AW3" s="289">
+      <c r="AV3" s="326"/>
+      <c r="AW3" s="311">
         <v>30</v>
       </c>
       <c r="AX3" s="287"/>
@@ -10954,43 +11014,43 @@
       <c r="BC3" s="287"/>
       <c r="BD3" s="287"/>
       <c r="BE3" s="287"/>
-      <c r="BF3" s="288"/>
-      <c r="BG3" s="290">
+      <c r="BF3" s="326"/>
+      <c r="BG3" s="310">
         <v>34</v>
       </c>
-      <c r="BH3" s="290"/>
-      <c r="BI3" s="289"/>
-      <c r="BJ3" s="289"/>
-      <c r="BK3" s="289"/>
-      <c r="BL3" s="289"/>
-      <c r="BM3" s="289"/>
-      <c r="BN3" s="289"/>
-      <c r="BO3" s="289"/>
-      <c r="BP3" s="289"/>
-      <c r="BQ3" s="290">
+      <c r="BH3" s="310"/>
+      <c r="BI3" s="311"/>
+      <c r="BJ3" s="311"/>
+      <c r="BK3" s="311"/>
+      <c r="BL3" s="311"/>
+      <c r="BM3" s="311"/>
+      <c r="BN3" s="311"/>
+      <c r="BO3" s="311"/>
+      <c r="BP3" s="311"/>
+      <c r="BQ3" s="310">
         <v>40</v>
       </c>
-      <c r="BR3" s="290"/>
-      <c r="BS3" s="289"/>
-      <c r="BT3" s="289"/>
-      <c r="BU3" s="289"/>
-      <c r="BV3" s="289"/>
-      <c r="BW3" s="289"/>
-      <c r="BX3" s="289"/>
-      <c r="BY3" s="289"/>
-      <c r="BZ3" s="289"/>
-      <c r="CA3" s="290">
+      <c r="BR3" s="310"/>
+      <c r="BS3" s="311"/>
+      <c r="BT3" s="311"/>
+      <c r="BU3" s="311"/>
+      <c r="BV3" s="311"/>
+      <c r="BW3" s="311"/>
+      <c r="BX3" s="311"/>
+      <c r="BY3" s="311"/>
+      <c r="BZ3" s="311"/>
+      <c r="CA3" s="310">
         <v>43</v>
       </c>
-      <c r="CB3" s="290"/>
-      <c r="CC3" s="289"/>
-      <c r="CD3" s="289"/>
-      <c r="CE3" s="289"/>
-      <c r="CF3" s="289"/>
-      <c r="CG3" s="289"/>
-      <c r="CH3" s="289"/>
-      <c r="CI3" s="289"/>
-      <c r="CJ3" s="290"/>
+      <c r="CB3" s="310"/>
+      <c r="CC3" s="311"/>
+      <c r="CD3" s="311"/>
+      <c r="CE3" s="311"/>
+      <c r="CF3" s="311"/>
+      <c r="CG3" s="311"/>
+      <c r="CH3" s="311"/>
+      <c r="CI3" s="311"/>
+      <c r="CJ3" s="310"/>
       <c r="CK3" s="287">
         <v>46</v>
       </c>
@@ -11007,403 +11067,403 @@
       <c r="CV3" s="287"/>
       <c r="CW3" s="287"/>
       <c r="CX3" s="287"/>
-      <c r="CY3" s="338"/>
+      <c r="CY3" s="288"/>
       <c r="CZ3" s="251"/>
       <c r="DA3" s="252"/>
     </row>
     <row r="4" spans="2:113" s="242" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="291"/>
-      <c r="C4" s="292"/>
-      <c r="D4" s="293">
+      <c r="B4" s="312"/>
+      <c r="C4" s="313"/>
+      <c r="D4" s="314">
         <v>43107</v>
       </c>
-      <c r="E4" s="294"/>
-      <c r="F4" s="294"/>
-      <c r="G4" s="294"/>
-      <c r="H4" s="295"/>
-      <c r="I4" s="305">
+      <c r="E4" s="315"/>
+      <c r="F4" s="315"/>
+      <c r="G4" s="315"/>
+      <c r="H4" s="316"/>
+      <c r="I4" s="378">
         <v>43118</v>
       </c>
-      <c r="J4" s="306"/>
-      <c r="K4" s="306"/>
-      <c r="L4" s="306"/>
-      <c r="M4" s="306"/>
-      <c r="N4" s="306"/>
-      <c r="O4" s="306"/>
-      <c r="P4" s="306"/>
-      <c r="Q4" s="306"/>
-      <c r="R4" s="307"/>
-      <c r="S4" s="296">
+      <c r="J4" s="379"/>
+      <c r="K4" s="379"/>
+      <c r="L4" s="379"/>
+      <c r="M4" s="379"/>
+      <c r="N4" s="379"/>
+      <c r="O4" s="379"/>
+      <c r="P4" s="379"/>
+      <c r="Q4" s="379"/>
+      <c r="R4" s="380"/>
+      <c r="S4" s="317">
         <v>43125</v>
       </c>
-      <c r="T4" s="297"/>
-      <c r="U4" s="297"/>
-      <c r="V4" s="297"/>
-      <c r="W4" s="297"/>
-      <c r="X4" s="297"/>
-      <c r="Y4" s="297"/>
-      <c r="Z4" s="297"/>
-      <c r="AA4" s="297"/>
-      <c r="AB4" s="298"/>
-      <c r="AC4" s="299">
+      <c r="T4" s="318"/>
+      <c r="U4" s="318"/>
+      <c r="V4" s="318"/>
+      <c r="W4" s="318"/>
+      <c r="X4" s="318"/>
+      <c r="Y4" s="318"/>
+      <c r="Z4" s="318"/>
+      <c r="AA4" s="318"/>
+      <c r="AB4" s="319"/>
+      <c r="AC4" s="284">
         <v>43144</v>
       </c>
-      <c r="AD4" s="300"/>
-      <c r="AE4" s="300"/>
-      <c r="AF4" s="300"/>
-      <c r="AG4" s="300"/>
-      <c r="AH4" s="300"/>
-      <c r="AI4" s="300"/>
-      <c r="AJ4" s="300"/>
-      <c r="AK4" s="300"/>
-      <c r="AL4" s="300"/>
-      <c r="AM4" s="300"/>
-      <c r="AN4" s="300"/>
-      <c r="AO4" s="300"/>
-      <c r="AP4" s="300"/>
-      <c r="AQ4" s="300"/>
-      <c r="AR4" s="300"/>
-      <c r="AS4" s="300"/>
-      <c r="AT4" s="300"/>
-      <c r="AU4" s="300"/>
-      <c r="AV4" s="301"/>
-      <c r="AW4" s="302">
+      <c r="AD4" s="285"/>
+      <c r="AE4" s="285"/>
+      <c r="AF4" s="285"/>
+      <c r="AG4" s="285"/>
+      <c r="AH4" s="285"/>
+      <c r="AI4" s="285"/>
+      <c r="AJ4" s="285"/>
+      <c r="AK4" s="285"/>
+      <c r="AL4" s="285"/>
+      <c r="AM4" s="285"/>
+      <c r="AN4" s="285"/>
+      <c r="AO4" s="285"/>
+      <c r="AP4" s="285"/>
+      <c r="AQ4" s="285"/>
+      <c r="AR4" s="285"/>
+      <c r="AS4" s="285"/>
+      <c r="AT4" s="285"/>
+      <c r="AU4" s="285"/>
+      <c r="AV4" s="286"/>
+      <c r="AW4" s="372">
         <v>43154</v>
       </c>
-      <c r="AX4" s="303"/>
-      <c r="AY4" s="303"/>
-      <c r="AZ4" s="303"/>
-      <c r="BA4" s="303"/>
-      <c r="BB4" s="303"/>
-      <c r="BC4" s="303"/>
-      <c r="BD4" s="303"/>
-      <c r="BE4" s="303"/>
-      <c r="BF4" s="304"/>
-      <c r="BG4" s="302">
+      <c r="AX4" s="373"/>
+      <c r="AY4" s="373"/>
+      <c r="AZ4" s="373"/>
+      <c r="BA4" s="373"/>
+      <c r="BB4" s="373"/>
+      <c r="BC4" s="373"/>
+      <c r="BD4" s="373"/>
+      <c r="BE4" s="373"/>
+      <c r="BF4" s="374"/>
+      <c r="BG4" s="307">
         <v>43162</v>
       </c>
-      <c r="BH4" s="303"/>
-      <c r="BI4" s="303"/>
-      <c r="BJ4" s="303"/>
-      <c r="BK4" s="303"/>
-      <c r="BL4" s="303"/>
-      <c r="BM4" s="303"/>
-      <c r="BN4" s="303"/>
-      <c r="BO4" s="303"/>
-      <c r="BP4" s="304"/>
-      <c r="BQ4" s="302">
+      <c r="BH4" s="308"/>
+      <c r="BI4" s="308"/>
+      <c r="BJ4" s="308"/>
+      <c r="BK4" s="308"/>
+      <c r="BL4" s="308"/>
+      <c r="BM4" s="308"/>
+      <c r="BN4" s="308"/>
+      <c r="BO4" s="308"/>
+      <c r="BP4" s="309"/>
+      <c r="BQ4" s="320">
         <v>43172</v>
       </c>
-      <c r="BR4" s="303"/>
-      <c r="BS4" s="303"/>
-      <c r="BT4" s="303"/>
-      <c r="BU4" s="303"/>
-      <c r="BV4" s="303"/>
-      <c r="BW4" s="303"/>
-      <c r="BX4" s="303"/>
-      <c r="BY4" s="303"/>
-      <c r="BZ4" s="304"/>
-      <c r="CA4" s="302">
+      <c r="BR4" s="321"/>
+      <c r="BS4" s="321"/>
+      <c r="BT4" s="321"/>
+      <c r="BU4" s="321"/>
+      <c r="BV4" s="321"/>
+      <c r="BW4" s="321"/>
+      <c r="BX4" s="321"/>
+      <c r="BY4" s="321"/>
+      <c r="BZ4" s="322"/>
+      <c r="CA4" s="378">
         <v>43179</v>
       </c>
-      <c r="CB4" s="303"/>
-      <c r="CC4" s="303"/>
-      <c r="CD4" s="303"/>
-      <c r="CE4" s="303"/>
-      <c r="CF4" s="303"/>
-      <c r="CG4" s="303"/>
-      <c r="CH4" s="303"/>
-      <c r="CI4" s="303"/>
-      <c r="CJ4" s="304"/>
-      <c r="CK4" s="299">
+      <c r="CB4" s="379"/>
+      <c r="CC4" s="379"/>
+      <c r="CD4" s="379"/>
+      <c r="CE4" s="379"/>
+      <c r="CF4" s="379"/>
+      <c r="CG4" s="379"/>
+      <c r="CH4" s="379"/>
+      <c r="CI4" s="379"/>
+      <c r="CJ4" s="380"/>
+      <c r="CK4" s="314">
         <v>43181</v>
       </c>
-      <c r="CL4" s="300"/>
-      <c r="CM4" s="300"/>
-      <c r="CN4" s="300"/>
-      <c r="CO4" s="300"/>
-      <c r="CP4" s="300"/>
-      <c r="CQ4" s="300"/>
-      <c r="CR4" s="300"/>
-      <c r="CS4" s="300"/>
-      <c r="CT4" s="300"/>
-      <c r="CU4" s="300"/>
-      <c r="CV4" s="300"/>
-      <c r="CW4" s="300"/>
-      <c r="CX4" s="300"/>
-      <c r="CY4" s="301"/>
+      <c r="CL4" s="315"/>
+      <c r="CM4" s="315"/>
+      <c r="CN4" s="315"/>
+      <c r="CO4" s="315"/>
+      <c r="CP4" s="315"/>
+      <c r="CQ4" s="315"/>
+      <c r="CR4" s="315"/>
+      <c r="CS4" s="315"/>
+      <c r="CT4" s="315"/>
+      <c r="CU4" s="315"/>
+      <c r="CV4" s="315"/>
+      <c r="CW4" s="315"/>
+      <c r="CX4" s="315"/>
+      <c r="CY4" s="316"/>
       <c r="CZ4" s="245"/>
       <c r="DA4" s="246"/>
     </row>
     <row r="5" spans="2:113" s="127" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="312" t="s">
+      <c r="B5" s="297" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="313"/>
-      <c r="D5" s="314" t="s">
+      <c r="C5" s="298"/>
+      <c r="D5" s="299" t="s">
         <v>333</v>
       </c>
-      <c r="E5" s="315"/>
-      <c r="F5" s="315"/>
-      <c r="G5" s="315"/>
-      <c r="H5" s="316"/>
-      <c r="I5" s="326" t="s">
+      <c r="E5" s="300"/>
+      <c r="F5" s="300"/>
+      <c r="G5" s="300"/>
+      <c r="H5" s="301"/>
+      <c r="I5" s="381" t="s">
         <v>373</v>
       </c>
-      <c r="J5" s="327"/>
-      <c r="K5" s="327"/>
-      <c r="L5" s="327"/>
-      <c r="M5" s="327"/>
-      <c r="N5" s="327"/>
-      <c r="O5" s="327"/>
-      <c r="P5" s="327"/>
-      <c r="Q5" s="327"/>
-      <c r="R5" s="328"/>
-      <c r="S5" s="317" t="s">
+      <c r="J5" s="382"/>
+      <c r="K5" s="382"/>
+      <c r="L5" s="382"/>
+      <c r="M5" s="382"/>
+      <c r="N5" s="382"/>
+      <c r="O5" s="382"/>
+      <c r="P5" s="382"/>
+      <c r="Q5" s="382"/>
+      <c r="R5" s="383"/>
+      <c r="S5" s="302" t="s">
         <v>374</v>
       </c>
-      <c r="T5" s="318"/>
-      <c r="U5" s="318"/>
-      <c r="V5" s="318"/>
-      <c r="W5" s="318"/>
-      <c r="X5" s="318"/>
-      <c r="Y5" s="318"/>
-      <c r="Z5" s="318"/>
-      <c r="AA5" s="318"/>
-      <c r="AB5" s="319"/>
-      <c r="AC5" s="332" t="s">
+      <c r="T5" s="303"/>
+      <c r="U5" s="303"/>
+      <c r="V5" s="303"/>
+      <c r="W5" s="303"/>
+      <c r="X5" s="303"/>
+      <c r="Y5" s="303"/>
+      <c r="Z5" s="303"/>
+      <c r="AA5" s="303"/>
+      <c r="AB5" s="304"/>
+      <c r="AC5" s="290" t="s">
         <v>49</v>
       </c>
-      <c r="AD5" s="333"/>
-      <c r="AE5" s="333"/>
-      <c r="AF5" s="333"/>
-      <c r="AG5" s="333"/>
-      <c r="AH5" s="333"/>
-      <c r="AI5" s="333"/>
-      <c r="AJ5" s="333"/>
-      <c r="AK5" s="333"/>
-      <c r="AL5" s="333"/>
-      <c r="AM5" s="333"/>
-      <c r="AN5" s="333"/>
-      <c r="AO5" s="333"/>
-      <c r="AP5" s="333"/>
-      <c r="AQ5" s="333"/>
-      <c r="AR5" s="333"/>
-      <c r="AS5" s="333"/>
-      <c r="AT5" s="333"/>
-      <c r="AU5" s="333"/>
-      <c r="AV5" s="334"/>
-      <c r="AW5" s="308" t="s">
+      <c r="AD5" s="291"/>
+      <c r="AE5" s="291"/>
+      <c r="AF5" s="291"/>
+      <c r="AG5" s="291"/>
+      <c r="AH5" s="291"/>
+      <c r="AI5" s="291"/>
+      <c r="AJ5" s="291"/>
+      <c r="AK5" s="291"/>
+      <c r="AL5" s="291"/>
+      <c r="AM5" s="291"/>
+      <c r="AN5" s="291"/>
+      <c r="AO5" s="291"/>
+      <c r="AP5" s="291"/>
+      <c r="AQ5" s="291"/>
+      <c r="AR5" s="291"/>
+      <c r="AS5" s="291"/>
+      <c r="AT5" s="291"/>
+      <c r="AU5" s="291"/>
+      <c r="AV5" s="292"/>
+      <c r="AW5" s="387" t="s">
         <v>53</v>
       </c>
-      <c r="AX5" s="309"/>
-      <c r="AY5" s="309"/>
-      <c r="AZ5" s="309"/>
-      <c r="BA5" s="309"/>
-      <c r="BB5" s="309"/>
-      <c r="BC5" s="309"/>
-      <c r="BD5" s="309"/>
-      <c r="BE5" s="309"/>
-      <c r="BF5" s="310"/>
-      <c r="BG5" s="308" t="s">
+      <c r="AX5" s="388"/>
+      <c r="AY5" s="388"/>
+      <c r="AZ5" s="388"/>
+      <c r="BA5" s="388"/>
+      <c r="BB5" s="388"/>
+      <c r="BC5" s="388"/>
+      <c r="BD5" s="388"/>
+      <c r="BE5" s="388"/>
+      <c r="BF5" s="389"/>
+      <c r="BG5" s="294" t="s">
         <v>375</v>
       </c>
-      <c r="BH5" s="309"/>
-      <c r="BI5" s="309"/>
-      <c r="BJ5" s="309"/>
-      <c r="BK5" s="309"/>
-      <c r="BL5" s="309"/>
-      <c r="BM5" s="309"/>
-      <c r="BN5" s="309"/>
-      <c r="BO5" s="309"/>
-      <c r="BP5" s="310"/>
-      <c r="BQ5" s="308" t="s">
+      <c r="BH5" s="295"/>
+      <c r="BI5" s="295"/>
+      <c r="BJ5" s="295"/>
+      <c r="BK5" s="295"/>
+      <c r="BL5" s="295"/>
+      <c r="BM5" s="295"/>
+      <c r="BN5" s="295"/>
+      <c r="BO5" s="295"/>
+      <c r="BP5" s="296"/>
+      <c r="BQ5" s="391" t="s">
         <v>376</v>
       </c>
-      <c r="BR5" s="309"/>
-      <c r="BS5" s="309"/>
-      <c r="BT5" s="309"/>
-      <c r="BU5" s="309"/>
-      <c r="BV5" s="309"/>
-      <c r="BW5" s="309"/>
-      <c r="BX5" s="309"/>
-      <c r="BY5" s="309"/>
-      <c r="BZ5" s="310"/>
-      <c r="CA5" s="308" t="s">
+      <c r="BR5" s="392"/>
+      <c r="BS5" s="392"/>
+      <c r="BT5" s="392"/>
+      <c r="BU5" s="392"/>
+      <c r="BV5" s="392"/>
+      <c r="BW5" s="392"/>
+      <c r="BX5" s="392"/>
+      <c r="BY5" s="392"/>
+      <c r="BZ5" s="393"/>
+      <c r="CA5" s="395" t="s">
         <v>377</v>
       </c>
-      <c r="CB5" s="309"/>
-      <c r="CC5" s="309"/>
-      <c r="CD5" s="309"/>
-      <c r="CE5" s="309"/>
-      <c r="CF5" s="309"/>
-      <c r="CG5" s="309"/>
-      <c r="CH5" s="309"/>
-      <c r="CI5" s="309"/>
-      <c r="CJ5" s="310"/>
-      <c r="CK5" s="335" t="s">
+      <c r="CB5" s="396"/>
+      <c r="CC5" s="396"/>
+      <c r="CD5" s="396"/>
+      <c r="CE5" s="396"/>
+      <c r="CF5" s="396"/>
+      <c r="CG5" s="396"/>
+      <c r="CH5" s="396"/>
+      <c r="CI5" s="396"/>
+      <c r="CJ5" s="397"/>
+      <c r="CK5" s="375" t="s">
         <v>72</v>
       </c>
-      <c r="CL5" s="336"/>
-      <c r="CM5" s="336"/>
-      <c r="CN5" s="336"/>
-      <c r="CO5" s="336"/>
-      <c r="CP5" s="336"/>
-      <c r="CQ5" s="336"/>
-      <c r="CR5" s="336"/>
-      <c r="CS5" s="336"/>
-      <c r="CT5" s="336"/>
-      <c r="CU5" s="336"/>
-      <c r="CV5" s="336"/>
-      <c r="CW5" s="336"/>
-      <c r="CX5" s="336"/>
-      <c r="CY5" s="337"/>
+      <c r="CL5" s="376"/>
+      <c r="CM5" s="376"/>
+      <c r="CN5" s="376"/>
+      <c r="CO5" s="376"/>
+      <c r="CP5" s="376"/>
+      <c r="CQ5" s="376"/>
+      <c r="CR5" s="376"/>
+      <c r="CS5" s="376"/>
+      <c r="CT5" s="376"/>
+      <c r="CU5" s="376"/>
+      <c r="CV5" s="376"/>
+      <c r="CW5" s="376"/>
+      <c r="CX5" s="376"/>
+      <c r="CY5" s="377"/>
       <c r="CZ5" s="247"/>
       <c r="DA5" s="248"/>
     </row>
     <row r="6" spans="2:113" s="171" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="243"/>
       <c r="C6" s="244"/>
-      <c r="D6" s="320" t="s">
+      <c r="D6" s="305" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="320"/>
-      <c r="F6" s="320"/>
-      <c r="G6" s="320"/>
-      <c r="H6" s="320"/>
-      <c r="I6" s="321" t="s">
+      <c r="E6" s="305"/>
+      <c r="F6" s="305"/>
+      <c r="G6" s="305"/>
+      <c r="H6" s="305"/>
+      <c r="I6" s="384" t="s">
         <v>86</v>
       </c>
-      <c r="J6" s="322"/>
-      <c r="K6" s="322"/>
-      <c r="L6" s="322"/>
-      <c r="M6" s="323"/>
-      <c r="N6" s="321" t="s">
+      <c r="J6" s="385"/>
+      <c r="K6" s="385"/>
+      <c r="L6" s="385"/>
+      <c r="M6" s="386"/>
+      <c r="N6" s="384" t="s">
         <v>87</v>
       </c>
-      <c r="O6" s="322"/>
-      <c r="P6" s="322"/>
-      <c r="Q6" s="322"/>
-      <c r="R6" s="323"/>
-      <c r="S6" s="324" t="s">
+      <c r="O6" s="385"/>
+      <c r="P6" s="385"/>
+      <c r="Q6" s="385"/>
+      <c r="R6" s="386"/>
+      <c r="S6" s="306" t="s">
         <v>86</v>
       </c>
-      <c r="T6" s="324"/>
-      <c r="U6" s="324"/>
-      <c r="V6" s="324"/>
-      <c r="W6" s="324"/>
-      <c r="X6" s="324" t="s">
+      <c r="T6" s="306"/>
+      <c r="U6" s="306"/>
+      <c r="V6" s="306"/>
+      <c r="W6" s="306"/>
+      <c r="X6" s="306" t="s">
         <v>87</v>
       </c>
-      <c r="Y6" s="324"/>
-      <c r="Z6" s="324"/>
-      <c r="AA6" s="324"/>
-      <c r="AB6" s="324"/>
-      <c r="AC6" s="325" t="s">
+      <c r="Y6" s="306"/>
+      <c r="Z6" s="306"/>
+      <c r="AA6" s="306"/>
+      <c r="AB6" s="306"/>
+      <c r="AC6" s="289" t="s">
         <v>86</v>
       </c>
-      <c r="AD6" s="325"/>
-      <c r="AE6" s="325"/>
-      <c r="AF6" s="325"/>
-      <c r="AG6" s="325"/>
-      <c r="AH6" s="325" t="s">
+      <c r="AD6" s="289"/>
+      <c r="AE6" s="289"/>
+      <c r="AF6" s="289"/>
+      <c r="AG6" s="289"/>
+      <c r="AH6" s="289" t="s">
         <v>87</v>
       </c>
-      <c r="AI6" s="325"/>
-      <c r="AJ6" s="325"/>
-      <c r="AK6" s="325"/>
-      <c r="AL6" s="325"/>
-      <c r="AM6" s="325" t="s">
+      <c r="AI6" s="289"/>
+      <c r="AJ6" s="289"/>
+      <c r="AK6" s="289"/>
+      <c r="AL6" s="289"/>
+      <c r="AM6" s="289" t="s">
         <v>88</v>
       </c>
-      <c r="AN6" s="325"/>
-      <c r="AO6" s="325"/>
-      <c r="AP6" s="325"/>
-      <c r="AQ6" s="325"/>
-      <c r="AR6" s="325" t="s">
+      <c r="AN6" s="289"/>
+      <c r="AO6" s="289"/>
+      <c r="AP6" s="289"/>
+      <c r="AQ6" s="289"/>
+      <c r="AR6" s="289" t="s">
         <v>89</v>
       </c>
-      <c r="AS6" s="325"/>
-      <c r="AT6" s="325"/>
-      <c r="AU6" s="325"/>
-      <c r="AV6" s="325"/>
-      <c r="AW6" s="311" t="s">
+      <c r="AS6" s="289"/>
+      <c r="AT6" s="289"/>
+      <c r="AU6" s="289"/>
+      <c r="AV6" s="289"/>
+      <c r="AW6" s="390" t="s">
         <v>86</v>
       </c>
-      <c r="AX6" s="311"/>
-      <c r="AY6" s="311"/>
-      <c r="AZ6" s="311"/>
-      <c r="BA6" s="311"/>
-      <c r="BB6" s="311" t="s">
+      <c r="AX6" s="390"/>
+      <c r="AY6" s="390"/>
+      <c r="AZ6" s="390"/>
+      <c r="BA6" s="390"/>
+      <c r="BB6" s="390" t="s">
         <v>87</v>
       </c>
-      <c r="BC6" s="311"/>
-      <c r="BD6" s="311"/>
-      <c r="BE6" s="311"/>
-      <c r="BF6" s="311"/>
-      <c r="BG6" s="311" t="s">
+      <c r="BC6" s="390"/>
+      <c r="BD6" s="390"/>
+      <c r="BE6" s="390"/>
+      <c r="BF6" s="390"/>
+      <c r="BG6" s="293" t="s">
         <v>86</v>
       </c>
-      <c r="BH6" s="311"/>
-      <c r="BI6" s="311"/>
-      <c r="BJ6" s="311"/>
-      <c r="BK6" s="311"/>
-      <c r="BL6" s="311" t="s">
+      <c r="BH6" s="293"/>
+      <c r="BI6" s="293"/>
+      <c r="BJ6" s="293"/>
+      <c r="BK6" s="293"/>
+      <c r="BL6" s="293" t="s">
         <v>87</v>
       </c>
-      <c r="BM6" s="311"/>
-      <c r="BN6" s="311"/>
-      <c r="BO6" s="311"/>
-      <c r="BP6" s="311"/>
-      <c r="BQ6" s="311" t="s">
+      <c r="BM6" s="293"/>
+      <c r="BN6" s="293"/>
+      <c r="BO6" s="293"/>
+      <c r="BP6" s="293"/>
+      <c r="BQ6" s="394" t="s">
         <v>86</v>
       </c>
-      <c r="BR6" s="311"/>
-      <c r="BS6" s="311"/>
-      <c r="BT6" s="311"/>
-      <c r="BU6" s="311"/>
-      <c r="BV6" s="311" t="s">
+      <c r="BR6" s="394"/>
+      <c r="BS6" s="394"/>
+      <c r="BT6" s="394"/>
+      <c r="BU6" s="394"/>
+      <c r="BV6" s="394" t="s">
         <v>87</v>
       </c>
-      <c r="BW6" s="311"/>
-      <c r="BX6" s="311"/>
-      <c r="BY6" s="311"/>
-      <c r="BZ6" s="311"/>
-      <c r="CA6" s="311" t="s">
+      <c r="BW6" s="394"/>
+      <c r="BX6" s="394"/>
+      <c r="BY6" s="394"/>
+      <c r="BZ6" s="394"/>
+      <c r="CA6" s="398" t="s">
         <v>86</v>
       </c>
-      <c r="CB6" s="311"/>
-      <c r="CC6" s="311"/>
-      <c r="CD6" s="311"/>
-      <c r="CE6" s="311"/>
-      <c r="CF6" s="311" t="s">
+      <c r="CB6" s="398"/>
+      <c r="CC6" s="398"/>
+      <c r="CD6" s="398"/>
+      <c r="CE6" s="398"/>
+      <c r="CF6" s="398" t="s">
         <v>87</v>
       </c>
-      <c r="CG6" s="311"/>
-      <c r="CH6" s="311"/>
-      <c r="CI6" s="311"/>
-      <c r="CJ6" s="311"/>
-      <c r="CK6" s="329" t="s">
+      <c r="CG6" s="398"/>
+      <c r="CH6" s="398"/>
+      <c r="CI6" s="398"/>
+      <c r="CJ6" s="398"/>
+      <c r="CK6" s="399" t="s">
         <v>86</v>
       </c>
-      <c r="CL6" s="330"/>
-      <c r="CM6" s="330"/>
-      <c r="CN6" s="330"/>
-      <c r="CO6" s="331"/>
-      <c r="CP6" s="329" t="s">
+      <c r="CL6" s="400"/>
+      <c r="CM6" s="400"/>
+      <c r="CN6" s="400"/>
+      <c r="CO6" s="401"/>
+      <c r="CP6" s="399" t="s">
         <v>90</v>
       </c>
-      <c r="CQ6" s="330"/>
-      <c r="CR6" s="330"/>
-      <c r="CS6" s="330"/>
-      <c r="CT6" s="331"/>
-      <c r="CU6" s="329" t="s">
+      <c r="CQ6" s="400"/>
+      <c r="CR6" s="400"/>
+      <c r="CS6" s="400"/>
+      <c r="CT6" s="401"/>
+      <c r="CU6" s="399" t="s">
         <v>87</v>
       </c>
-      <c r="CV6" s="330"/>
-      <c r="CW6" s="330"/>
-      <c r="CX6" s="330"/>
-      <c r="CY6" s="331"/>
+      <c r="CV6" s="400"/>
+      <c r="CW6" s="400"/>
+      <c r="CX6" s="400"/>
+      <c r="CY6" s="401"/>
       <c r="CZ6" s="249" t="s">
         <v>85</v>
       </c>
@@ -11413,10 +11473,10 @@
     </row>
     <row r="7" spans="2:113" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="192" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="C7" s="179" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="D7" s="181"/>
       <c r="E7" s="180"/>
@@ -11463,16 +11523,12 @@
       <c r="AT7" s="180"/>
       <c r="AU7" s="180"/>
       <c r="AV7" s="182"/>
-      <c r="AW7" s="180">
-        <v>100</v>
-      </c>
+      <c r="AW7" s="180"/>
       <c r="AX7" s="180"/>
       <c r="AY7" s="180"/>
       <c r="AZ7" s="180"/>
       <c r="BA7" s="180"/>
-      <c r="BB7" s="181">
-        <v>100</v>
-      </c>
+      <c r="BB7" s="181"/>
       <c r="BC7" s="180"/>
       <c r="BD7" s="180"/>
       <c r="BE7" s="180"/>
@@ -11538,12 +11594,8 @@
       <c r="DI7" s="128"/>
     </row>
     <row r="8" spans="2:113" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="193" t="s">
-        <v>387</v>
-      </c>
-      <c r="C8" s="173" t="s">
-        <v>388</v>
-      </c>
+      <c r="B8" s="193"/>
+      <c r="C8" s="173"/>
       <c r="D8" s="184"/>
       <c r="E8" s="183"/>
       <c r="F8" s="183"/>
@@ -11629,9 +11681,7 @@
       <c r="CH8" s="183"/>
       <c r="CI8" s="183"/>
       <c r="CJ8" s="185"/>
-      <c r="CK8" s="184">
-        <v>77</v>
-      </c>
+      <c r="CK8" s="184"/>
       <c r="CL8" s="183"/>
       <c r="CM8" s="183"/>
       <c r="CN8" s="183"/>
@@ -11666,15 +11716,9 @@
       <c r="DI8" s="128"/>
     </row>
     <row r="9" spans="2:113" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="193" t="s">
-        <v>383</v>
-      </c>
-      <c r="C9" s="173" t="s">
-        <v>384</v>
-      </c>
-      <c r="D9" s="184">
-        <v>55</v>
-      </c>
+      <c r="B9" s="193"/>
+      <c r="C9" s="173"/>
+      <c r="D9" s="184"/>
       <c r="E9" s="183"/>
       <c r="F9" s="183"/>
       <c r="G9" s="183"/>
@@ -11729,16 +11773,12 @@
       <c r="BD9" s="183"/>
       <c r="BE9" s="183"/>
       <c r="BF9" s="185"/>
-      <c r="BG9" s="184">
-        <v>77</v>
-      </c>
+      <c r="BG9" s="184"/>
       <c r="BH9" s="183"/>
       <c r="BI9" s="183"/>
       <c r="BJ9" s="183"/>
       <c r="BK9" s="185"/>
-      <c r="BL9" s="184">
-        <v>77</v>
-      </c>
+      <c r="BL9" s="184"/>
       <c r="BM9" s="183"/>
       <c r="BN9" s="183"/>
       <c r="BO9" s="183"/>
@@ -11794,18 +11834,10 @@
       <c r="DI9" s="128"/>
     </row>
     <row r="10" spans="2:113" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="193" t="s">
-        <v>381</v>
-      </c>
-      <c r="C10" s="173" t="s">
-        <v>382</v>
-      </c>
-      <c r="D10" s="184">
-        <v>44</v>
-      </c>
-      <c r="E10" s="183">
-        <v>33</v>
-      </c>
+      <c r="B10" s="193"/>
+      <c r="C10" s="173"/>
+      <c r="D10" s="184"/>
+      <c r="E10" s="183"/>
       <c r="F10" s="183"/>
       <c r="G10" s="183"/>
       <c r="H10" s="185"/>
@@ -11849,16 +11881,12 @@
       <c r="AT10" s="183"/>
       <c r="AU10" s="183"/>
       <c r="AV10" s="185"/>
-      <c r="AW10" s="183">
-        <v>33</v>
-      </c>
+      <c r="AW10" s="183"/>
       <c r="AX10" s="183"/>
       <c r="AY10" s="183"/>
       <c r="AZ10" s="183"/>
       <c r="BA10" s="183"/>
-      <c r="BB10" s="184">
-        <v>44</v>
-      </c>
+      <c r="BB10" s="184"/>
       <c r="BC10" s="183"/>
       <c r="BD10" s="183"/>
       <c r="BE10" s="183"/>
@@ -11883,16 +11911,12 @@
       <c r="BX10" s="183"/>
       <c r="BY10" s="183"/>
       <c r="BZ10" s="185"/>
-      <c r="CA10" s="184">
-        <v>23</v>
-      </c>
+      <c r="CA10" s="184"/>
       <c r="CB10" s="183"/>
       <c r="CC10" s="183"/>
       <c r="CD10" s="183"/>
       <c r="CE10" s="185"/>
-      <c r="CF10" s="184">
-        <v>22</v>
-      </c>
+      <c r="CF10" s="184"/>
       <c r="CG10" s="183"/>
       <c r="CH10" s="183"/>
       <c r="CI10" s="183"/>
@@ -11928,12 +11952,8 @@
       <c r="DI10" s="128"/>
     </row>
     <row r="11" spans="2:113" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="193" t="s">
-        <v>385</v>
-      </c>
-      <c r="C11" s="173" t="s">
-        <v>386</v>
-      </c>
+      <c r="B11" s="193"/>
+      <c r="C11" s="173"/>
       <c r="D11" s="184"/>
       <c r="E11" s="183"/>
       <c r="F11" s="183"/>
@@ -15171,25 +15191,41 @@
       <c r="EJ53" s="128"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <sortState ref="B7:DA35">
     <sortCondition descending="1" ref="CZ13"/>
   </sortState>
   <dataConsolidate/>
   <mergeCells count="52">
-    <mergeCell ref="CK4:CY4"/>
-    <mergeCell ref="CK5:CY5"/>
-    <mergeCell ref="CK3:CY3"/>
-    <mergeCell ref="CK6:CO6"/>
-    <mergeCell ref="CP6:CT6"/>
-    <mergeCell ref="CU6:CY6"/>
-    <mergeCell ref="AH6:AL6"/>
-    <mergeCell ref="AC5:AV5"/>
-    <mergeCell ref="BQ6:BU6"/>
-    <mergeCell ref="AM6:AQ6"/>
-    <mergeCell ref="AR6:AV6"/>
-    <mergeCell ref="AW6:BA6"/>
-    <mergeCell ref="BB6:BF6"/>
+    <mergeCell ref="AX2:CC2"/>
+    <mergeCell ref="AC2:AW2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="S3:AB3"/>
+    <mergeCell ref="AC3:AV3"/>
+    <mergeCell ref="AW3:BF3"/>
+    <mergeCell ref="CA3:CJ3"/>
+    <mergeCell ref="I3:R3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="S4:AB4"/>
+    <mergeCell ref="AC4:AV4"/>
+    <mergeCell ref="AW4:BF4"/>
+    <mergeCell ref="I4:R4"/>
+    <mergeCell ref="CA4:CJ4"/>
+    <mergeCell ref="BG4:BP4"/>
+    <mergeCell ref="BG3:BP3"/>
+    <mergeCell ref="BQ4:BZ4"/>
+    <mergeCell ref="BQ3:BZ3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="S5:AB5"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="S6:W6"/>
+    <mergeCell ref="X6:AB6"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="I5:R5"/>
     <mergeCell ref="CA6:CE6"/>
     <mergeCell ref="BL6:BP6"/>
     <mergeCell ref="AW5:BF5"/>
@@ -15199,36 +15235,20 @@
     <mergeCell ref="BG6:BK6"/>
     <mergeCell ref="BQ5:BZ5"/>
     <mergeCell ref="BV6:BZ6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="S5:AB5"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="N6:R6"/>
-    <mergeCell ref="S6:W6"/>
-    <mergeCell ref="X6:AB6"/>
+    <mergeCell ref="AH6:AL6"/>
+    <mergeCell ref="AC5:AV5"/>
+    <mergeCell ref="BQ6:BU6"/>
+    <mergeCell ref="AM6:AQ6"/>
+    <mergeCell ref="AR6:AV6"/>
+    <mergeCell ref="AW6:BA6"/>
+    <mergeCell ref="BB6:BF6"/>
     <mergeCell ref="AC6:AG6"/>
-    <mergeCell ref="I6:M6"/>
-    <mergeCell ref="I5:R5"/>
-    <mergeCell ref="CA4:CJ4"/>
-    <mergeCell ref="BG4:BP4"/>
-    <mergeCell ref="BG3:BP3"/>
-    <mergeCell ref="BQ4:BZ4"/>
-    <mergeCell ref="BQ3:BZ3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="S4:AB4"/>
-    <mergeCell ref="AC4:AV4"/>
-    <mergeCell ref="AW4:BF4"/>
-    <mergeCell ref="I4:R4"/>
-    <mergeCell ref="AX2:CC2"/>
-    <mergeCell ref="AC2:AW2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="S3:AB3"/>
-    <mergeCell ref="AC3:AV3"/>
-    <mergeCell ref="AW3:BF3"/>
-    <mergeCell ref="CA3:CJ3"/>
-    <mergeCell ref="I3:R3"/>
+    <mergeCell ref="CK4:CY4"/>
+    <mergeCell ref="CK5:CY5"/>
+    <mergeCell ref="CK3:CY3"/>
+    <mergeCell ref="CK6:CO6"/>
+    <mergeCell ref="CP6:CT6"/>
+    <mergeCell ref="CU6:CY6"/>
   </mergeCells>
   <conditionalFormatting sqref="CZ35">
     <cfRule type="top10" dxfId="45" priority="58" percent="1" bottom="1" rank="10"/>
@@ -15372,8 +15392,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="3075" r:id="rId4" name="BtnEditAssess">
+        <control shapeId="3073" r:id="rId4" name="BtnAddAssess">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3073" r:id="rId4" name="BtnAddAssess"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3075" r:id="rId6" name="BtnEditAssess">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>2</xdr:col>
@@ -15392,32 +15437,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="3075" r:id="rId4" name="BtnEditAssess"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="3073" r:id="rId6" name="BtnAddAssess">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>457200</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="3073" r:id="rId6" name="BtnAddAssess"/>
+        <control shapeId="3075" r:id="rId6" name="BtnEditAssess"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -16679,14 +16699,14 @@
       </c>
     </row>
     <row r="3" spans="1:11" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="339" t="s">
+      <c r="A3" s="330" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="340"/>
-      <c r="C3" s="340"/>
-      <c r="D3" s="340"/>
-      <c r="E3" s="340"/>
-      <c r="F3" s="341"/>
+      <c r="B3" s="331"/>
+      <c r="C3" s="331"/>
+      <c r="D3" s="331"/>
+      <c r="E3" s="331"/>
+      <c r="F3" s="332"/>
       <c r="H3" s="74"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -16731,14 +16751,14 @@
     </row>
     <row r="6" spans="1:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:11" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="339" t="s">
+      <c r="A7" s="330" t="s">
         <v>165</v>
       </c>
-      <c r="B7" s="340"/>
-      <c r="C7" s="340"/>
-      <c r="D7" s="340"/>
-      <c r="E7" s="340"/>
-      <c r="F7" s="341"/>
+      <c r="B7" s="331"/>
+      <c r="C7" s="331"/>
+      <c r="D7" s="331"/>
+      <c r="E7" s="331"/>
+      <c r="F7" s="332"/>
       <c r="H7" s="74"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -16751,11 +16771,11 @@
       <c r="C8" s="57" t="s">
         <v>167</v>
       </c>
-      <c r="D8" s="342" t="s">
+      <c r="D8" s="333" t="s">
         <v>330</v>
       </c>
-      <c r="E8" s="343"/>
-      <c r="F8" s="344"/>
+      <c r="E8" s="334"/>
+      <c r="F8" s="335"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="55" t="s">
@@ -16779,27 +16799,27 @@
     </row>
     <row r="10" spans="1:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:11" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="339" t="s">
+      <c r="A11" s="330" t="s">
         <v>116</v>
       </c>
-      <c r="B11" s="340"/>
-      <c r="C11" s="340"/>
-      <c r="D11" s="340"/>
-      <c r="E11" s="340"/>
-      <c r="F11" s="341"/>
+      <c r="B11" s="331"/>
+      <c r="C11" s="331"/>
+      <c r="D11" s="331"/>
+      <c r="E11" s="331"/>
+      <c r="F11" s="332"/>
       <c r="H11" s="74"/>
     </row>
     <row r="12" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="B12" s="345" t="s">
+      <c r="B12" s="336" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="346"/>
-      <c r="D12" s="346"/>
-      <c r="E12" s="346"/>
-      <c r="F12" s="347"/>
+      <c r="C12" s="337"/>
+      <c r="D12" s="337"/>
+      <c r="E12" s="337"/>
+      <c r="F12" s="338"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="64"/>
@@ -16815,25 +16835,25 @@
     </row>
     <row r="14" spans="1:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:11" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="339" t="s">
+      <c r="A15" s="330" t="s">
         <v>114</v>
       </c>
-      <c r="B15" s="340"/>
-      <c r="C15" s="340"/>
-      <c r="D15" s="340"/>
-      <c r="E15" s="340"/>
-      <c r="F15" s="341"/>
+      <c r="B15" s="331"/>
+      <c r="C15" s="331"/>
+      <c r="D15" s="331"/>
+      <c r="E15" s="331"/>
+      <c r="F15" s="332"/>
       <c r="H15" s="74"/>
     </row>
     <row r="16" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="B16" s="348"/>
-      <c r="C16" s="349"/>
-      <c r="D16" s="349"/>
-      <c r="E16" s="349"/>
-      <c r="F16" s="350"/>
+      <c r="B16" s="327"/>
+      <c r="C16" s="328"/>
+      <c r="D16" s="328"/>
+      <c r="E16" s="328"/>
+      <c r="F16" s="329"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="64"/>
@@ -16849,25 +16869,25 @@
     </row>
     <row r="18" spans="1:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:8" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="339" t="s">
+      <c r="A19" s="330" t="s">
         <v>115</v>
       </c>
-      <c r="B19" s="340"/>
-      <c r="C19" s="340"/>
-      <c r="D19" s="340"/>
-      <c r="E19" s="340"/>
-      <c r="F19" s="341"/>
+      <c r="B19" s="331"/>
+      <c r="C19" s="331"/>
+      <c r="D19" s="331"/>
+      <c r="E19" s="331"/>
+      <c r="F19" s="332"/>
       <c r="H19" s="74"/>
     </row>
     <row r="20" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="B20" s="348"/>
-      <c r="C20" s="349"/>
-      <c r="D20" s="349"/>
-      <c r="E20" s="349"/>
-      <c r="F20" s="350"/>
+      <c r="B20" s="327"/>
+      <c r="C20" s="328"/>
+      <c r="D20" s="328"/>
+      <c r="E20" s="328"/>
+      <c r="F20" s="329"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="64"/>
@@ -16883,25 +16903,25 @@
     </row>
     <row r="22" spans="1:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:8" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="339" t="s">
+      <c r="A23" s="330" t="s">
         <v>171</v>
       </c>
-      <c r="B23" s="340"/>
-      <c r="C23" s="340"/>
-      <c r="D23" s="340"/>
-      <c r="E23" s="340"/>
-      <c r="F23" s="341"/>
+      <c r="B23" s="331"/>
+      <c r="C23" s="331"/>
+      <c r="D23" s="331"/>
+      <c r="E23" s="331"/>
+      <c r="F23" s="332"/>
       <c r="H23" s="74"/>
     </row>
     <row r="24" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="B24" s="348"/>
-      <c r="C24" s="349"/>
-      <c r="D24" s="349"/>
-      <c r="E24" s="349"/>
-      <c r="F24" s="350"/>
+      <c r="B24" s="327"/>
+      <c r="C24" s="328"/>
+      <c r="D24" s="328"/>
+      <c r="E24" s="328"/>
+      <c r="F24" s="329"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="64"/>
@@ -16917,27 +16937,27 @@
     </row>
     <row r="26" spans="1:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:8" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="339" t="s">
+      <c r="A27" s="330" t="s">
         <v>172</v>
       </c>
-      <c r="B27" s="340"/>
-      <c r="C27" s="340"/>
-      <c r="D27" s="340"/>
-      <c r="E27" s="340"/>
-      <c r="F27" s="341"/>
+      <c r="B27" s="331"/>
+      <c r="C27" s="331"/>
+      <c r="D27" s="331"/>
+      <c r="E27" s="331"/>
+      <c r="F27" s="332"/>
       <c r="H27" s="74"/>
     </row>
     <row r="28" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="B28" s="348" t="s">
+      <c r="B28" s="327" t="s">
         <v>331</v>
       </c>
-      <c r="C28" s="349"/>
-      <c r="D28" s="349"/>
-      <c r="E28" s="349"/>
-      <c r="F28" s="350"/>
+      <c r="C28" s="328"/>
+      <c r="D28" s="328"/>
+      <c r="E28" s="328"/>
+      <c r="F28" s="329"/>
       <c r="H28" s="74" t="s">
         <v>331</v>
       </c>
@@ -16953,6 +16973,12 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="13">
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="B12:F12"/>
     <mergeCell ref="B28:F28"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="A19:F19"/>
@@ -16960,12 +16986,6 @@
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="B12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -17009,10 +17029,10 @@
       <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C3" s="354" t="s">
+      <c r="C3" s="342" t="s">
         <v>232</v>
       </c>
-      <c r="D3" s="354"/>
+      <c r="D3" s="342"/>
     </row>
     <row r="4" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:6" s="40" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -17074,35 +17094,35 @@
     </row>
     <row r="10" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:6" s="17" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="355" t="s">
+      <c r="A11" s="343" t="s">
         <v>128</v>
       </c>
-      <c r="B11" s="357"/>
-      <c r="C11" s="358"/>
+      <c r="B11" s="345"/>
+      <c r="C11" s="346"/>
       <c r="D11" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="E11" s="361"/>
-      <c r="F11" s="362"/>
+      <c r="E11" s="349"/>
+      <c r="F11" s="350"/>
     </row>
     <row r="12" spans="1:6" s="17" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="356"/>
-      <c r="B12" s="359"/>
-      <c r="C12" s="360"/>
+      <c r="A12" s="344"/>
+      <c r="B12" s="347"/>
+      <c r="C12" s="348"/>
       <c r="D12" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="E12" s="361"/>
-      <c r="F12" s="362"/>
+      <c r="E12" s="349"/>
+      <c r="F12" s="350"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:6" s="22" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="351" t="s">
+      <c r="B14" s="339" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="352"/>
-      <c r="D14" s="352"/>
-      <c r="E14" s="353"/>
+      <c r="C14" s="340"/>
+      <c r="D14" s="340"/>
+      <c r="E14" s="341"/>
       <c r="F14"/>
     </row>
     <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17168,30 +17188,30 @@
         <v>184</v>
       </c>
       <c r="C3" s="100"/>
-      <c r="E3" s="375">
+      <c r="E3" s="352">
         <v>5665</v>
       </c>
-      <c r="F3" s="375"/>
+      <c r="F3" s="352"/>
       <c r="G3" s="96" t="s">
         <v>124</v>
       </c>
-      <c r="I3" s="375" t="s">
+      <c r="I3" s="352" t="s">
         <v>329</v>
       </c>
-      <c r="J3" s="375"/>
-      <c r="K3" s="375"/>
-      <c r="L3" s="375"/>
-      <c r="M3" s="375"/>
+      <c r="J3" s="352"/>
+      <c r="K3" s="352"/>
+      <c r="L3" s="352"/>
+      <c r="M3" s="352"/>
       <c r="N3" s="96" t="s">
         <v>162</v>
       </c>
-      <c r="P3" s="375" t="s">
+      <c r="P3" s="352" t="s">
         <v>252</v>
       </c>
-      <c r="Q3" s="375"/>
-      <c r="R3" s="375"/>
-      <c r="S3" s="375"/>
-      <c r="T3" s="375"/>
+      <c r="Q3" s="352"/>
+      <c r="R3" s="352"/>
+      <c r="S3" s="352"/>
+      <c r="T3" s="352"/>
       <c r="V3" s="96" t="s">
         <v>163</v>
       </c>
@@ -17202,10 +17222,10 @@
         <v>63</v>
       </c>
       <c r="AD3" s="99"/>
-      <c r="AF3" s="374" t="s">
+      <c r="AF3" s="351" t="s">
         <v>328</v>
       </c>
-      <c r="AG3" s="374"/>
+      <c r="AG3" s="351"/>
     </row>
     <row r="5" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="76" t="s">
@@ -17798,153 +17818,148 @@
     </row>
     <row r="17" spans="2:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="366" t="s">
+      <c r="B18" s="356" t="s">
         <v>207</v>
       </c>
-      <c r="C18" s="367"/>
-      <c r="D18" s="363" t="s">
+      <c r="C18" s="357"/>
+      <c r="D18" s="353" t="s">
         <v>202</v>
       </c>
-      <c r="E18" s="364"/>
-      <c r="F18" s="364"/>
-      <c r="G18" s="364"/>
-      <c r="H18" s="364"/>
-      <c r="I18" s="364"/>
-      <c r="J18" s="364"/>
-      <c r="K18" s="364"/>
-      <c r="L18" s="364"/>
-      <c r="M18" s="364"/>
-      <c r="N18" s="364"/>
-      <c r="O18" s="364"/>
-      <c r="P18" s="364"/>
-      <c r="Q18" s="364"/>
-      <c r="R18" s="364"/>
-      <c r="S18" s="364"/>
-      <c r="T18" s="364"/>
-      <c r="U18" s="364"/>
-      <c r="V18" s="364"/>
-      <c r="W18" s="365"/>
+      <c r="E18" s="354"/>
+      <c r="F18" s="354"/>
+      <c r="G18" s="354"/>
+      <c r="H18" s="354"/>
+      <c r="I18" s="354"/>
+      <c r="J18" s="354"/>
+      <c r="K18" s="354"/>
+      <c r="L18" s="354"/>
+      <c r="M18" s="354"/>
+      <c r="N18" s="354"/>
+      <c r="O18" s="354"/>
+      <c r="P18" s="354"/>
+      <c r="Q18" s="354"/>
+      <c r="R18" s="354"/>
+      <c r="S18" s="354"/>
+      <c r="T18" s="354"/>
+      <c r="U18" s="354"/>
+      <c r="V18" s="354"/>
+      <c r="W18" s="355"/>
     </row>
     <row r="19" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="368">
+      <c r="B19" s="358">
         <v>2</v>
       </c>
-      <c r="C19" s="369"/>
-      <c r="D19" s="363" t="s">
+      <c r="C19" s="359"/>
+      <c r="D19" s="353" t="s">
         <v>203</v>
       </c>
-      <c r="E19" s="364"/>
-      <c r="F19" s="364"/>
-      <c r="G19" s="364"/>
-      <c r="H19" s="364"/>
-      <c r="I19" s="364"/>
-      <c r="J19" s="364"/>
-      <c r="K19" s="364"/>
-      <c r="L19" s="364"/>
-      <c r="M19" s="364"/>
-      <c r="N19" s="364"/>
-      <c r="O19" s="364"/>
-      <c r="P19" s="364"/>
-      <c r="Q19" s="364"/>
-      <c r="R19" s="364"/>
-      <c r="S19" s="364"/>
-      <c r="T19" s="364"/>
-      <c r="U19" s="364"/>
-      <c r="V19" s="364"/>
-      <c r="W19" s="365"/>
+      <c r="E19" s="354"/>
+      <c r="F19" s="354"/>
+      <c r="G19" s="354"/>
+      <c r="H19" s="354"/>
+      <c r="I19" s="354"/>
+      <c r="J19" s="354"/>
+      <c r="K19" s="354"/>
+      <c r="L19" s="354"/>
+      <c r="M19" s="354"/>
+      <c r="N19" s="354"/>
+      <c r="O19" s="354"/>
+      <c r="P19" s="354"/>
+      <c r="Q19" s="354"/>
+      <c r="R19" s="354"/>
+      <c r="S19" s="354"/>
+      <c r="T19" s="354"/>
+      <c r="U19" s="354"/>
+      <c r="V19" s="354"/>
+      <c r="W19" s="355"/>
     </row>
     <row r="20" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="370">
+      <c r="B20" s="360">
         <v>3</v>
       </c>
-      <c r="C20" s="371"/>
-      <c r="D20" s="363" t="s">
+      <c r="C20" s="361"/>
+      <c r="D20" s="353" t="s">
         <v>204</v>
       </c>
-      <c r="E20" s="364"/>
-      <c r="F20" s="364"/>
-      <c r="G20" s="364"/>
-      <c r="H20" s="364"/>
-      <c r="I20" s="364"/>
-      <c r="J20" s="364"/>
-      <c r="K20" s="364"/>
-      <c r="L20" s="364"/>
-      <c r="M20" s="364"/>
-      <c r="N20" s="364"/>
-      <c r="O20" s="364"/>
-      <c r="P20" s="364"/>
-      <c r="Q20" s="364"/>
-      <c r="R20" s="364"/>
-      <c r="S20" s="364"/>
-      <c r="T20" s="364"/>
-      <c r="U20" s="364"/>
-      <c r="V20" s="364"/>
-      <c r="W20" s="365"/>
+      <c r="E20" s="354"/>
+      <c r="F20" s="354"/>
+      <c r="G20" s="354"/>
+      <c r="H20" s="354"/>
+      <c r="I20" s="354"/>
+      <c r="J20" s="354"/>
+      <c r="K20" s="354"/>
+      <c r="L20" s="354"/>
+      <c r="M20" s="354"/>
+      <c r="N20" s="354"/>
+      <c r="O20" s="354"/>
+      <c r="P20" s="354"/>
+      <c r="Q20" s="354"/>
+      <c r="R20" s="354"/>
+      <c r="S20" s="354"/>
+      <c r="T20" s="354"/>
+      <c r="U20" s="354"/>
+      <c r="V20" s="354"/>
+      <c r="W20" s="355"/>
     </row>
     <row r="21" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="372">
+      <c r="B21" s="362">
         <v>4</v>
       </c>
-      <c r="C21" s="373"/>
-      <c r="D21" s="363" t="s">
+      <c r="C21" s="363"/>
+      <c r="D21" s="353" t="s">
         <v>205</v>
       </c>
-      <c r="E21" s="364"/>
-      <c r="F21" s="364"/>
-      <c r="G21" s="364"/>
-      <c r="H21" s="364"/>
-      <c r="I21" s="364"/>
-      <c r="J21" s="364"/>
-      <c r="K21" s="364"/>
-      <c r="L21" s="364"/>
-      <c r="M21" s="364"/>
-      <c r="N21" s="364"/>
-      <c r="O21" s="364"/>
-      <c r="P21" s="364"/>
-      <c r="Q21" s="364"/>
-      <c r="R21" s="364"/>
-      <c r="S21" s="364"/>
-      <c r="T21" s="364"/>
-      <c r="U21" s="364"/>
-      <c r="V21" s="364"/>
-      <c r="W21" s="365"/>
+      <c r="E21" s="354"/>
+      <c r="F21" s="354"/>
+      <c r="G21" s="354"/>
+      <c r="H21" s="354"/>
+      <c r="I21" s="354"/>
+      <c r="J21" s="354"/>
+      <c r="K21" s="354"/>
+      <c r="L21" s="354"/>
+      <c r="M21" s="354"/>
+      <c r="N21" s="354"/>
+      <c r="O21" s="354"/>
+      <c r="P21" s="354"/>
+      <c r="Q21" s="354"/>
+      <c r="R21" s="354"/>
+      <c r="S21" s="354"/>
+      <c r="T21" s="354"/>
+      <c r="U21" s="354"/>
+      <c r="V21" s="354"/>
+      <c r="W21" s="355"/>
     </row>
     <row r="22" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="372">
+      <c r="B22" s="362">
         <v>5</v>
       </c>
-      <c r="C22" s="373"/>
-      <c r="D22" s="363" t="s">
+      <c r="C22" s="363"/>
+      <c r="D22" s="353" t="s">
         <v>206</v>
       </c>
-      <c r="E22" s="364"/>
-      <c r="F22" s="364"/>
-      <c r="G22" s="364"/>
-      <c r="H22" s="364"/>
-      <c r="I22" s="364"/>
-      <c r="J22" s="364"/>
-      <c r="K22" s="364"/>
-      <c r="L22" s="364"/>
-      <c r="M22" s="364"/>
-      <c r="N22" s="364"/>
-      <c r="O22" s="364"/>
-      <c r="P22" s="364"/>
-      <c r="Q22" s="364"/>
-      <c r="R22" s="364"/>
-      <c r="S22" s="364"/>
-      <c r="T22" s="364"/>
-      <c r="U22" s="364"/>
-      <c r="V22" s="364"/>
-      <c r="W22" s="365"/>
+      <c r="E22" s="354"/>
+      <c r="F22" s="354"/>
+      <c r="G22" s="354"/>
+      <c r="H22" s="354"/>
+      <c r="I22" s="354"/>
+      <c r="J22" s="354"/>
+      <c r="K22" s="354"/>
+      <c r="L22" s="354"/>
+      <c r="M22" s="354"/>
+      <c r="N22" s="354"/>
+      <c r="O22" s="354"/>
+      <c r="P22" s="354"/>
+      <c r="Q22" s="354"/>
+      <c r="R22" s="354"/>
+      <c r="S22" s="354"/>
+      <c r="T22" s="354"/>
+      <c r="U22" s="354"/>
+      <c r="V22" s="354"/>
+      <c r="W22" s="355"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="14">
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="D18:W18"/>
     <mergeCell ref="D19:W19"/>
     <mergeCell ref="D20:W20"/>
     <mergeCell ref="D21:W21"/>
@@ -17954,6 +17969,11 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="D18:W18"/>
   </mergeCells>
   <conditionalFormatting sqref="B8:AG13">
     <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
@@ -18100,14 +18120,14 @@
       </c>
     </row>
     <row r="28" spans="13:19" x14ac:dyDescent="0.2">
-      <c r="N28" s="376" t="s">
+      <c r="N28" s="364" t="s">
         <v>197</v>
       </c>
-      <c r="O28" s="376"/>
-      <c r="P28" s="376"/>
-      <c r="Q28" s="376"/>
-      <c r="R28" s="376"/>
-      <c r="S28" s="376"/>
+      <c r="O28" s="364"/>
+      <c r="P28" s="364"/>
+      <c r="Q28" s="364"/>
+      <c r="R28" s="364"/>
+      <c r="S28" s="364"/>
     </row>
     <row r="30" spans="13:19" x14ac:dyDescent="0.2">
       <c r="N30" s="10" t="s">
@@ -18130,14 +18150,14 @@
       <c r="S33" s="106"/>
     </row>
     <row r="36" spans="14:19" x14ac:dyDescent="0.2">
-      <c r="N36" s="376" t="s">
+      <c r="N36" s="364" t="s">
         <v>199</v>
       </c>
-      <c r="O36" s="376"/>
-      <c r="P36" s="376"/>
-      <c r="Q36" s="376"/>
-      <c r="R36" s="376"/>
-      <c r="S36" s="376"/>
+      <c r="O36" s="364"/>
+      <c r="P36" s="364"/>
+      <c r="Q36" s="364"/>
+      <c r="R36" s="364"/>
+      <c r="S36" s="364"/>
     </row>
     <row r="38" spans="14:19" x14ac:dyDescent="0.2">
       <c r="N38" s="10" t="s">

</xml_diff>

<commit_message>
Final version of WT2019
</commit_message>
<xml_diff>
--- a/Phase 1 Candidate Database v2.xlsx
+++ b/Phase 1 Candidate Database v2.xlsx
@@ -54,6 +54,7 @@
     <definedName name="Divisions" localSheetId="3">Lists!$A$1:$D$3</definedName>
     <definedName name="Divisions">#REF!</definedName>
     <definedName name="DL_Assessor">'Daily Log'!$B$9</definedName>
+    <definedName name="DL_Clear_Area">'Daily Logs'!$B$6:$AY$34</definedName>
     <definedName name="DL_Comments1">'Daily Log'!$B$12</definedName>
     <definedName name="DL_Comments2">'Daily Log'!$B$16</definedName>
     <definedName name="DL_Comments3">'Daily Log'!$B$20</definedName>
@@ -115,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="391">
   <si>
     <t>DAY</t>
   </si>
@@ -1288,12 +1289,6 @@
   </si>
   <si>
     <t>Jeff Bloom</t>
-  </si>
-  <si>
-    <t>5696</t>
-  </si>
-  <si>
-    <t>John Ashby</t>
   </si>
 </sst>
 </file>
@@ -4431,6 +4426,51 @@
     <xf numFmtId="0" fontId="29" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="142" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="141" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="143" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="30" fillId="6" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="30" fillId="6" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="26" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="26" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="22" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="22" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
     <xf numFmtId="167" fontId="31" fillId="24" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
@@ -4440,125 +4480,197 @@
     <xf numFmtId="167" fontId="31" fillId="24" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="104" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="31" fillId="19" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="19" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="21" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="21" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="23" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="23" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="25" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="167" fontId="31" fillId="25" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="19" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="19" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="21" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="19" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="6" borderId="105" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="91" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="88" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="22" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="22" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="26" borderId="115" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="22" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="31" fillId="23" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="23" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="23" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="143" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="141" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="30" fillId="6" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="30" fillId="6" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="26" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="26" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="26" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="22" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="22" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="22" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="25" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="25" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="25" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="100" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="6" borderId="142" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4569,33 +4681,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="38" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="39" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="40" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="40" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="38" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="39" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4632,158 +4717,68 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="120" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="120" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="119" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="119" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="119" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="120" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" textRotation="180"/>
+    </xf>
     <xf numFmtId="0" fontId="30" fillId="19" borderId="121" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="120" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="120" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="22" borderId="119" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="119" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="119" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="22" borderId="120" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="19" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="19" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="21" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="21" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="167" fontId="31" fillId="21" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="101" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="102" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="111" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="112" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="113" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="19" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="19" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="19" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="89" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="90" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="110" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="114" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="87" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="26" borderId="115" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -6298,8 +6293,8 @@
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>18</xdr:col>
-          <xdr:colOff>171450</xdr:colOff>
+          <xdr:col>19</xdr:col>
+          <xdr:colOff>33618</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>371475</xdr:rowOff>
         </xdr:to>
@@ -6332,15 +6327,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>128083</xdr:colOff>
+      <xdr:colOff>128077</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>70350</xdr:rowOff>
+      <xdr:rowOff>162385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>179673</xdr:colOff>
+      <xdr:colOff>11132</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>788599</xdr:rowOff>
+      <xdr:rowOff>702385</xdr:rowOff>
     </xdr:to>
     <xdr:pic macro="[0]!ShtCourse.ShowCourseFrm">
       <xdr:nvPicPr>
@@ -6356,8 +6351,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5137112" y="70350"/>
-          <a:ext cx="679120" cy="718249"/>
+          <a:off x="5047459" y="162385"/>
+          <a:ext cx="510585" cy="540000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6369,15 +6364,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>80923</xdr:colOff>
+      <xdr:colOff>46793</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>64747</xdr:rowOff>
+      <xdr:rowOff>162385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>71097</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>193843</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>788599</xdr:rowOff>
+      <xdr:rowOff>702385</xdr:rowOff>
     </xdr:to>
     <xdr:pic macro="[0]!ShtCourse.ShowCandidateFrm">
       <xdr:nvPicPr>
@@ -6393,8 +6388,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6064864" y="64747"/>
-          <a:ext cx="617704" cy="723852"/>
+          <a:off x="5907469" y="162385"/>
+          <a:ext cx="460815" cy="540000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6406,15 +6401,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>297318</xdr:colOff>
+      <xdr:colOff>229503</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>68599</xdr:rowOff>
+      <xdr:rowOff>162385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>230683</xdr:colOff>
+      <xdr:colOff>22649</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>788599</xdr:rowOff>
+      <xdr:rowOff>702385</xdr:rowOff>
     </xdr:to>
     <xdr:pic macro="[0]!ShtCourse.ShowDailyLogFrm">
       <xdr:nvPicPr>
@@ -6430,8 +6425,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6931200" y="68599"/>
-          <a:ext cx="560894" cy="720000"/>
+          <a:off x="6717709" y="162385"/>
+          <a:ext cx="420675" cy="540000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6443,15 +6438,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>131932</xdr:colOff>
+      <xdr:colOff>58309</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>127671</xdr:rowOff>
+      <xdr:rowOff>162385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>153743</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>275079</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>788599</xdr:rowOff>
+      <xdr:rowOff>702385</xdr:rowOff>
     </xdr:to>
     <xdr:pic macro="[0]!ShtCourse.ShowDevelopmentPlanFrm">
       <xdr:nvPicPr>
@@ -6467,8 +6462,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7740726" y="127671"/>
-          <a:ext cx="649340" cy="660928"/>
+          <a:off x="7487809" y="162385"/>
+          <a:ext cx="530535" cy="540000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6479,16 +6474,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>54992</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>310740</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>57043</xdr:rowOff>
+      <xdr:rowOff>162385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>305923</xdr:colOff>
+      <xdr:colOff>100045</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>788599</xdr:rowOff>
+      <xdr:rowOff>702385</xdr:rowOff>
     </xdr:to>
     <xdr:pic macro="[0]!ShtCourse.RunSupervisionFile">
       <xdr:nvPicPr>
@@ -6504,8 +6499,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8638698" y="57043"/>
-          <a:ext cx="564696" cy="731556"/>
+          <a:off x="8367769" y="162385"/>
+          <a:ext cx="416835" cy="540000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6558,15 +6553,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>218379</xdr:colOff>
+      <xdr:colOff>135705</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>194688</xdr:rowOff>
+      <xdr:rowOff>162385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>160765</xdr:colOff>
+      <xdr:colOff>26351</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>788599</xdr:rowOff>
+      <xdr:rowOff>702385</xdr:rowOff>
     </xdr:to>
     <xdr:pic macro="[0]!ShtCourse.ShowAdminForm">
       <xdr:nvPicPr>
@@ -6594,8 +6589,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9452026" y="194688"/>
-          <a:ext cx="569915" cy="593911"/>
+          <a:off x="9134029" y="162385"/>
+          <a:ext cx="518175" cy="540000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6609,13 +6604,13 @@
       <xdr:col>27</xdr:col>
       <xdr:colOff>62013</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>267727</xdr:rowOff>
+      <xdr:rowOff>162385</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>290568</xdr:colOff>
+      <xdr:colOff>310479</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>788599</xdr:rowOff>
+      <xdr:rowOff>702385</xdr:rowOff>
     </xdr:to>
     <xdr:pic macro="[0]!ShtCourse.SendSupportMail">
       <xdr:nvPicPr>
@@ -6643,8 +6638,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10270572" y="267727"/>
-          <a:ext cx="542319" cy="520872"/>
+          <a:off x="10001631" y="162385"/>
+          <a:ext cx="562230" cy="540000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7849,7 +7844,7 @@
   <dimension ref="A1:AY52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AY8" sqref="AY8"/>
+      <selection activeCell="AE1" sqref="AE1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8497,9 +8492,7 @@
       <c r="AJ7" s="153"/>
       <c r="AK7" s="150"/>
       <c r="AL7" s="153"/>
-      <c r="AM7" s="153">
-        <v>1</v>
-      </c>
+      <c r="AM7" s="153"/>
       <c r="AN7" s="153"/>
       <c r="AO7" s="153"/>
       <c r="AP7" s="153"/>
@@ -8563,9 +8556,7 @@
       <c r="AJ8" s="153"/>
       <c r="AK8" s="150"/>
       <c r="AL8" s="153"/>
-      <c r="AM8" s="153">
-        <v>2</v>
-      </c>
+      <c r="AM8" s="153"/>
       <c r="AN8" s="153"/>
       <c r="AO8" s="153"/>
       <c r="AP8" s="153"/>
@@ -8625,9 +8616,7 @@
       <c r="AL9" s="153">
         <v>1.5</v>
       </c>
-      <c r="AM9" s="153">
-        <v>3</v>
-      </c>
+      <c r="AM9" s="153"/>
       <c r="AN9" s="153"/>
       <c r="AO9" s="153"/>
       <c r="AP9" s="153"/>
@@ -9619,9 +9608,7 @@
       <c r="AJ28" s="153"/>
       <c r="AK28" s="150"/>
       <c r="AL28" s="153"/>
-      <c r="AM28" s="153">
-        <v>4</v>
-      </c>
+      <c r="AM28" s="153"/>
       <c r="AN28" s="153"/>
       <c r="AO28" s="153"/>
       <c r="AP28" s="153"/>
@@ -9673,9 +9660,7 @@
       <c r="AJ29" s="153"/>
       <c r="AK29" s="150"/>
       <c r="AL29" s="153"/>
-      <c r="AM29" s="153">
-        <v>5</v>
-      </c>
+      <c r="AM29" s="153"/>
       <c r="AN29" s="153"/>
       <c r="AO29" s="153"/>
       <c r="AP29" s="153"/>
@@ -10005,7 +9990,7 @@
       <c r="A52" s="131"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <dataConsolidate/>
   <mergeCells count="8">
     <mergeCell ref="O1:T1"/>
@@ -10058,8 +10043,58 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1036" r:id="rId5" name="BtnReset">
+        <control shapeId="1031" r:id="rId5" name="BtnConnectDB">
           <controlPr defaultSize="0" autoFill="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>28</xdr:col>
+                <xdr:colOff>285750</xdr:colOff>
+                <xdr:row>37</xdr:row>
+                <xdr:rowOff>47625</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>32</xdr:col>
+                <xdr:colOff>285750</xdr:colOff>
+                <xdr:row>39</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1031" r:id="rId5" name="BtnConnectDB"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1035" r:id="rId7" name="CmoCourseNo">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>15</xdr:col>
+                <xdr:colOff>161925</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>19</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>371475</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="1035" r:id="rId7" name="CmoCourseNo"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="1036" r:id="rId9" name="BtnReset">
+          <controlPr defaultSize="0" autoFill="0" autoLine="0" r:id="rId10">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>24</xdr:col>
@@ -10078,57 +10113,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1036" r:id="rId5" name="BtnReset"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1035" r:id="rId7" name="CmoCourseNo">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>15</xdr:col>
-                <xdr:colOff>161925</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>18</xdr:col>
-                <xdr:colOff>171450</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>371475</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1035" r:id="rId7" name="CmoCourseNo"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="1031" r:id="rId9" name="BtnConnectDB">
-          <controlPr defaultSize="0" autoFill="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>28</xdr:col>
-                <xdr:colOff>285750</xdr:colOff>
-                <xdr:row>37</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>32</xdr:col>
-                <xdr:colOff>285750</xdr:colOff>
-                <xdr:row>39</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="1031" r:id="rId9" name="BtnConnectDB"/>
+        <control shapeId="1036" r:id="rId9" name="BtnReset"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -10253,30 +10238,30 @@
       <c r="C4" s="213">
         <v>9</v>
       </c>
-      <c r="D4" s="365">
+      <c r="D4" s="401">
         <v>11</v>
       </c>
-      <c r="E4" s="365"/>
-      <c r="F4" s="365">
+      <c r="E4" s="401"/>
+      <c r="F4" s="401">
         <v>17</v>
       </c>
-      <c r="G4" s="365"/>
-      <c r="H4" s="365">
+      <c r="G4" s="401"/>
+      <c r="H4" s="401">
         <v>20</v>
       </c>
-      <c r="I4" s="365"/>
-      <c r="J4" s="365"/>
-      <c r="K4" s="365"/>
-      <c r="L4" s="365">
+      <c r="I4" s="401"/>
+      <c r="J4" s="401"/>
+      <c r="K4" s="401"/>
+      <c r="L4" s="401">
         <v>27</v>
       </c>
-      <c r="M4" s="365"/>
-      <c r="N4" s="365">
+      <c r="M4" s="401"/>
+      <c r="N4" s="401">
         <v>28</v>
       </c>
-      <c r="O4" s="365"/>
-      <c r="P4" s="365"/>
-      <c r="Q4" s="365"/>
+      <c r="O4" s="401"/>
+      <c r="P4" s="401"/>
+      <c r="Q4" s="401"/>
       <c r="R4" s="213">
         <v>29</v>
       </c>
@@ -10290,30 +10275,30 @@
       <c r="C5" s="208" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="371" t="s">
+      <c r="D5" s="400" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="371"/>
-      <c r="F5" s="366" t="s">
+      <c r="E5" s="400"/>
+      <c r="F5" s="395" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="366"/>
-      <c r="H5" s="366" t="s">
+      <c r="G5" s="395"/>
+      <c r="H5" s="395" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="366"/>
-      <c r="J5" s="366"/>
-      <c r="K5" s="366"/>
-      <c r="L5" s="367" t="s">
+      <c r="I5" s="395"/>
+      <c r="J5" s="395"/>
+      <c r="K5" s="395"/>
+      <c r="L5" s="396" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="367"/>
-      <c r="N5" s="367" t="s">
+      <c r="M5" s="396"/>
+      <c r="N5" s="396" t="s">
         <v>23</v>
       </c>
-      <c r="O5" s="367"/>
-      <c r="P5" s="367"/>
-      <c r="Q5" s="367"/>
+      <c r="O5" s="396"/>
+      <c r="P5" s="396"/>
+      <c r="Q5" s="396"/>
       <c r="R5" s="209" t="s">
         <v>17</v>
       </c>
@@ -10327,30 +10312,30 @@
       <c r="C6" s="211" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="368" t="s">
+      <c r="D6" s="397" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="368"/>
-      <c r="F6" s="369" t="s">
+      <c r="E6" s="397"/>
+      <c r="F6" s="398" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="369"/>
-      <c r="H6" s="369" t="s">
+      <c r="G6" s="398"/>
+      <c r="H6" s="398" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="369"/>
-      <c r="J6" s="369"/>
-      <c r="K6" s="369"/>
-      <c r="L6" s="370" t="s">
+      <c r="I6" s="398"/>
+      <c r="J6" s="398"/>
+      <c r="K6" s="398"/>
+      <c r="L6" s="399" t="s">
         <v>53</v>
       </c>
-      <c r="M6" s="370"/>
-      <c r="N6" s="370" t="s">
+      <c r="M6" s="399"/>
+      <c r="N6" s="399" t="s">
         <v>72</v>
       </c>
-      <c r="O6" s="370"/>
-      <c r="P6" s="370"/>
-      <c r="Q6" s="370"/>
+      <c r="O6" s="399"/>
+      <c r="P6" s="399"/>
+      <c r="Q6" s="399"/>
       <c r="R6" s="212" t="s">
         <v>227</v>
       </c>
@@ -10592,6 +10577,11 @@
     <row r="13" spans="1:85" ht="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="N4:Q4"/>
     <mergeCell ref="H5:K5"/>
     <mergeCell ref="N5:Q5"/>
     <mergeCell ref="L5:M5"/>
@@ -10602,11 +10592,6 @@
     <mergeCell ref="N6:Q6"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="N4:Q4"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:J8 B8:D12 F8:J12 L8:R12">
     <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
@@ -10715,7 +10700,7 @@
       <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="BM11" sqref="BM11"/>
+      <selection pane="bottomRight" activeCell="BL8" sqref="BL8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10878,41 +10863,41 @@
       <c r="AU2" s="281"/>
       <c r="AV2" s="281"/>
       <c r="AW2" s="281"/>
-      <c r="AX2" s="323" t="str">
+      <c r="AX2" s="284" t="str">
         <f>CONCATENATE("Course No - ", CourseNo)</f>
         <v>Course No - WT2018</v>
       </c>
-      <c r="AY2" s="323"/>
-      <c r="AZ2" s="323"/>
-      <c r="BA2" s="323"/>
-      <c r="BB2" s="323"/>
-      <c r="BC2" s="323"/>
-      <c r="BD2" s="323"/>
-      <c r="BE2" s="323"/>
-      <c r="BF2" s="323"/>
-      <c r="BG2" s="323"/>
-      <c r="BH2" s="323"/>
-      <c r="BI2" s="323"/>
-      <c r="BJ2" s="323"/>
-      <c r="BK2" s="323"/>
-      <c r="BL2" s="323"/>
-      <c r="BM2" s="323"/>
-      <c r="BN2" s="323"/>
-      <c r="BO2" s="323"/>
-      <c r="BP2" s="323"/>
-      <c r="BQ2" s="323"/>
-      <c r="BR2" s="323"/>
-      <c r="BS2" s="323"/>
-      <c r="BT2" s="323"/>
-      <c r="BU2" s="323"/>
-      <c r="BV2" s="323"/>
-      <c r="BW2" s="323"/>
-      <c r="BX2" s="323"/>
-      <c r="BY2" s="323"/>
-      <c r="BZ2" s="323"/>
-      <c r="CA2" s="323"/>
-      <c r="CB2" s="323"/>
-      <c r="CC2" s="323"/>
+      <c r="AY2" s="284"/>
+      <c r="AZ2" s="284"/>
+      <c r="BA2" s="284"/>
+      <c r="BB2" s="284"/>
+      <c r="BC2" s="284"/>
+      <c r="BD2" s="284"/>
+      <c r="BE2" s="284"/>
+      <c r="BF2" s="284"/>
+      <c r="BG2" s="284"/>
+      <c r="BH2" s="284"/>
+      <c r="BI2" s="284"/>
+      <c r="BJ2" s="284"/>
+      <c r="BK2" s="284"/>
+      <c r="BL2" s="284"/>
+      <c r="BM2" s="284"/>
+      <c r="BN2" s="284"/>
+      <c r="BO2" s="284"/>
+      <c r="BP2" s="284"/>
+      <c r="BQ2" s="284"/>
+      <c r="BR2" s="284"/>
+      <c r="BS2" s="284"/>
+      <c r="BT2" s="284"/>
+      <c r="BU2" s="284"/>
+      <c r="BV2" s="284"/>
+      <c r="BW2" s="284"/>
+      <c r="BX2" s="284"/>
+      <c r="BY2" s="284"/>
+      <c r="BZ2" s="284"/>
+      <c r="CA2" s="284"/>
+      <c r="CB2" s="284"/>
+      <c r="CC2" s="284"/>
       <c r="CD2" s="170"/>
       <c r="CE2" s="170"/>
       <c r="CF2" s="170"/>
@@ -10946,18 +10931,18 @@
       <c r="DH2" s="170"/>
     </row>
     <row r="3" spans="2:113" s="129" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="324" t="s">
+      <c r="B3" s="285" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="325"/>
+      <c r="C3" s="286"/>
       <c r="D3" s="287">
         <v>3</v>
       </c>
       <c r="E3" s="287"/>
       <c r="F3" s="287"/>
       <c r="G3" s="287"/>
-      <c r="H3" s="326"/>
-      <c r="I3" s="311">
+      <c r="H3" s="288"/>
+      <c r="I3" s="289">
         <v>10</v>
       </c>
       <c r="J3" s="287"/>
@@ -10968,8 +10953,8 @@
       <c r="O3" s="287"/>
       <c r="P3" s="287"/>
       <c r="Q3" s="287"/>
-      <c r="R3" s="326"/>
-      <c r="S3" s="311">
+      <c r="R3" s="288"/>
+      <c r="S3" s="289">
         <v>13</v>
       </c>
       <c r="T3" s="287"/>
@@ -10980,8 +10965,8 @@
       <c r="Y3" s="287"/>
       <c r="Z3" s="287"/>
       <c r="AA3" s="287"/>
-      <c r="AB3" s="326"/>
-      <c r="AC3" s="311">
+      <c r="AB3" s="288"/>
+      <c r="AC3" s="289">
         <v>24</v>
       </c>
       <c r="AD3" s="287"/>
@@ -11002,8 +10987,8 @@
       <c r="AS3" s="287"/>
       <c r="AT3" s="287"/>
       <c r="AU3" s="287"/>
-      <c r="AV3" s="326"/>
-      <c r="AW3" s="311">
+      <c r="AV3" s="288"/>
+      <c r="AW3" s="289">
         <v>30</v>
       </c>
       <c r="AX3" s="287"/>
@@ -11014,43 +10999,43 @@
       <c r="BC3" s="287"/>
       <c r="BD3" s="287"/>
       <c r="BE3" s="287"/>
-      <c r="BF3" s="326"/>
-      <c r="BG3" s="310">
+      <c r="BF3" s="288"/>
+      <c r="BG3" s="290">
         <v>34</v>
       </c>
-      <c r="BH3" s="310"/>
-      <c r="BI3" s="311"/>
-      <c r="BJ3" s="311"/>
-      <c r="BK3" s="311"/>
-      <c r="BL3" s="311"/>
-      <c r="BM3" s="311"/>
-      <c r="BN3" s="311"/>
-      <c r="BO3" s="311"/>
-      <c r="BP3" s="311"/>
-      <c r="BQ3" s="310">
+      <c r="BH3" s="290"/>
+      <c r="BI3" s="289"/>
+      <c r="BJ3" s="289"/>
+      <c r="BK3" s="289"/>
+      <c r="BL3" s="289"/>
+      <c r="BM3" s="289"/>
+      <c r="BN3" s="289"/>
+      <c r="BO3" s="289"/>
+      <c r="BP3" s="289"/>
+      <c r="BQ3" s="290">
         <v>40</v>
       </c>
-      <c r="BR3" s="310"/>
-      <c r="BS3" s="311"/>
-      <c r="BT3" s="311"/>
-      <c r="BU3" s="311"/>
-      <c r="BV3" s="311"/>
-      <c r="BW3" s="311"/>
-      <c r="BX3" s="311"/>
-      <c r="BY3" s="311"/>
-      <c r="BZ3" s="311"/>
-      <c r="CA3" s="310">
+      <c r="BR3" s="290"/>
+      <c r="BS3" s="289"/>
+      <c r="BT3" s="289"/>
+      <c r="BU3" s="289"/>
+      <c r="BV3" s="289"/>
+      <c r="BW3" s="289"/>
+      <c r="BX3" s="289"/>
+      <c r="BY3" s="289"/>
+      <c r="BZ3" s="289"/>
+      <c r="CA3" s="290">
         <v>43</v>
       </c>
-      <c r="CB3" s="310"/>
-      <c r="CC3" s="311"/>
-      <c r="CD3" s="311"/>
-      <c r="CE3" s="311"/>
-      <c r="CF3" s="311"/>
-      <c r="CG3" s="311"/>
-      <c r="CH3" s="311"/>
-      <c r="CI3" s="311"/>
-      <c r="CJ3" s="310"/>
+      <c r="CB3" s="290"/>
+      <c r="CC3" s="289"/>
+      <c r="CD3" s="289"/>
+      <c r="CE3" s="289"/>
+      <c r="CF3" s="289"/>
+      <c r="CG3" s="289"/>
+      <c r="CH3" s="289"/>
+      <c r="CI3" s="289"/>
+      <c r="CJ3" s="290"/>
       <c r="CK3" s="287">
         <v>46</v>
       </c>
@@ -11067,403 +11052,403 @@
       <c r="CV3" s="287"/>
       <c r="CW3" s="287"/>
       <c r="CX3" s="287"/>
-      <c r="CY3" s="288"/>
+      <c r="CY3" s="353"/>
       <c r="CZ3" s="251"/>
       <c r="DA3" s="252"/>
     </row>
     <row r="4" spans="2:113" s="242" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="312"/>
-      <c r="C4" s="313"/>
-      <c r="D4" s="314">
+      <c r="B4" s="291"/>
+      <c r="C4" s="292"/>
+      <c r="D4" s="293">
         <v>43107</v>
       </c>
-      <c r="E4" s="315"/>
-      <c r="F4" s="315"/>
-      <c r="G4" s="315"/>
-      <c r="H4" s="316"/>
-      <c r="I4" s="378">
+      <c r="E4" s="294"/>
+      <c r="F4" s="294"/>
+      <c r="G4" s="294"/>
+      <c r="H4" s="295"/>
+      <c r="I4" s="305">
         <v>43118</v>
       </c>
-      <c r="J4" s="379"/>
-      <c r="K4" s="379"/>
-      <c r="L4" s="379"/>
-      <c r="M4" s="379"/>
-      <c r="N4" s="379"/>
-      <c r="O4" s="379"/>
-      <c r="P4" s="379"/>
-      <c r="Q4" s="379"/>
-      <c r="R4" s="380"/>
-      <c r="S4" s="317">
+      <c r="J4" s="306"/>
+      <c r="K4" s="306"/>
+      <c r="L4" s="306"/>
+      <c r="M4" s="306"/>
+      <c r="N4" s="306"/>
+      <c r="O4" s="306"/>
+      <c r="P4" s="306"/>
+      <c r="Q4" s="306"/>
+      <c r="R4" s="307"/>
+      <c r="S4" s="296">
         <v>43125</v>
       </c>
-      <c r="T4" s="318"/>
-      <c r="U4" s="318"/>
-      <c r="V4" s="318"/>
-      <c r="W4" s="318"/>
-      <c r="X4" s="318"/>
-      <c r="Y4" s="318"/>
-      <c r="Z4" s="318"/>
-      <c r="AA4" s="318"/>
-      <c r="AB4" s="319"/>
-      <c r="AC4" s="284">
+      <c r="T4" s="297"/>
+      <c r="U4" s="297"/>
+      <c r="V4" s="297"/>
+      <c r="W4" s="297"/>
+      <c r="X4" s="297"/>
+      <c r="Y4" s="297"/>
+      <c r="Z4" s="297"/>
+      <c r="AA4" s="297"/>
+      <c r="AB4" s="298"/>
+      <c r="AC4" s="299">
         <v>43144</v>
       </c>
-      <c r="AD4" s="285"/>
-      <c r="AE4" s="285"/>
-      <c r="AF4" s="285"/>
-      <c r="AG4" s="285"/>
-      <c r="AH4" s="285"/>
-      <c r="AI4" s="285"/>
-      <c r="AJ4" s="285"/>
-      <c r="AK4" s="285"/>
-      <c r="AL4" s="285"/>
-      <c r="AM4" s="285"/>
-      <c r="AN4" s="285"/>
-      <c r="AO4" s="285"/>
-      <c r="AP4" s="285"/>
-      <c r="AQ4" s="285"/>
-      <c r="AR4" s="285"/>
-      <c r="AS4" s="285"/>
-      <c r="AT4" s="285"/>
-      <c r="AU4" s="285"/>
-      <c r="AV4" s="286"/>
-      <c r="AW4" s="372">
+      <c r="AD4" s="300"/>
+      <c r="AE4" s="300"/>
+      <c r="AF4" s="300"/>
+      <c r="AG4" s="300"/>
+      <c r="AH4" s="300"/>
+      <c r="AI4" s="300"/>
+      <c r="AJ4" s="300"/>
+      <c r="AK4" s="300"/>
+      <c r="AL4" s="300"/>
+      <c r="AM4" s="300"/>
+      <c r="AN4" s="300"/>
+      <c r="AO4" s="300"/>
+      <c r="AP4" s="300"/>
+      <c r="AQ4" s="300"/>
+      <c r="AR4" s="300"/>
+      <c r="AS4" s="300"/>
+      <c r="AT4" s="300"/>
+      <c r="AU4" s="300"/>
+      <c r="AV4" s="301"/>
+      <c r="AW4" s="302">
         <v>43154</v>
       </c>
-      <c r="AX4" s="373"/>
-      <c r="AY4" s="373"/>
-      <c r="AZ4" s="373"/>
-      <c r="BA4" s="373"/>
-      <c r="BB4" s="373"/>
-      <c r="BC4" s="373"/>
-      <c r="BD4" s="373"/>
-      <c r="BE4" s="373"/>
-      <c r="BF4" s="374"/>
-      <c r="BG4" s="307">
+      <c r="AX4" s="303"/>
+      <c r="AY4" s="303"/>
+      <c r="AZ4" s="303"/>
+      <c r="BA4" s="303"/>
+      <c r="BB4" s="303"/>
+      <c r="BC4" s="303"/>
+      <c r="BD4" s="303"/>
+      <c r="BE4" s="303"/>
+      <c r="BF4" s="304"/>
+      <c r="BG4" s="308">
         <v>43162</v>
       </c>
-      <c r="BH4" s="308"/>
-      <c r="BI4" s="308"/>
-      <c r="BJ4" s="308"/>
-      <c r="BK4" s="308"/>
-      <c r="BL4" s="308"/>
-      <c r="BM4" s="308"/>
-      <c r="BN4" s="308"/>
-      <c r="BO4" s="308"/>
-      <c r="BP4" s="309"/>
-      <c r="BQ4" s="320">
+      <c r="BH4" s="309"/>
+      <c r="BI4" s="309"/>
+      <c r="BJ4" s="309"/>
+      <c r="BK4" s="309"/>
+      <c r="BL4" s="309"/>
+      <c r="BM4" s="309"/>
+      <c r="BN4" s="309"/>
+      <c r="BO4" s="309"/>
+      <c r="BP4" s="310"/>
+      <c r="BQ4" s="311">
         <v>43172</v>
       </c>
-      <c r="BR4" s="321"/>
-      <c r="BS4" s="321"/>
-      <c r="BT4" s="321"/>
-      <c r="BU4" s="321"/>
-      <c r="BV4" s="321"/>
-      <c r="BW4" s="321"/>
-      <c r="BX4" s="321"/>
-      <c r="BY4" s="321"/>
-      <c r="BZ4" s="322"/>
-      <c r="CA4" s="378">
+      <c r="BR4" s="312"/>
+      <c r="BS4" s="312"/>
+      <c r="BT4" s="312"/>
+      <c r="BU4" s="312"/>
+      <c r="BV4" s="312"/>
+      <c r="BW4" s="312"/>
+      <c r="BX4" s="312"/>
+      <c r="BY4" s="312"/>
+      <c r="BZ4" s="313"/>
+      <c r="CA4" s="305">
         <v>43179</v>
       </c>
-      <c r="CB4" s="379"/>
-      <c r="CC4" s="379"/>
-      <c r="CD4" s="379"/>
-      <c r="CE4" s="379"/>
-      <c r="CF4" s="379"/>
-      <c r="CG4" s="379"/>
-      <c r="CH4" s="379"/>
-      <c r="CI4" s="379"/>
-      <c r="CJ4" s="380"/>
-      <c r="CK4" s="314">
+      <c r="CB4" s="306"/>
+      <c r="CC4" s="306"/>
+      <c r="CD4" s="306"/>
+      <c r="CE4" s="306"/>
+      <c r="CF4" s="306"/>
+      <c r="CG4" s="306"/>
+      <c r="CH4" s="306"/>
+      <c r="CI4" s="306"/>
+      <c r="CJ4" s="307"/>
+      <c r="CK4" s="293">
         <v>43181</v>
       </c>
-      <c r="CL4" s="315"/>
-      <c r="CM4" s="315"/>
-      <c r="CN4" s="315"/>
-      <c r="CO4" s="315"/>
-      <c r="CP4" s="315"/>
-      <c r="CQ4" s="315"/>
-      <c r="CR4" s="315"/>
-      <c r="CS4" s="315"/>
-      <c r="CT4" s="315"/>
-      <c r="CU4" s="315"/>
-      <c r="CV4" s="315"/>
-      <c r="CW4" s="315"/>
-      <c r="CX4" s="315"/>
-      <c r="CY4" s="316"/>
+      <c r="CL4" s="294"/>
+      <c r="CM4" s="294"/>
+      <c r="CN4" s="294"/>
+      <c r="CO4" s="294"/>
+      <c r="CP4" s="294"/>
+      <c r="CQ4" s="294"/>
+      <c r="CR4" s="294"/>
+      <c r="CS4" s="294"/>
+      <c r="CT4" s="294"/>
+      <c r="CU4" s="294"/>
+      <c r="CV4" s="294"/>
+      <c r="CW4" s="294"/>
+      <c r="CX4" s="294"/>
+      <c r="CY4" s="295"/>
       <c r="CZ4" s="245"/>
       <c r="DA4" s="246"/>
     </row>
     <row r="5" spans="2:113" s="127" customFormat="1" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="297" t="s">
+      <c r="B5" s="314" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="298"/>
-      <c r="D5" s="299" t="s">
+      <c r="C5" s="315"/>
+      <c r="D5" s="316" t="s">
         <v>333</v>
       </c>
-      <c r="E5" s="300"/>
-      <c r="F5" s="300"/>
-      <c r="G5" s="300"/>
-      <c r="H5" s="301"/>
-      <c r="I5" s="381" t="s">
+      <c r="E5" s="317"/>
+      <c r="F5" s="317"/>
+      <c r="G5" s="317"/>
+      <c r="H5" s="318"/>
+      <c r="I5" s="327" t="s">
         <v>373</v>
       </c>
-      <c r="J5" s="382"/>
-      <c r="K5" s="382"/>
-      <c r="L5" s="382"/>
-      <c r="M5" s="382"/>
-      <c r="N5" s="382"/>
-      <c r="O5" s="382"/>
-      <c r="P5" s="382"/>
-      <c r="Q5" s="382"/>
-      <c r="R5" s="383"/>
-      <c r="S5" s="302" t="s">
+      <c r="J5" s="328"/>
+      <c r="K5" s="328"/>
+      <c r="L5" s="328"/>
+      <c r="M5" s="328"/>
+      <c r="N5" s="328"/>
+      <c r="O5" s="328"/>
+      <c r="P5" s="328"/>
+      <c r="Q5" s="328"/>
+      <c r="R5" s="329"/>
+      <c r="S5" s="319" t="s">
         <v>374</v>
       </c>
-      <c r="T5" s="303"/>
-      <c r="U5" s="303"/>
-      <c r="V5" s="303"/>
-      <c r="W5" s="303"/>
-      <c r="X5" s="303"/>
-      <c r="Y5" s="303"/>
-      <c r="Z5" s="303"/>
-      <c r="AA5" s="303"/>
-      <c r="AB5" s="304"/>
-      <c r="AC5" s="290" t="s">
+      <c r="T5" s="320"/>
+      <c r="U5" s="320"/>
+      <c r="V5" s="320"/>
+      <c r="W5" s="320"/>
+      <c r="X5" s="320"/>
+      <c r="Y5" s="320"/>
+      <c r="Z5" s="320"/>
+      <c r="AA5" s="320"/>
+      <c r="AB5" s="321"/>
+      <c r="AC5" s="346" t="s">
         <v>49</v>
       </c>
-      <c r="AD5" s="291"/>
-      <c r="AE5" s="291"/>
-      <c r="AF5" s="291"/>
-      <c r="AG5" s="291"/>
-      <c r="AH5" s="291"/>
-      <c r="AI5" s="291"/>
-      <c r="AJ5" s="291"/>
-      <c r="AK5" s="291"/>
-      <c r="AL5" s="291"/>
-      <c r="AM5" s="291"/>
-      <c r="AN5" s="291"/>
-      <c r="AO5" s="291"/>
-      <c r="AP5" s="291"/>
-      <c r="AQ5" s="291"/>
-      <c r="AR5" s="291"/>
-      <c r="AS5" s="291"/>
-      <c r="AT5" s="291"/>
-      <c r="AU5" s="291"/>
-      <c r="AV5" s="292"/>
-      <c r="AW5" s="387" t="s">
+      <c r="AD5" s="347"/>
+      <c r="AE5" s="347"/>
+      <c r="AF5" s="347"/>
+      <c r="AG5" s="347"/>
+      <c r="AH5" s="347"/>
+      <c r="AI5" s="347"/>
+      <c r="AJ5" s="347"/>
+      <c r="AK5" s="347"/>
+      <c r="AL5" s="347"/>
+      <c r="AM5" s="347"/>
+      <c r="AN5" s="347"/>
+      <c r="AO5" s="347"/>
+      <c r="AP5" s="347"/>
+      <c r="AQ5" s="347"/>
+      <c r="AR5" s="347"/>
+      <c r="AS5" s="347"/>
+      <c r="AT5" s="347"/>
+      <c r="AU5" s="347"/>
+      <c r="AV5" s="348"/>
+      <c r="AW5" s="332" t="s">
         <v>53</v>
       </c>
-      <c r="AX5" s="388"/>
-      <c r="AY5" s="388"/>
-      <c r="AZ5" s="388"/>
-      <c r="BA5" s="388"/>
-      <c r="BB5" s="388"/>
-      <c r="BC5" s="388"/>
-      <c r="BD5" s="388"/>
-      <c r="BE5" s="388"/>
-      <c r="BF5" s="389"/>
-      <c r="BG5" s="294" t="s">
+      <c r="AX5" s="333"/>
+      <c r="AY5" s="333"/>
+      <c r="AZ5" s="333"/>
+      <c r="BA5" s="333"/>
+      <c r="BB5" s="333"/>
+      <c r="BC5" s="333"/>
+      <c r="BD5" s="333"/>
+      <c r="BE5" s="333"/>
+      <c r="BF5" s="334"/>
+      <c r="BG5" s="338" t="s">
         <v>375</v>
       </c>
-      <c r="BH5" s="295"/>
-      <c r="BI5" s="295"/>
-      <c r="BJ5" s="295"/>
-      <c r="BK5" s="295"/>
-      <c r="BL5" s="295"/>
-      <c r="BM5" s="295"/>
-      <c r="BN5" s="295"/>
-      <c r="BO5" s="295"/>
-      <c r="BP5" s="296"/>
-      <c r="BQ5" s="391" t="s">
+      <c r="BH5" s="339"/>
+      <c r="BI5" s="339"/>
+      <c r="BJ5" s="339"/>
+      <c r="BK5" s="339"/>
+      <c r="BL5" s="339"/>
+      <c r="BM5" s="339"/>
+      <c r="BN5" s="339"/>
+      <c r="BO5" s="339"/>
+      <c r="BP5" s="340"/>
+      <c r="BQ5" s="341" t="s">
         <v>376</v>
       </c>
-      <c r="BR5" s="392"/>
-      <c r="BS5" s="392"/>
-      <c r="BT5" s="392"/>
-      <c r="BU5" s="392"/>
-      <c r="BV5" s="392"/>
-      <c r="BW5" s="392"/>
-      <c r="BX5" s="392"/>
-      <c r="BY5" s="392"/>
-      <c r="BZ5" s="393"/>
-      <c r="CA5" s="395" t="s">
+      <c r="BR5" s="342"/>
+      <c r="BS5" s="342"/>
+      <c r="BT5" s="342"/>
+      <c r="BU5" s="342"/>
+      <c r="BV5" s="342"/>
+      <c r="BW5" s="342"/>
+      <c r="BX5" s="342"/>
+      <c r="BY5" s="342"/>
+      <c r="BZ5" s="343"/>
+      <c r="CA5" s="335" t="s">
         <v>377</v>
       </c>
-      <c r="CB5" s="396"/>
-      <c r="CC5" s="396"/>
-      <c r="CD5" s="396"/>
-      <c r="CE5" s="396"/>
-      <c r="CF5" s="396"/>
-      <c r="CG5" s="396"/>
-      <c r="CH5" s="396"/>
-      <c r="CI5" s="396"/>
-      <c r="CJ5" s="397"/>
-      <c r="CK5" s="375" t="s">
+      <c r="CB5" s="336"/>
+      <c r="CC5" s="336"/>
+      <c r="CD5" s="336"/>
+      <c r="CE5" s="336"/>
+      <c r="CF5" s="336"/>
+      <c r="CG5" s="336"/>
+      <c r="CH5" s="336"/>
+      <c r="CI5" s="336"/>
+      <c r="CJ5" s="337"/>
+      <c r="CK5" s="350" t="s">
         <v>72</v>
       </c>
-      <c r="CL5" s="376"/>
-      <c r="CM5" s="376"/>
-      <c r="CN5" s="376"/>
-      <c r="CO5" s="376"/>
-      <c r="CP5" s="376"/>
-      <c r="CQ5" s="376"/>
-      <c r="CR5" s="376"/>
-      <c r="CS5" s="376"/>
-      <c r="CT5" s="376"/>
-      <c r="CU5" s="376"/>
-      <c r="CV5" s="376"/>
-      <c r="CW5" s="376"/>
-      <c r="CX5" s="376"/>
-      <c r="CY5" s="377"/>
+      <c r="CL5" s="351"/>
+      <c r="CM5" s="351"/>
+      <c r="CN5" s="351"/>
+      <c r="CO5" s="351"/>
+      <c r="CP5" s="351"/>
+      <c r="CQ5" s="351"/>
+      <c r="CR5" s="351"/>
+      <c r="CS5" s="351"/>
+      <c r="CT5" s="351"/>
+      <c r="CU5" s="351"/>
+      <c r="CV5" s="351"/>
+      <c r="CW5" s="351"/>
+      <c r="CX5" s="351"/>
+      <c r="CY5" s="352"/>
       <c r="CZ5" s="247"/>
       <c r="DA5" s="248"/>
     </row>
     <row r="6" spans="2:113" s="171" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="243"/>
       <c r="C6" s="244"/>
-      <c r="D6" s="305" t="s">
+      <c r="D6" s="322" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="305"/>
-      <c r="F6" s="305"/>
-      <c r="G6" s="305"/>
-      <c r="H6" s="305"/>
-      <c r="I6" s="384" t="s">
+      <c r="E6" s="322"/>
+      <c r="F6" s="322"/>
+      <c r="G6" s="322"/>
+      <c r="H6" s="322"/>
+      <c r="I6" s="323" t="s">
         <v>86</v>
       </c>
-      <c r="J6" s="385"/>
-      <c r="K6" s="385"/>
-      <c r="L6" s="385"/>
-      <c r="M6" s="386"/>
-      <c r="N6" s="384" t="s">
+      <c r="J6" s="324"/>
+      <c r="K6" s="324"/>
+      <c r="L6" s="324"/>
+      <c r="M6" s="325"/>
+      <c r="N6" s="323" t="s">
         <v>87</v>
       </c>
-      <c r="O6" s="385"/>
-      <c r="P6" s="385"/>
-      <c r="Q6" s="385"/>
-      <c r="R6" s="386"/>
-      <c r="S6" s="306" t="s">
+      <c r="O6" s="324"/>
+      <c r="P6" s="324"/>
+      <c r="Q6" s="324"/>
+      <c r="R6" s="325"/>
+      <c r="S6" s="326" t="s">
         <v>86</v>
       </c>
-      <c r="T6" s="306"/>
-      <c r="U6" s="306"/>
-      <c r="V6" s="306"/>
-      <c r="W6" s="306"/>
-      <c r="X6" s="306" t="s">
+      <c r="T6" s="326"/>
+      <c r="U6" s="326"/>
+      <c r="V6" s="326"/>
+      <c r="W6" s="326"/>
+      <c r="X6" s="326" t="s">
         <v>87</v>
       </c>
-      <c r="Y6" s="306"/>
-      <c r="Z6" s="306"/>
-      <c r="AA6" s="306"/>
-      <c r="AB6" s="306"/>
-      <c r="AC6" s="289" t="s">
+      <c r="Y6" s="326"/>
+      <c r="Z6" s="326"/>
+      <c r="AA6" s="326"/>
+      <c r="AB6" s="326"/>
+      <c r="AC6" s="345" t="s">
         <v>86</v>
       </c>
-      <c r="AD6" s="289"/>
-      <c r="AE6" s="289"/>
-      <c r="AF6" s="289"/>
-      <c r="AG6" s="289"/>
-      <c r="AH6" s="289" t="s">
+      <c r="AD6" s="345"/>
+      <c r="AE6" s="345"/>
+      <c r="AF6" s="345"/>
+      <c r="AG6" s="345"/>
+      <c r="AH6" s="345" t="s">
         <v>87</v>
       </c>
-      <c r="AI6" s="289"/>
-      <c r="AJ6" s="289"/>
-      <c r="AK6" s="289"/>
-      <c r="AL6" s="289"/>
-      <c r="AM6" s="289" t="s">
+      <c r="AI6" s="345"/>
+      <c r="AJ6" s="345"/>
+      <c r="AK6" s="345"/>
+      <c r="AL6" s="345"/>
+      <c r="AM6" s="345" t="s">
         <v>88</v>
       </c>
-      <c r="AN6" s="289"/>
-      <c r="AO6" s="289"/>
-      <c r="AP6" s="289"/>
-      <c r="AQ6" s="289"/>
-      <c r="AR6" s="289" t="s">
+      <c r="AN6" s="345"/>
+      <c r="AO6" s="345"/>
+      <c r="AP6" s="345"/>
+      <c r="AQ6" s="345"/>
+      <c r="AR6" s="345" t="s">
         <v>89</v>
       </c>
-      <c r="AS6" s="289"/>
-      <c r="AT6" s="289"/>
-      <c r="AU6" s="289"/>
-      <c r="AV6" s="289"/>
-      <c r="AW6" s="390" t="s">
+      <c r="AS6" s="345"/>
+      <c r="AT6" s="345"/>
+      <c r="AU6" s="345"/>
+      <c r="AV6" s="345"/>
+      <c r="AW6" s="349" t="s">
         <v>86</v>
       </c>
-      <c r="AX6" s="390"/>
-      <c r="AY6" s="390"/>
-      <c r="AZ6" s="390"/>
-      <c r="BA6" s="390"/>
-      <c r="BB6" s="390" t="s">
+      <c r="AX6" s="349"/>
+      <c r="AY6" s="349"/>
+      <c r="AZ6" s="349"/>
+      <c r="BA6" s="349"/>
+      <c r="BB6" s="349" t="s">
         <v>87</v>
       </c>
-      <c r="BC6" s="390"/>
-      <c r="BD6" s="390"/>
-      <c r="BE6" s="390"/>
-      <c r="BF6" s="390"/>
-      <c r="BG6" s="293" t="s">
+      <c r="BC6" s="349"/>
+      <c r="BD6" s="349"/>
+      <c r="BE6" s="349"/>
+      <c r="BF6" s="349"/>
+      <c r="BG6" s="331" t="s">
         <v>86</v>
       </c>
-      <c r="BH6" s="293"/>
-      <c r="BI6" s="293"/>
-      <c r="BJ6" s="293"/>
-      <c r="BK6" s="293"/>
-      <c r="BL6" s="293" t="s">
+      <c r="BH6" s="331"/>
+      <c r="BI6" s="331"/>
+      <c r="BJ6" s="331"/>
+      <c r="BK6" s="331"/>
+      <c r="BL6" s="331" t="s">
         <v>87</v>
       </c>
-      <c r="BM6" s="293"/>
-      <c r="BN6" s="293"/>
-      <c r="BO6" s="293"/>
-      <c r="BP6" s="293"/>
-      <c r="BQ6" s="394" t="s">
+      <c r="BM6" s="331"/>
+      <c r="BN6" s="331"/>
+      <c r="BO6" s="331"/>
+      <c r="BP6" s="331"/>
+      <c r="BQ6" s="344" t="s">
         <v>86</v>
       </c>
-      <c r="BR6" s="394"/>
-      <c r="BS6" s="394"/>
-      <c r="BT6" s="394"/>
-      <c r="BU6" s="394"/>
-      <c r="BV6" s="394" t="s">
+      <c r="BR6" s="344"/>
+      <c r="BS6" s="344"/>
+      <c r="BT6" s="344"/>
+      <c r="BU6" s="344"/>
+      <c r="BV6" s="344" t="s">
         <v>87</v>
       </c>
-      <c r="BW6" s="394"/>
-      <c r="BX6" s="394"/>
-      <c r="BY6" s="394"/>
-      <c r="BZ6" s="394"/>
-      <c r="CA6" s="398" t="s">
+      <c r="BW6" s="344"/>
+      <c r="BX6" s="344"/>
+      <c r="BY6" s="344"/>
+      <c r="BZ6" s="344"/>
+      <c r="CA6" s="330" t="s">
         <v>86</v>
       </c>
-      <c r="CB6" s="398"/>
-      <c r="CC6" s="398"/>
-      <c r="CD6" s="398"/>
-      <c r="CE6" s="398"/>
-      <c r="CF6" s="398" t="s">
+      <c r="CB6" s="330"/>
+      <c r="CC6" s="330"/>
+      <c r="CD6" s="330"/>
+      <c r="CE6" s="330"/>
+      <c r="CF6" s="330" t="s">
         <v>87</v>
       </c>
-      <c r="CG6" s="398"/>
-      <c r="CH6" s="398"/>
-      <c r="CI6" s="398"/>
-      <c r="CJ6" s="398"/>
-      <c r="CK6" s="399" t="s">
+      <c r="CG6" s="330"/>
+      <c r="CH6" s="330"/>
+      <c r="CI6" s="330"/>
+      <c r="CJ6" s="330"/>
+      <c r="CK6" s="354" t="s">
         <v>86</v>
       </c>
-      <c r="CL6" s="400"/>
-      <c r="CM6" s="400"/>
-      <c r="CN6" s="400"/>
-      <c r="CO6" s="401"/>
-      <c r="CP6" s="399" t="s">
+      <c r="CL6" s="355"/>
+      <c r="CM6" s="355"/>
+      <c r="CN6" s="355"/>
+      <c r="CO6" s="356"/>
+      <c r="CP6" s="354" t="s">
         <v>90</v>
       </c>
-      <c r="CQ6" s="400"/>
-      <c r="CR6" s="400"/>
-      <c r="CS6" s="400"/>
-      <c r="CT6" s="401"/>
-      <c r="CU6" s="399" t="s">
+      <c r="CQ6" s="355"/>
+      <c r="CR6" s="355"/>
+      <c r="CS6" s="355"/>
+      <c r="CT6" s="356"/>
+      <c r="CU6" s="354" t="s">
         <v>87</v>
       </c>
-      <c r="CV6" s="400"/>
-      <c r="CW6" s="400"/>
-      <c r="CX6" s="400"/>
-      <c r="CY6" s="401"/>
+      <c r="CV6" s="355"/>
+      <c r="CW6" s="355"/>
+      <c r="CX6" s="355"/>
+      <c r="CY6" s="356"/>
       <c r="CZ6" s="249" t="s">
         <v>85</v>
       </c>
@@ -11473,10 +11458,10 @@
     </row>
     <row r="7" spans="2:113" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="192" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="C7" s="179" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="D7" s="181"/>
       <c r="E7" s="180"/>
@@ -11493,8 +11478,12 @@
       <c r="P7" s="180"/>
       <c r="Q7" s="180"/>
       <c r="R7" s="182"/>
-      <c r="S7" s="180"/>
-      <c r="T7" s="180"/>
+      <c r="S7" s="180">
+        <v>44</v>
+      </c>
+      <c r="T7" s="180">
+        <v>33</v>
+      </c>
       <c r="U7" s="180"/>
       <c r="V7" s="180"/>
       <c r="W7" s="180"/>
@@ -11523,12 +11512,16 @@
       <c r="AT7" s="180"/>
       <c r="AU7" s="180"/>
       <c r="AV7" s="182"/>
-      <c r="AW7" s="180"/>
+      <c r="AW7" s="180">
+        <v>33</v>
+      </c>
       <c r="AX7" s="180"/>
       <c r="AY7" s="180"/>
       <c r="AZ7" s="180"/>
       <c r="BA7" s="180"/>
-      <c r="BB7" s="181"/>
+      <c r="BB7" s="181">
+        <v>44</v>
+      </c>
       <c r="BC7" s="180"/>
       <c r="BD7" s="180"/>
       <c r="BE7" s="180"/>
@@ -11553,18 +11546,26 @@
       <c r="BX7" s="180"/>
       <c r="BY7" s="180"/>
       <c r="BZ7" s="182"/>
-      <c r="CA7" s="181"/>
+      <c r="CA7" s="181">
+        <v>23</v>
+      </c>
       <c r="CB7" s="180"/>
       <c r="CC7" s="180"/>
       <c r="CD7" s="180"/>
       <c r="CE7" s="182"/>
-      <c r="CF7" s="181"/>
+      <c r="CF7" s="181">
+        <v>22</v>
+      </c>
       <c r="CG7" s="180"/>
       <c r="CH7" s="180"/>
       <c r="CI7" s="180"/>
       <c r="CJ7" s="182"/>
-      <c r="CK7" s="181"/>
-      <c r="CL7" s="180"/>
+      <c r="CK7" s="181">
+        <v>33.200000762939453</v>
+      </c>
+      <c r="CL7" s="180">
+        <v>1</v>
+      </c>
       <c r="CM7" s="180"/>
       <c r="CN7" s="180"/>
       <c r="CO7" s="182"/>
@@ -11594,8 +11595,12 @@
       <c r="DI7" s="128"/>
     </row>
     <row r="8" spans="2:113" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="193"/>
-      <c r="C8" s="173"/>
+      <c r="B8" s="193" t="s">
+        <v>383</v>
+      </c>
+      <c r="C8" s="173" t="s">
+        <v>384</v>
+      </c>
       <c r="D8" s="184"/>
       <c r="E8" s="183"/>
       <c r="F8" s="183"/>
@@ -11611,7 +11616,9 @@
       <c r="P8" s="183"/>
       <c r="Q8" s="183"/>
       <c r="R8" s="185"/>
-      <c r="S8" s="183"/>
+      <c r="S8" s="183">
+        <v>55</v>
+      </c>
       <c r="T8" s="183"/>
       <c r="U8" s="183"/>
       <c r="V8" s="183"/>
@@ -11651,12 +11658,16 @@
       <c r="BD8" s="183"/>
       <c r="BE8" s="183"/>
       <c r="BF8" s="185"/>
-      <c r="BG8" s="184"/>
+      <c r="BG8" s="184">
+        <v>77</v>
+      </c>
       <c r="BH8" s="183"/>
       <c r="BI8" s="183"/>
       <c r="BJ8" s="183"/>
       <c r="BK8" s="185"/>
-      <c r="BL8" s="184"/>
+      <c r="BL8" s="184">
+        <v>77</v>
+      </c>
       <c r="BM8" s="183"/>
       <c r="BN8" s="183"/>
       <c r="BO8" s="183"/>
@@ -11681,8 +11692,12 @@
       <c r="CH8" s="183"/>
       <c r="CI8" s="183"/>
       <c r="CJ8" s="185"/>
-      <c r="CK8" s="184"/>
-      <c r="CL8" s="183"/>
+      <c r="CK8" s="184">
+        <v>69.666664123535156</v>
+      </c>
+      <c r="CL8" s="183">
+        <v>3</v>
+      </c>
       <c r="CM8" s="183"/>
       <c r="CN8" s="183"/>
       <c r="CO8" s="185"/>
@@ -11716,8 +11731,12 @@
       <c r="DI8" s="128"/>
     </row>
     <row r="9" spans="2:113" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="193"/>
-      <c r="C9" s="173"/>
+      <c r="B9" s="193" t="s">
+        <v>385</v>
+      </c>
+      <c r="C9" s="173" t="s">
+        <v>386</v>
+      </c>
       <c r="D9" s="184"/>
       <c r="E9" s="183"/>
       <c r="F9" s="183"/>
@@ -11803,8 +11822,12 @@
       <c r="CH9" s="183"/>
       <c r="CI9" s="183"/>
       <c r="CJ9" s="185"/>
-      <c r="CK9" s="184"/>
-      <c r="CL9" s="183"/>
+      <c r="CK9" s="184">
+        <v>0</v>
+      </c>
+      <c r="CL9" s="183">
+        <v>2</v>
+      </c>
       <c r="CM9" s="183"/>
       <c r="CN9" s="183"/>
       <c r="CO9" s="185"/>
@@ -11834,8 +11857,12 @@
       <c r="DI9" s="128"/>
     </row>
     <row r="10" spans="2:113" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="193"/>
-      <c r="C10" s="173"/>
+      <c r="B10" s="193" t="s">
+        <v>387</v>
+      </c>
+      <c r="C10" s="173" t="s">
+        <v>388</v>
+      </c>
       <c r="D10" s="184"/>
       <c r="E10" s="183"/>
       <c r="F10" s="183"/>
@@ -15197,6 +15224,49 @@
   </sortState>
   <dataConsolidate/>
   <mergeCells count="52">
+    <mergeCell ref="CK4:CY4"/>
+    <mergeCell ref="CK5:CY5"/>
+    <mergeCell ref="CK3:CY3"/>
+    <mergeCell ref="CK6:CO6"/>
+    <mergeCell ref="CP6:CT6"/>
+    <mergeCell ref="CU6:CY6"/>
+    <mergeCell ref="AH6:AL6"/>
+    <mergeCell ref="AC5:AV5"/>
+    <mergeCell ref="BQ6:BU6"/>
+    <mergeCell ref="AM6:AQ6"/>
+    <mergeCell ref="AR6:AV6"/>
+    <mergeCell ref="AW6:BA6"/>
+    <mergeCell ref="BB6:BF6"/>
+    <mergeCell ref="AC6:AG6"/>
+    <mergeCell ref="CA6:CE6"/>
+    <mergeCell ref="BL6:BP6"/>
+    <mergeCell ref="AW5:BF5"/>
+    <mergeCell ref="CA5:CJ5"/>
+    <mergeCell ref="CF6:CJ6"/>
+    <mergeCell ref="BG5:BP5"/>
+    <mergeCell ref="BG6:BK6"/>
+    <mergeCell ref="BQ5:BZ5"/>
+    <mergeCell ref="BV6:BZ6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="S5:AB5"/>
+    <mergeCell ref="D6:H6"/>
+    <mergeCell ref="N6:R6"/>
+    <mergeCell ref="S6:W6"/>
+    <mergeCell ref="X6:AB6"/>
+    <mergeCell ref="I6:M6"/>
+    <mergeCell ref="I5:R5"/>
+    <mergeCell ref="CA4:CJ4"/>
+    <mergeCell ref="BG4:BP4"/>
+    <mergeCell ref="BG3:BP3"/>
+    <mergeCell ref="BQ4:BZ4"/>
+    <mergeCell ref="BQ3:BZ3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="S4:AB4"/>
+    <mergeCell ref="AC4:AV4"/>
+    <mergeCell ref="AW4:BF4"/>
+    <mergeCell ref="I4:R4"/>
     <mergeCell ref="AX2:CC2"/>
     <mergeCell ref="AC2:AW2"/>
     <mergeCell ref="B3:C3"/>
@@ -15206,49 +15276,6 @@
     <mergeCell ref="AW3:BF3"/>
     <mergeCell ref="CA3:CJ3"/>
     <mergeCell ref="I3:R3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="S4:AB4"/>
-    <mergeCell ref="AC4:AV4"/>
-    <mergeCell ref="AW4:BF4"/>
-    <mergeCell ref="I4:R4"/>
-    <mergeCell ref="CA4:CJ4"/>
-    <mergeCell ref="BG4:BP4"/>
-    <mergeCell ref="BG3:BP3"/>
-    <mergeCell ref="BQ4:BZ4"/>
-    <mergeCell ref="BQ3:BZ3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="S5:AB5"/>
-    <mergeCell ref="D6:H6"/>
-    <mergeCell ref="N6:R6"/>
-    <mergeCell ref="S6:W6"/>
-    <mergeCell ref="X6:AB6"/>
-    <mergeCell ref="I6:M6"/>
-    <mergeCell ref="I5:R5"/>
-    <mergeCell ref="CA6:CE6"/>
-    <mergeCell ref="BL6:BP6"/>
-    <mergeCell ref="AW5:BF5"/>
-    <mergeCell ref="CA5:CJ5"/>
-    <mergeCell ref="CF6:CJ6"/>
-    <mergeCell ref="BG5:BP5"/>
-    <mergeCell ref="BG6:BK6"/>
-    <mergeCell ref="BQ5:BZ5"/>
-    <mergeCell ref="BV6:BZ6"/>
-    <mergeCell ref="AH6:AL6"/>
-    <mergeCell ref="AC5:AV5"/>
-    <mergeCell ref="BQ6:BU6"/>
-    <mergeCell ref="AM6:AQ6"/>
-    <mergeCell ref="AR6:AV6"/>
-    <mergeCell ref="AW6:BA6"/>
-    <mergeCell ref="BB6:BF6"/>
-    <mergeCell ref="AC6:AG6"/>
-    <mergeCell ref="CK4:CY4"/>
-    <mergeCell ref="CK5:CY5"/>
-    <mergeCell ref="CK3:CY3"/>
-    <mergeCell ref="CK6:CO6"/>
-    <mergeCell ref="CP6:CT6"/>
-    <mergeCell ref="CU6:CY6"/>
   </mergeCells>
   <conditionalFormatting sqref="CZ35">
     <cfRule type="top10" dxfId="45" priority="58" percent="1" bottom="1" rank="10"/>
@@ -15392,8 +15419,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="3073" r:id="rId4" name="BtnAddAssess">
+        <control shapeId="3075" r:id="rId4" name="BtnEditAssess">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>457200</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="3075" r:id="rId4" name="BtnEditAssess"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="3073" r:id="rId6" name="BtnAddAssess">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
@@ -15412,32 +15464,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="3073" r:id="rId4" name="BtnAddAssess"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="3075" r:id="rId6" name="BtnEditAssess">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>457200</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="3075" r:id="rId6" name="BtnEditAssess"/>
+        <control shapeId="3073" r:id="rId6" name="BtnAddAssess"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -16699,14 +16726,14 @@
       </c>
     </row>
     <row r="3" spans="1:11" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="330" t="s">
+      <c r="A3" s="357" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="331"/>
-      <c r="C3" s="331"/>
-      <c r="D3" s="331"/>
-      <c r="E3" s="331"/>
-      <c r="F3" s="332"/>
+      <c r="B3" s="358"/>
+      <c r="C3" s="358"/>
+      <c r="D3" s="358"/>
+      <c r="E3" s="358"/>
+      <c r="F3" s="359"/>
       <c r="H3" s="74"/>
     </row>
     <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -16751,14 +16778,14 @@
     </row>
     <row r="6" spans="1:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:11" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="330" t="s">
+      <c r="A7" s="357" t="s">
         <v>165</v>
       </c>
-      <c r="B7" s="331"/>
-      <c r="C7" s="331"/>
-      <c r="D7" s="331"/>
-      <c r="E7" s="331"/>
-      <c r="F7" s="332"/>
+      <c r="B7" s="358"/>
+      <c r="C7" s="358"/>
+      <c r="D7" s="358"/>
+      <c r="E7" s="358"/>
+      <c r="F7" s="359"/>
       <c r="H7" s="74"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -16771,11 +16798,11 @@
       <c r="C8" s="57" t="s">
         <v>167</v>
       </c>
-      <c r="D8" s="333" t="s">
+      <c r="D8" s="360" t="s">
         <v>330</v>
       </c>
-      <c r="E8" s="334"/>
-      <c r="F8" s="335"/>
+      <c r="E8" s="361"/>
+      <c r="F8" s="362"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="55" t="s">
@@ -16799,27 +16826,27 @@
     </row>
     <row r="10" spans="1:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:11" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="330" t="s">
+      <c r="A11" s="357" t="s">
         <v>116</v>
       </c>
-      <c r="B11" s="331"/>
-      <c r="C11" s="331"/>
-      <c r="D11" s="331"/>
-      <c r="E11" s="331"/>
-      <c r="F11" s="332"/>
+      <c r="B11" s="358"/>
+      <c r="C11" s="358"/>
+      <c r="D11" s="358"/>
+      <c r="E11" s="358"/>
+      <c r="F11" s="359"/>
       <c r="H11" s="74"/>
     </row>
     <row r="12" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="B12" s="336" t="s">
+      <c r="B12" s="363" t="s">
         <v>113</v>
       </c>
-      <c r="C12" s="337"/>
-      <c r="D12" s="337"/>
-      <c r="E12" s="337"/>
-      <c r="F12" s="338"/>
+      <c r="C12" s="364"/>
+      <c r="D12" s="364"/>
+      <c r="E12" s="364"/>
+      <c r="F12" s="365"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="64"/>
@@ -16835,25 +16862,25 @@
     </row>
     <row r="14" spans="1:11" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:11" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="330" t="s">
+      <c r="A15" s="357" t="s">
         <v>114</v>
       </c>
-      <c r="B15" s="331"/>
-      <c r="C15" s="331"/>
-      <c r="D15" s="331"/>
-      <c r="E15" s="331"/>
-      <c r="F15" s="332"/>
+      <c r="B15" s="358"/>
+      <c r="C15" s="358"/>
+      <c r="D15" s="358"/>
+      <c r="E15" s="358"/>
+      <c r="F15" s="359"/>
       <c r="H15" s="74"/>
     </row>
     <row r="16" spans="1:11" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="B16" s="327"/>
-      <c r="C16" s="328"/>
-      <c r="D16" s="328"/>
-      <c r="E16" s="328"/>
-      <c r="F16" s="329"/>
+      <c r="B16" s="366"/>
+      <c r="C16" s="367"/>
+      <c r="D16" s="367"/>
+      <c r="E16" s="367"/>
+      <c r="F16" s="368"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="64"/>
@@ -16869,25 +16896,25 @@
     </row>
     <row r="18" spans="1:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" spans="1:8" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="330" t="s">
+      <c r="A19" s="357" t="s">
         <v>115</v>
       </c>
-      <c r="B19" s="331"/>
-      <c r="C19" s="331"/>
-      <c r="D19" s="331"/>
-      <c r="E19" s="331"/>
-      <c r="F19" s="332"/>
+      <c r="B19" s="358"/>
+      <c r="C19" s="358"/>
+      <c r="D19" s="358"/>
+      <c r="E19" s="358"/>
+      <c r="F19" s="359"/>
       <c r="H19" s="74"/>
     </row>
     <row r="20" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="B20" s="327"/>
-      <c r="C20" s="328"/>
-      <c r="D20" s="328"/>
-      <c r="E20" s="328"/>
-      <c r="F20" s="329"/>
+      <c r="B20" s="366"/>
+      <c r="C20" s="367"/>
+      <c r="D20" s="367"/>
+      <c r="E20" s="367"/>
+      <c r="F20" s="368"/>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="64"/>
@@ -16903,25 +16930,25 @@
     </row>
     <row r="22" spans="1:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:8" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="330" t="s">
+      <c r="A23" s="357" t="s">
         <v>171</v>
       </c>
-      <c r="B23" s="331"/>
-      <c r="C23" s="331"/>
-      <c r="D23" s="331"/>
-      <c r="E23" s="331"/>
-      <c r="F23" s="332"/>
+      <c r="B23" s="358"/>
+      <c r="C23" s="358"/>
+      <c r="D23" s="358"/>
+      <c r="E23" s="358"/>
+      <c r="F23" s="359"/>
       <c r="H23" s="74"/>
     </row>
     <row r="24" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="B24" s="327"/>
-      <c r="C24" s="328"/>
-      <c r="D24" s="328"/>
-      <c r="E24" s="328"/>
-      <c r="F24" s="329"/>
+      <c r="B24" s="366"/>
+      <c r="C24" s="367"/>
+      <c r="D24" s="367"/>
+      <c r="E24" s="367"/>
+      <c r="F24" s="368"/>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="64"/>
@@ -16937,27 +16964,27 @@
     </row>
     <row r="26" spans="1:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="27" spans="1:8" s="50" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="330" t="s">
+      <c r="A27" s="357" t="s">
         <v>172</v>
       </c>
-      <c r="B27" s="331"/>
-      <c r="C27" s="331"/>
-      <c r="D27" s="331"/>
-      <c r="E27" s="331"/>
-      <c r="F27" s="332"/>
+      <c r="B27" s="358"/>
+      <c r="C27" s="358"/>
+      <c r="D27" s="358"/>
+      <c r="E27" s="358"/>
+      <c r="F27" s="359"/>
       <c r="H27" s="74"/>
     </row>
     <row r="28" spans="1:8" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="B28" s="327" t="s">
+      <c r="B28" s="366" t="s">
         <v>331</v>
       </c>
-      <c r="C28" s="328"/>
-      <c r="D28" s="328"/>
-      <c r="E28" s="328"/>
-      <c r="F28" s="329"/>
+      <c r="C28" s="367"/>
+      <c r="D28" s="367"/>
+      <c r="E28" s="367"/>
+      <c r="F28" s="368"/>
       <c r="H28" s="74" t="s">
         <v>331</v>
       </c>
@@ -16973,12 +17000,6 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="13">
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="B12:F12"/>
     <mergeCell ref="B28:F28"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="A19:F19"/>
@@ -16986,6 +17007,12 @@
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="B12:F12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="94" fitToHeight="0" orientation="portrait" r:id="rId1"/>
@@ -17029,10 +17056,10 @@
       <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="C3" s="342" t="s">
+      <c r="C3" s="372" t="s">
         <v>232</v>
       </c>
-      <c r="D3" s="342"/>
+      <c r="D3" s="372"/>
     </row>
     <row r="4" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:6" s="40" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -17094,35 +17121,35 @@
     </row>
     <row r="10" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:6" s="17" customFormat="1" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="343" t="s">
+      <c r="A11" s="373" t="s">
         <v>128</v>
       </c>
-      <c r="B11" s="345"/>
-      <c r="C11" s="346"/>
+      <c r="B11" s="375"/>
+      <c r="C11" s="376"/>
       <c r="D11" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="E11" s="349"/>
-      <c r="F11" s="350"/>
+      <c r="E11" s="379"/>
+      <c r="F11" s="380"/>
     </row>
     <row r="12" spans="1:6" s="17" customFormat="1" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="344"/>
-      <c r="B12" s="347"/>
-      <c r="C12" s="348"/>
+      <c r="A12" s="374"/>
+      <c r="B12" s="377"/>
+      <c r="C12" s="378"/>
       <c r="D12" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="E12" s="349"/>
-      <c r="F12" s="350"/>
+      <c r="E12" s="379"/>
+      <c r="F12" s="380"/>
     </row>
     <row r="13" spans="1:6" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:6" s="22" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="339" t="s">
+      <c r="B14" s="369" t="s">
         <v>131</v>
       </c>
-      <c r="C14" s="340"/>
-      <c r="D14" s="340"/>
-      <c r="E14" s="341"/>
+      <c r="C14" s="370"/>
+      <c r="D14" s="370"/>
+      <c r="E14" s="371"/>
       <c r="F14"/>
     </row>
     <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -17188,30 +17215,30 @@
         <v>184</v>
       </c>
       <c r="C3" s="100"/>
-      <c r="E3" s="352">
+      <c r="E3" s="393">
         <v>5665</v>
       </c>
-      <c r="F3" s="352"/>
+      <c r="F3" s="393"/>
       <c r="G3" s="96" t="s">
         <v>124</v>
       </c>
-      <c r="I3" s="352" t="s">
+      <c r="I3" s="393" t="s">
         <v>329</v>
       </c>
-      <c r="J3" s="352"/>
-      <c r="K3" s="352"/>
-      <c r="L3" s="352"/>
-      <c r="M3" s="352"/>
+      <c r="J3" s="393"/>
+      <c r="K3" s="393"/>
+      <c r="L3" s="393"/>
+      <c r="M3" s="393"/>
       <c r="N3" s="96" t="s">
         <v>162</v>
       </c>
-      <c r="P3" s="352" t="s">
+      <c r="P3" s="393" t="s">
         <v>252</v>
       </c>
-      <c r="Q3" s="352"/>
-      <c r="R3" s="352"/>
-      <c r="S3" s="352"/>
-      <c r="T3" s="352"/>
+      <c r="Q3" s="393"/>
+      <c r="R3" s="393"/>
+      <c r="S3" s="393"/>
+      <c r="T3" s="393"/>
       <c r="V3" s="96" t="s">
         <v>163</v>
       </c>
@@ -17222,10 +17249,10 @@
         <v>63</v>
       </c>
       <c r="AD3" s="99"/>
-      <c r="AF3" s="351" t="s">
+      <c r="AF3" s="392" t="s">
         <v>328</v>
       </c>
-      <c r="AG3" s="351"/>
+      <c r="AG3" s="392"/>
     </row>
     <row r="5" spans="1:33" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="76" t="s">
@@ -17818,148 +17845,153 @@
     </row>
     <row r="17" spans="2:23" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="18" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="356" t="s">
+      <c r="B18" s="384" t="s">
         <v>207</v>
       </c>
-      <c r="C18" s="357"/>
-      <c r="D18" s="353" t="s">
+      <c r="C18" s="385"/>
+      <c r="D18" s="381" t="s">
         <v>202</v>
       </c>
-      <c r="E18" s="354"/>
-      <c r="F18" s="354"/>
-      <c r="G18" s="354"/>
-      <c r="H18" s="354"/>
-      <c r="I18" s="354"/>
-      <c r="J18" s="354"/>
-      <c r="K18" s="354"/>
-      <c r="L18" s="354"/>
-      <c r="M18" s="354"/>
-      <c r="N18" s="354"/>
-      <c r="O18" s="354"/>
-      <c r="P18" s="354"/>
-      <c r="Q18" s="354"/>
-      <c r="R18" s="354"/>
-      <c r="S18" s="354"/>
-      <c r="T18" s="354"/>
-      <c r="U18" s="354"/>
-      <c r="V18" s="354"/>
-      <c r="W18" s="355"/>
+      <c r="E18" s="382"/>
+      <c r="F18" s="382"/>
+      <c r="G18" s="382"/>
+      <c r="H18" s="382"/>
+      <c r="I18" s="382"/>
+      <c r="J18" s="382"/>
+      <c r="K18" s="382"/>
+      <c r="L18" s="382"/>
+      <c r="M18" s="382"/>
+      <c r="N18" s="382"/>
+      <c r="O18" s="382"/>
+      <c r="P18" s="382"/>
+      <c r="Q18" s="382"/>
+      <c r="R18" s="382"/>
+      <c r="S18" s="382"/>
+      <c r="T18" s="382"/>
+      <c r="U18" s="382"/>
+      <c r="V18" s="382"/>
+      <c r="W18" s="383"/>
     </row>
     <row r="19" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="358">
+      <c r="B19" s="386">
         <v>2</v>
       </c>
-      <c r="C19" s="359"/>
-      <c r="D19" s="353" t="s">
+      <c r="C19" s="387"/>
+      <c r="D19" s="381" t="s">
         <v>203</v>
       </c>
-      <c r="E19" s="354"/>
-      <c r="F19" s="354"/>
-      <c r="G19" s="354"/>
-      <c r="H19" s="354"/>
-      <c r="I19" s="354"/>
-      <c r="J19" s="354"/>
-      <c r="K19" s="354"/>
-      <c r="L19" s="354"/>
-      <c r="M19" s="354"/>
-      <c r="N19" s="354"/>
-      <c r="O19" s="354"/>
-      <c r="P19" s="354"/>
-      <c r="Q19" s="354"/>
-      <c r="R19" s="354"/>
-      <c r="S19" s="354"/>
-      <c r="T19" s="354"/>
-      <c r="U19" s="354"/>
-      <c r="V19" s="354"/>
-      <c r="W19" s="355"/>
+      <c r="E19" s="382"/>
+      <c r="F19" s="382"/>
+      <c r="G19" s="382"/>
+      <c r="H19" s="382"/>
+      <c r="I19" s="382"/>
+      <c r="J19" s="382"/>
+      <c r="K19" s="382"/>
+      <c r="L19" s="382"/>
+      <c r="M19" s="382"/>
+      <c r="N19" s="382"/>
+      <c r="O19" s="382"/>
+      <c r="P19" s="382"/>
+      <c r="Q19" s="382"/>
+      <c r="R19" s="382"/>
+      <c r="S19" s="382"/>
+      <c r="T19" s="382"/>
+      <c r="U19" s="382"/>
+      <c r="V19" s="382"/>
+      <c r="W19" s="383"/>
     </row>
     <row r="20" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="360">
+      <c r="B20" s="388">
         <v>3</v>
       </c>
-      <c r="C20" s="361"/>
-      <c r="D20" s="353" t="s">
+      <c r="C20" s="389"/>
+      <c r="D20" s="381" t="s">
         <v>204</v>
       </c>
-      <c r="E20" s="354"/>
-      <c r="F20" s="354"/>
-      <c r="G20" s="354"/>
-      <c r="H20" s="354"/>
-      <c r="I20" s="354"/>
-      <c r="J20" s="354"/>
-      <c r="K20" s="354"/>
-      <c r="L20" s="354"/>
-      <c r="M20" s="354"/>
-      <c r="N20" s="354"/>
-      <c r="O20" s="354"/>
-      <c r="P20" s="354"/>
-      <c r="Q20" s="354"/>
-      <c r="R20" s="354"/>
-      <c r="S20" s="354"/>
-      <c r="T20" s="354"/>
-      <c r="U20" s="354"/>
-      <c r="V20" s="354"/>
-      <c r="W20" s="355"/>
+      <c r="E20" s="382"/>
+      <c r="F20" s="382"/>
+      <c r="G20" s="382"/>
+      <c r="H20" s="382"/>
+      <c r="I20" s="382"/>
+      <c r="J20" s="382"/>
+      <c r="K20" s="382"/>
+      <c r="L20" s="382"/>
+      <c r="M20" s="382"/>
+      <c r="N20" s="382"/>
+      <c r="O20" s="382"/>
+      <c r="P20" s="382"/>
+      <c r="Q20" s="382"/>
+      <c r="R20" s="382"/>
+      <c r="S20" s="382"/>
+      <c r="T20" s="382"/>
+      <c r="U20" s="382"/>
+      <c r="V20" s="382"/>
+      <c r="W20" s="383"/>
     </row>
     <row r="21" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="362">
+      <c r="B21" s="390">
         <v>4</v>
       </c>
-      <c r="C21" s="363"/>
-      <c r="D21" s="353" t="s">
+      <c r="C21" s="391"/>
+      <c r="D21" s="381" t="s">
         <v>205</v>
       </c>
-      <c r="E21" s="354"/>
-      <c r="F21" s="354"/>
-      <c r="G21" s="354"/>
-      <c r="H21" s="354"/>
-      <c r="I21" s="354"/>
-      <c r="J21" s="354"/>
-      <c r="K21" s="354"/>
-      <c r="L21" s="354"/>
-      <c r="M21" s="354"/>
-      <c r="N21" s="354"/>
-      <c r="O21" s="354"/>
-      <c r="P21" s="354"/>
-      <c r="Q21" s="354"/>
-      <c r="R21" s="354"/>
-      <c r="S21" s="354"/>
-      <c r="T21" s="354"/>
-      <c r="U21" s="354"/>
-      <c r="V21" s="354"/>
-      <c r="W21" s="355"/>
+      <c r="E21" s="382"/>
+      <c r="F21" s="382"/>
+      <c r="G21" s="382"/>
+      <c r="H21" s="382"/>
+      <c r="I21" s="382"/>
+      <c r="J21" s="382"/>
+      <c r="K21" s="382"/>
+      <c r="L21" s="382"/>
+      <c r="M21" s="382"/>
+      <c r="N21" s="382"/>
+      <c r="O21" s="382"/>
+      <c r="P21" s="382"/>
+      <c r="Q21" s="382"/>
+      <c r="R21" s="382"/>
+      <c r="S21" s="382"/>
+      <c r="T21" s="382"/>
+      <c r="U21" s="382"/>
+      <c r="V21" s="382"/>
+      <c r="W21" s="383"/>
     </row>
     <row r="22" spans="2:23" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="362">
+      <c r="B22" s="390">
         <v>5</v>
       </c>
-      <c r="C22" s="363"/>
-      <c r="D22" s="353" t="s">
+      <c r="C22" s="391"/>
+      <c r="D22" s="381" t="s">
         <v>206</v>
       </c>
-      <c r="E22" s="354"/>
-      <c r="F22" s="354"/>
-      <c r="G22" s="354"/>
-      <c r="H22" s="354"/>
-      <c r="I22" s="354"/>
-      <c r="J22" s="354"/>
-      <c r="K22" s="354"/>
-      <c r="L22" s="354"/>
-      <c r="M22" s="354"/>
-      <c r="N22" s="354"/>
-      <c r="O22" s="354"/>
-      <c r="P22" s="354"/>
-      <c r="Q22" s="354"/>
-      <c r="R22" s="354"/>
-      <c r="S22" s="354"/>
-      <c r="T22" s="354"/>
-      <c r="U22" s="354"/>
-      <c r="V22" s="354"/>
-      <c r="W22" s="355"/>
+      <c r="E22" s="382"/>
+      <c r="F22" s="382"/>
+      <c r="G22" s="382"/>
+      <c r="H22" s="382"/>
+      <c r="I22" s="382"/>
+      <c r="J22" s="382"/>
+      <c r="K22" s="382"/>
+      <c r="L22" s="382"/>
+      <c r="M22" s="382"/>
+      <c r="N22" s="382"/>
+      <c r="O22" s="382"/>
+      <c r="P22" s="382"/>
+      <c r="Q22" s="382"/>
+      <c r="R22" s="382"/>
+      <c r="S22" s="382"/>
+      <c r="T22" s="382"/>
+      <c r="U22" s="382"/>
+      <c r="V22" s="382"/>
+      <c r="W22" s="383"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="14">
+    <mergeCell ref="AF3:AG3"/>
+    <mergeCell ref="P3:T3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="D18:W18"/>
     <mergeCell ref="D19:W19"/>
     <mergeCell ref="D20:W20"/>
     <mergeCell ref="D21:W21"/>
@@ -17969,11 +18001,6 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
-    <mergeCell ref="AF3:AG3"/>
-    <mergeCell ref="P3:T3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="D18:W18"/>
   </mergeCells>
   <conditionalFormatting sqref="B8:AG13">
     <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
@@ -18120,14 +18147,14 @@
       </c>
     </row>
     <row r="28" spans="13:19" x14ac:dyDescent="0.2">
-      <c r="N28" s="364" t="s">
+      <c r="N28" s="394" t="s">
         <v>197</v>
       </c>
-      <c r="O28" s="364"/>
-      <c r="P28" s="364"/>
-      <c r="Q28" s="364"/>
-      <c r="R28" s="364"/>
-      <c r="S28" s="364"/>
+      <c r="O28" s="394"/>
+      <c r="P28" s="394"/>
+      <c r="Q28" s="394"/>
+      <c r="R28" s="394"/>
+      <c r="S28" s="394"/>
     </row>
     <row r="30" spans="13:19" x14ac:dyDescent="0.2">
       <c r="N30" s="10" t="s">
@@ -18150,14 +18177,14 @@
       <c r="S33" s="106"/>
     </row>
     <row r="36" spans="14:19" x14ac:dyDescent="0.2">
-      <c r="N36" s="364" t="s">
+      <c r="N36" s="394" t="s">
         <v>199</v>
       </c>
-      <c r="O36" s="364"/>
-      <c r="P36" s="364"/>
-      <c r="Q36" s="364"/>
-      <c r="R36" s="364"/>
-      <c r="S36" s="364"/>
+      <c r="O36" s="394"/>
+      <c r="P36" s="394"/>
+      <c r="Q36" s="394"/>
+      <c r="R36" s="394"/>
+      <c r="S36" s="394"/>
     </row>
     <row r="38" spans="14:19" x14ac:dyDescent="0.2">
       <c r="N38" s="10" t="s">

</xml_diff>